<commit_message>
add rich text box behavior, append sample test case
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -15,6 +15,7 @@
     <sheet name="HomePage" sheetId="1" r:id="rId6"/>
     <sheet name="SearchResultPage" sheetId="21" r:id="rId7"/>
     <sheet name="LoginPage" sheetId="22" r:id="rId8"/>
+    <sheet name="RichTextTestPage" sheetId="23" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$I$2:$I$4</definedName>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="89">
   <si>
     <t>Page</t>
   </si>
@@ -88,7 +89,7 @@
     <t>YesNo</t>
   </si>
   <si>
-    <t>Click</t>
+    <t>click</t>
   </si>
   <si>
     <t>chrome</t>
@@ -112,7 +113,7 @@
     <t>YES</t>
   </si>
   <si>
-    <t>Enter</t>
+    <t>enter</t>
   </si>
   <si>
     <t>firefox</t>
@@ -133,7 +134,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Focus</t>
+    <t>focus</t>
   </si>
   <si>
     <t>ie</t>
@@ -148,43 +149,43 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Blur</t>
+    <t>blur</t>
   </si>
   <si>
     <t>LoginButton</t>
   </si>
   <si>
-    <t>Select</t>
+    <t>select</t>
   </si>
   <si>
     <t>PasswordError</t>
   </si>
   <si>
-    <t>Check</t>
-  </si>
-  <si>
-    <t>Double Click</t>
-  </si>
-  <si>
-    <t>Hover</t>
-  </si>
-  <si>
-    <t>Wait For Ready</t>
-  </si>
-  <si>
-    <t>Wait To Click</t>
-  </si>
-  <si>
-    <t>Wait To Hide</t>
-  </si>
-  <si>
-    <t>Clear</t>
-  </si>
-  <si>
-    <t>Get</t>
-  </si>
-  <si>
-    <t>Size</t>
+    <t>check</t>
+  </si>
+  <si>
+    <t>doubleClick</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>waitForVisible</t>
+  </si>
+  <si>
+    <t>waitForClickable</t>
+  </si>
+  <si>
+    <t>waitForHidden</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>size</t>
   </si>
   <si>
     <t>[value]</t>
@@ -202,7 +203,16 @@
     <t>[attr]</t>
   </si>
   <si>
-    <t>Click If Visible</t>
+    <t>clickIfVisible</t>
+  </si>
+  <si>
+    <t>selectPartialContent</t>
+  </si>
+  <si>
+    <t>waitToPresent</t>
+  </si>
+  <si>
+    <t>waitForCheck</t>
   </si>
   <si>
     <t>TestCase ID</t>
@@ -229,6 +239,15 @@
     <t>https://cn.bing.com/</t>
   </si>
   <si>
+    <t>RichTextTest</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>http://localhost:8000/#/</t>
+  </si>
+  <si>
     <t>default</t>
   </si>
   <si>
@@ -271,6 +290,9 @@
     <t>Login</t>
   </si>
   <si>
+    <t>RichTextTestPage</t>
+  </si>
+  <si>
     <t>TestGroup ID</t>
   </si>
   <si>
@@ -296,6 +318,12 @@
   </si>
   <si>
     <t>zhaocxhey3@163.com</t>
+  </si>
+  <si>
+    <t>RichTextBox[1]</t>
+  </si>
+  <si>
+    <t>0,5</t>
   </si>
 </sst>
 </file>
@@ -341,7 +369,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -354,9 +382,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,62 +412,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -445,18 +436,40 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -467,6 +480,21 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -489,43 +517,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,67 +679,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,67 +697,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -683,17 +711,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -713,6 +744,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -728,40 +768,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,64 +797,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -846,85 +946,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1259,12 +1287,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1483,6 +1511,21 @@
     <row r="21" spans="2:2">
       <c r="B21" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1513,36 +1556,36 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1551,8 +1594,25 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="4:4">
-      <c r="D3" s="2"/>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -1565,6 +1625,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://cn.bing.com/"/>
+    <hyperlink ref="D3" r:id="rId2" display="http://localhost:8000/#/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1595,34 +1656,34 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1666,15 +1727,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="16.5047619047619" customWidth="1"/>
     <col min="2" max="2" width="20.3714285714286" customWidth="1"/>
@@ -1682,13 +1743,13 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1704,7 +1765,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1715,12 +1776,23 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1762,10 +1834,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1773,13 +1845,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1805,7 +1877,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10:B11"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1819,27 +1891,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1848,15 +1920,15 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1889,7 +1961,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="$A2:$XFD2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1900,27 +1972,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -1952,7 +2024,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="4"/>
@@ -1962,27 +2034,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -1991,15 +2063,15 @@
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -2011,10 +2083,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -2025,10 +2097,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -2042,10 +2114,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -2056,10 +2128,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2070,10 +2142,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2100,4 +2172,71 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="19.4285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+      <formula1>ContactPage</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update several control behavior
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12585" activeTab="1"/>
+    <workbookView windowWidth="27795" windowHeight="12585" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="92">
   <si>
     <t>Page</t>
   </si>
@@ -206,15 +206,24 @@
     <t>clickIfVisible</t>
   </si>
   <si>
+    <t>waitTextToBePresented</t>
+  </si>
+  <si>
+    <t>waitForCheck</t>
+  </si>
+  <si>
+    <t>waitUtilSelected</t>
+  </si>
+  <si>
+    <t>clickAndHold</t>
+  </si>
+  <si>
+    <t>dragAndDropByOffset</t>
+  </si>
+  <si>
     <t>selectPartialContent</t>
   </si>
   <si>
-    <t>waitToPresent</t>
-  </si>
-  <si>
-    <t>waitForCheck</t>
-  </si>
-  <si>
     <t>TestCase ID</t>
   </si>
   <si>
@@ -320,7 +329,7 @@
     <t>zhaocxhey3@163.com</t>
   </si>
   <si>
-    <t>RichTextBox[1]</t>
+    <t>RichTextBox</t>
   </si>
   <si>
     <t>0,5</t>
@@ -331,9 +340,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -368,13 +377,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -389,11 +392,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -413,25 +415,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -450,14 +437,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
@@ -465,9 +444,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,6 +468,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -489,8 +490,16 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -517,187 +526,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -713,33 +722,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -800,159 +787,181 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1287,12 +1296,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1528,6 +1537,21 @@
         <v>51</v>
       </c>
     </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1540,7 +1564,7 @@
   <sheetPr/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
@@ -1556,36 +1580,36 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1596,16 +1620,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1656,34 +1680,34 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:10">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1743,13 +1767,13 @@
   <sheetData>
     <row r="1" s="4" customFormat="1" spans="1:3">
       <c r="A1" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1765,7 +1789,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1776,7 +1800,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1787,10 +1811,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1834,10 +1858,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1845,13 +1869,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1891,27 +1915,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1920,15 +1944,15 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1972,27 +1996,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -2034,27 +2058,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2063,15 +2087,15 @@
         <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -2083,10 +2107,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -2097,10 +2121,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -2114,10 +2138,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -2128,10 +2152,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2142,10 +2166,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2179,8 +2203,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -2192,36 +2216,36 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update sendkey behavior for richbox
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="93">
   <si>
     <t>Page</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>selectPartialContent</t>
+  </si>
+  <si>
+    <t>sendEnter</t>
   </si>
   <si>
     <t>TestCase ID</t>
@@ -340,9 +343,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -379,9 +382,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -414,8 +425,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -432,6 +451,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -459,6 +486,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -473,37 +507,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -532,13 +535,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -550,61 +697,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,97 +709,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,11 +725,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -735,7 +736,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -751,6 +752,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -793,181 +820,158 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1296,12 +1300,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1314,35 +1318,35 @@
     <col min="9" max="9" width="10.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:10">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1356,7 +1360,7 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
@@ -1388,7 +1392,7 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="7"/>
       <c r="E3" t="s">
         <v>20</v>
       </c>
@@ -1550,6 +1554,11 @@
     <row r="27" spans="2:2">
       <c r="B27" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
+      <c r="B28" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1578,38 +1587,38 @@
     <col min="5" max="5" width="14.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:6">
-      <c r="A1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:6">
+      <c r="A1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>59</v>
+      <c r="F1" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>62</v>
+      <c r="D2" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1620,16 +1629,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>65</v>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1678,36 +1687,36 @@
     <col min="6" max="6" width="8.24761904761905" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:10">
-      <c r="A1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:10">
+      <c r="A1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>75</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1765,15 +1774,15 @@
     <col min="2" max="2" width="20.3714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:3">
+      <c r="A1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>77</v>
+      <c r="C1" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1789,7 +1798,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1800,7 +1809,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1811,10 +1820,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1858,10 +1867,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1869,13 +1878,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1915,27 +1924,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1944,15 +1953,15 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1996,27 +2005,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -2058,27 +2067,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2086,16 +2095,16 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>89</v>
+      <c r="E2" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -2103,14 +2112,14 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -2121,10 +2130,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -2138,10 +2147,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -2152,10 +2161,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2166,10 +2175,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2201,13 +2210,13 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+      <selection activeCell="A4" sqref="$A4:$XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
@@ -2216,37 +2225,54 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
       </c>
       <c r="E2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
         <v>91</v>
       </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5">
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>

<commit_message>
update dragAndDrop behavior, fix control behaviors
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -16,6 +16,7 @@
     <sheet name="SearchResultPage" sheetId="21" r:id="rId7"/>
     <sheet name="LoginPage" sheetId="22" r:id="rId8"/>
     <sheet name="RichTextTestPage" sheetId="23" r:id="rId9"/>
+    <sheet name="OffsetClickPage" sheetId="24" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$I$2:$I$4</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="98">
   <si>
     <t>Page</t>
   </si>
@@ -227,6 +228,9 @@
     <t>sendEnter</t>
   </si>
   <si>
+    <t>rightClick</t>
+  </si>
+  <si>
     <t>TestCase ID</t>
   </si>
   <si>
@@ -260,6 +264,12 @@
     <t>http://localhost:8000/#/</t>
   </si>
   <si>
+    <t>OffsetClick</t>
+  </si>
+  <si>
+    <t>https://antirobot.tianyancha.com/captcha/verify?return_url=https%3A%2F%2Fwww.tianyancha.com%2Fsearch%2FocH-e15-s2%3Fbase%3Dhangzhou%26areaCode%3D330185&amp;rnd=%22</t>
+  </si>
+  <si>
     <t>default</t>
   </si>
   <si>
@@ -336,6 +346,12 @@
   </si>
   <si>
     <t>0,5</t>
+  </si>
+  <si>
+    <t>drogAndDropRichBox</t>
+  </si>
+  <si>
+    <t>135,42,135,400</t>
   </si>
 </sst>
 </file>
@@ -343,8 +359,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -380,6 +396,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -393,13 +423,6 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -434,16 +457,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -451,6 +466,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -464,8 +486,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -477,36 +523,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -529,13 +545,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,169 +695,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,6 +736,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -741,28 +766,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -782,6 +796,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -797,150 +822,141 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -949,29 +965,28 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1300,12 +1315,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1318,35 +1333,35 @@
     <col min="9" max="9" width="10.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:10">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="4" customFormat="1" spans="1:10">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1360,7 +1375,7 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
@@ -1392,7 +1407,7 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="7"/>
+      <c r="D3" s="6"/>
       <c r="E3" t="s">
         <v>20</v>
       </c>
@@ -1559,6 +1574,11 @@
     <row r="28" spans="2:2">
       <c r="B28" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1568,18 +1588,80 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1">
+      <formula1>ContactPage</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="28.6285714285714" customWidth="1"/>
     <col min="2" max="2" width="38.752380952381" customWidth="1"/>
@@ -1587,38 +1669,38 @@
     <col min="5" max="5" width="14.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:6">
-      <c r="A1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" s="4" customFormat="1" spans="1:6">
+      <c r="A1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>60</v>
+      <c r="F1" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>63</v>
+      <c r="D2" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1629,22 +1711,36 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>66</v>
+      <c r="D3" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1652,13 +1748,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E3 E4:E5 E6:E1048576">
       <formula1>Browser</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C4 C5:C6 C7:C1048576">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://cn.bing.com/"/>
     <hyperlink ref="D3" r:id="rId2" display="http://localhost:8000/#/"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://antirobot.tianyancha.com/captcha/verify?return_url=https%3A%2F%2Fwww.tianyancha.com%2Fsearch%2FocH-e15-s2%3Fbase%3Dhangzhou%26areaCode%3D330185&amp;rnd=%22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1687,36 +1784,36 @@
     <col min="6" max="6" width="8.24761904761905" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:10">
-      <c r="A1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="5" t="s">
+    <row r="1" s="4" customFormat="1" spans="1:10">
+      <c r="A1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>76</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1774,15 +1871,15 @@
     <col min="2" max="2" width="20.3714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:3">
-      <c r="A1" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" s="4" customFormat="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>78</v>
+      <c r="C1" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1798,7 +1895,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1809,7 +1906,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1820,10 +1917,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1867,10 +1964,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1878,13 +1975,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1924,27 +2021,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1953,15 +2050,15 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -2005,27 +2102,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -2067,27 +2164,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2095,16 +2192,16 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>90</v>
+      <c r="E2" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -2112,14 +2209,14 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -2130,10 +2227,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -2147,10 +2244,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -2161,10 +2258,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2175,10 +2272,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2213,7 +2310,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="$A4:$XFD4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -2225,54 +2322,68 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="5:5">
-      <c r="E4" s="2"/>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>

<commit_message>
udpate offset click testcase
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12585" activeTab="8"/>
+    <workbookView windowWidth="27795" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="104">
   <si>
     <t>Page</t>
   </si>
@@ -315,6 +315,9 @@
     <t>RichTextTestPage</t>
   </si>
   <si>
+    <t>OffsetClickPage</t>
+  </si>
+  <si>
     <t>TestGroup ID</t>
   </si>
   <si>
@@ -352,6 +355,21 @@
   </si>
   <si>
     <t>135,42,135,400</t>
+  </si>
+  <si>
+    <t>BgImgie</t>
+  </si>
+  <si>
+    <t>moveByOffsetFromElement</t>
+  </si>
+  <si>
+    <t>100,90</t>
+  </si>
+  <si>
+    <t>clickAtCurrentPosition</t>
+  </si>
+  <si>
+    <t>50,60</t>
   </si>
 </sst>
 </file>
@@ -359,10 +377,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -397,7 +415,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -405,6 +423,20 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,69 +450,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -503,6 +475,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
@@ -510,8 +490,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,49 +563,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,79 +725,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,48 +744,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -736,48 +754,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -798,11 +774,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -836,97 +810,141 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -935,28 +953,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -965,28 +983,29 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1317,10 +1336,10 @@
   <sheetPr/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1333,35 +1352,35 @@
     <col min="9" max="9" width="10.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:10">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1375,7 +1394,7 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
@@ -1407,7 +1426,7 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="7"/>
       <c r="E3" t="s">
         <v>20</v>
       </c>
@@ -1427,7 +1446,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -1591,29 +1613,35 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="17.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="21.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="30.8571428571429" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1621,16 +1649,61 @@
         <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>95</v>
+        <v>100</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1658,7 +1731,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -1669,23 +1742,23 @@
     <col min="5" max="5" width="14.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:6">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:6">
+      <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1699,7 +1772,7 @@
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E2" t="s">
@@ -1717,9 +1790,9 @@
         <v>66</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>67</v>
       </c>
       <c r="E3" t="s">
@@ -1737,9 +1810,9 @@
         <v>66</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1784,35 +1857,35 @@
     <col min="6" max="6" width="8.24761904761905" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:10">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:10">
+      <c r="A1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1857,7 +1930,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1865,20 +1938,20 @@
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="16.5047619047619" customWidth="1"/>
     <col min="2" max="2" width="20.3714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:3">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="5" customFormat="1" spans="1:3">
+      <c r="A1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1923,6 +1996,17 @@
         <v>84</v>
       </c>
       <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1967,7 +2051,7 @@
         <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1978,10 +2062,10 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2024,16 +2108,16 @@
         <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2041,7 +2125,7 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -2050,7 +2134,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2058,7 +2142,7 @@
         <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -2105,16 +2189,16 @@
         <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2122,7 +2206,7 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -2167,16 +2251,16 @@
         <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2184,7 +2268,7 @@
         <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2192,8 +2276,8 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>93</v>
+      <c r="E2" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2201,7 +2285,7 @@
         <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -2209,14 +2293,14 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -2230,7 +2314,7 @@
         <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -2247,7 +2331,7 @@
         <v>62</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -2261,7 +2345,7 @@
         <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -2275,7 +2359,7 @@
         <v>62</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -2309,7 +2393,7 @@
   <sheetPr/>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2325,16 +2409,16 @@
         <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2342,16 +2426,16 @@
         <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2359,10 +2443,10 @@
         <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
         <v>55</v>
@@ -2373,16 +2457,16 @@
         <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update selectPartialContext for richtextbox
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="97">
   <si>
     <t>Page</t>
   </si>
@@ -123,6 +123,9 @@
     <t>MyTaskSubMenu</t>
   </si>
   <si>
+    <t>Selections[1]</t>
+  </si>
+  <si>
     <t>DECLINE</t>
   </si>
   <si>
@@ -141,6 +144,9 @@
     <t>FirstTask</t>
   </si>
   <si>
+    <t>Selections[2]</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -219,10 +225,13 @@
     <t>sendKey</t>
   </si>
   <si>
+    <t>sendKeyByRobot</t>
+  </si>
+  <si>
     <t>rightClick</t>
   </si>
   <si>
-    <t>sendKeyByRobot</t>
+    <t>[css](background-color)</t>
   </si>
   <si>
     <t>TestCase ID</t>
@@ -312,6 +321,9 @@
     <t>dong</t>
   </si>
   <si>
+    <t>Parameter</t>
+  </si>
+  <si>
     <t>10,10,800,300</t>
   </si>
   <si>
@@ -322,6 +334,18 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>rgba(205, 79, 57, 1)</t>
+  </si>
+  <si>
+    <t>50,60</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>rgba(204, 152, 229,1)</t>
   </si>
 </sst>
 </file>
@@ -329,10 +353,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -359,23 +383,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -387,64 +420,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -464,8 +443,47 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -486,11 +504,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -527,31 +551,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,133 +671,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -706,6 +730,48 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -739,24 +805,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -782,151 +830,127 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -935,22 +959,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1286,12 +1310,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1385,14 +1409,17 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
       <c r="H3" t="b">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1400,158 +1427,166 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1582,36 +1617,36 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1655,34 +1690,34 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:10">
       <c r="A1" s="5" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1742,18 +1777,18 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1764,7 +1799,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1775,7 +1810,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1819,41 +1854,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1862,15 +1897,15 @@
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1884,13 +1919,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1922,7 +1957,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="4"/>
@@ -1933,27 +1968,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -1965,10 +2000,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1979,27 +2014,27 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -2007,27 +2042,27 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
@@ -2053,128 +2088,199 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="31.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D1:D2 D7:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D1:D2 D11:D1048576">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C1:C2 C7:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C7 C8 C9 C10 C1:C2 C11:C1048576">
       <formula1>PageObjectModel!$G:$G</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update selectPartialContext for rrichtextbox
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12585" activeTab="6"/>
+    <workbookView windowWidth="20835" windowHeight="8355"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$I$2:$I$4</definedName>
-    <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$25</definedName>
+    <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$23</definedName>
     <definedName name="AdditionalOnePage">PageObjectModel!#REF!</definedName>
     <definedName name="AdditionalTwoPage">PageObjectModel!#REF!</definedName>
     <definedName name="Boolean">PageObjectModel!$H$2:$H$3</definedName>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="99">
   <si>
     <t>Page</t>
   </si>
@@ -156,9 +156,15 @@
     <t>TestTask</t>
   </si>
   <si>
+    <t>Selections[3]</t>
+  </si>
+  <si>
     <t>select</t>
   </si>
   <si>
+    <t>AddIcon</t>
+  </si>
+  <si>
     <t>check</t>
   </si>
   <si>
@@ -195,12 +201,6 @@
     <t>[class]</t>
   </si>
   <si>
-    <t>[css]</t>
-  </si>
-  <si>
-    <t>[attr]</t>
-  </si>
-  <si>
     <t>clickIfVisible</t>
   </si>
   <si>
@@ -234,6 +234,9 @@
     <t>[css](background-color)</t>
   </si>
   <si>
+    <t>[attr](style)</t>
+  </si>
+  <si>
     <t>TestCase ID</t>
   </si>
   <si>
@@ -330,7 +333,7 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>0,10</t>
+    <t>双肺呼吸音清</t>
   </si>
   <si>
     <t>D</t>
@@ -339,13 +342,16 @@
     <t>rgba(205, 79, 57, 1)</t>
   </si>
   <si>
-    <t>50,60</t>
+    <t>无红肿、渗出</t>
   </si>
   <si>
     <t>C</t>
   </si>
   <si>
     <t>rgba(204, 152, 229,1)</t>
+  </si>
+  <si>
+    <t>抗炎，强心利尿治疗</t>
   </si>
 </sst>
 </file>
@@ -353,10 +359,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -390,7 +396,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -404,6 +410,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -412,11 +425,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -424,6 +437,14 @@
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -442,17 +463,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -460,6 +472,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -475,30 +503,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -511,8 +516,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -539,187 +545,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -738,6 +744,21 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -761,6 +782,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -771,21 +807,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -805,21 +826,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -833,85 +839,85 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -920,37 +926,37 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -959,19 +965,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1310,12 +1316,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1451,142 +1457,143 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:7">
       <c r="B5" t="s">
         <v>31</v>
       </c>
       <c r="F5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="2:2">
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2">
-      <c r="B31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1617,36 +1624,36 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1675,7 +1682,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1690,34 +1697,34 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:10">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1746,7 +1753,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -1777,18 +1784,18 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1799,7 +1806,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1810,7 +1817,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1854,41 +1861,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1897,15 +1904,15 @@
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1919,10 +1926,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -1968,27 +1975,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -2000,10 +2007,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -2014,24 +2021,24 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -2042,24 +2049,24 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -2088,10 +2095,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -2103,45 +2110,45 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -2150,15 +2157,15 @@
         <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -2167,15 +2174,15 @@
         <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -2184,15 +2191,15 @@
         <v>54</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -2201,15 +2208,15 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -2218,15 +2225,15 @@
         <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -2235,15 +2242,15 @@
         <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -2252,15 +2259,15 @@
         <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -2269,18 +2276,83 @@
         <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D1:D2 D11:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D14 D1:D2 D11:D13 D15:D1048576">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C7 C8 C9 C10 C1:C2 C11:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C7 C8 C9 C10 C13 C14 C1:C2 C11:C12 C15:C1048576">
       <formula1>PageObjectModel!$G:$G</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update annotationTool related methods
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20835" windowHeight="8355"/>
+    <workbookView windowWidth="27795" windowHeight="12585" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="99">
   <si>
     <t>Page</t>
   </si>
@@ -237,6 +237,9 @@
     <t>[attr](style)</t>
   </si>
   <si>
+    <t>takescreen</t>
+  </si>
+  <si>
     <t>TestCase ID</t>
   </si>
   <si>
@@ -322,9 +325,6 @@
   </si>
   <si>
     <t>dong</t>
-  </si>
-  <si>
-    <t>Parameter</t>
   </si>
   <si>
     <t>10,10,800,300</t>
@@ -360,8 +360,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -396,7 +396,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -411,17 +418,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -433,8 +432,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -457,13 +465,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -477,17 +478,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -502,6 +502,14 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="等线"/>
@@ -510,15 +518,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -545,187 +545,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,6 +744,56 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -772,45 +822,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -825,138 +836,127 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -965,19 +965,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1316,12 +1316,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7:G9"/>
+      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1594,6 +1594,11 @@
     <row r="30" spans="2:2">
       <c r="B30" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1624,36 +1629,36 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1697,34 +1702,34 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:10">
       <c r="A1" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1784,18 +1789,18 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1806,7 +1811,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1817,7 +1822,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1861,27 +1866,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1892,10 +1897,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1904,15 +1909,15 @@
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1926,10 +1931,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -1975,27 +1980,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -2007,10 +2012,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -2021,10 +2026,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -2035,10 +2040,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -2049,10 +2054,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -2063,10 +2068,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -2095,45 +2100,42 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="16.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="31.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2145,10 +2147,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -2162,10 +2164,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -2179,10 +2181,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -2196,10 +2198,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -2213,10 +2215,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -2230,10 +2232,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -2247,10 +2249,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -2264,10 +2266,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -2281,10 +2283,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -2298,10 +2300,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
@@ -2312,10 +2314,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
@@ -2329,10 +2331,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
@@ -2342,6 +2344,20 @@
       </c>
       <c r="E14" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2352,7 +2368,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C7 C8 C9 C10 C13 C14 C1:C2 C11:C12 C15:C1048576">
       <formula1>PageObjectModel!$G:$G</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update testcase, optimize code
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="103">
   <si>
     <t>Page</t>
   </si>
@@ -219,7 +219,7 @@
     <t>drogAndDropRichBox</t>
   </si>
   <si>
-    <t>selectPartialContext</t>
+    <t>selectPartialContextByContext</t>
   </si>
   <si>
     <t>sendKey</t>
@@ -240,6 +240,9 @@
     <t>takescreen</t>
   </si>
   <si>
+    <t>selectPartialContextByIndex</t>
+  </si>
+  <si>
     <t>TestCase ID</t>
   </si>
   <si>
@@ -352,6 +355,15 @@
   </si>
   <si>
     <t>抗炎，强心利尿治疗</t>
+  </si>
+  <si>
+    <t>25,35</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>rgba(206, 206, 206, 1)</t>
   </si>
 </sst>
 </file>
@@ -360,9 +372,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -396,14 +408,30 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -425,16 +453,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -449,16 +476,39 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -479,50 +529,12 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -545,181 +557,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,6 +756,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -765,9 +786,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,174 +842,133 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -965,19 +977,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1316,12 +1328,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1599,6 +1611,11 @@
     <row r="31" spans="2:2">
       <c r="B31" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1629,36 +1646,36 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:6">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1687,7 +1704,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1702,34 +1719,34 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:10">
       <c r="A1" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1737,7 +1754,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -1789,18 +1806,18 @@
   <sheetData>
     <row r="1" s="5" customFormat="1" spans="1:3">
       <c r="A1" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1811,7 +1828,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1822,7 +1839,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -1866,27 +1883,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
@@ -1897,10 +1914,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1909,15 +1926,15 @@
         <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -1931,10 +1948,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>27</v>
@@ -1980,27 +1997,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -2012,10 +2029,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -2026,10 +2043,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>32</v>
@@ -2040,10 +2057,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>32</v>
@@ -2054,10 +2071,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>28</v>
@@ -2068,10 +2085,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>28</v>
@@ -2100,10 +2117,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19:H20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2115,27 +2132,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2147,10 +2164,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -2159,15 +2176,15 @@
         <v>53</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -2176,15 +2193,15 @@
         <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -2193,15 +2210,15 @@
         <v>54</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
@@ -2210,15 +2227,15 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
@@ -2227,15 +2244,15 @@
         <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -2244,15 +2261,15 @@
         <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -2261,15 +2278,15 @@
         <v>56</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -2278,15 +2295,15 @@
         <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -2295,15 +2312,15 @@
         <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
@@ -2314,10 +2331,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C13" t="s">
         <v>29</v>
@@ -2326,15 +2343,15 @@
         <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>33</v>
@@ -2343,32 +2360,83 @@
         <v>58</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
         <v>15</v>
       </c>
       <c r="D15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
         <v>60</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D14 D1:D2 D11:D13 D15:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D14 D15 D16 D17 D18 D1:D2 D11:D13 D19:D1048576">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C7 C8 C9 C10 C13 C14 C1:C2 C11:C12 C15:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C6 C7 C8 C9 C10 C13 C14 C15 C16 C17 C18 C1:C2 C11:C12 C19:C1048576">
       <formula1>PageObjectModel!$G:$G</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update testcase and object model for CCM
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20835" windowHeight="8355" activeTab="2"/>
+    <workbookView windowWidth="27765" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -14,13 +14,17 @@
     <sheet name="AnnotationLoginPage" sheetId="22" r:id="rId5"/>
     <sheet name="AnnotationHomePage" sheetId="23" r:id="rId6"/>
     <sheet name="AnnotationImplementPage" sheetId="24" r:id="rId7"/>
+    <sheet name="CCMLoginPage" sheetId="25" r:id="rId8"/>
+    <sheet name="CCMMemberPage" sheetId="26" r:id="rId9"/>
+    <sheet name="CCMChronicPage" sheetId="27" r:id="rId10"/>
+    <sheet name="CCMEnrollmentPage" sheetId="28" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="Acceptable">PageObjectModel!$I$2:$I$4</definedName>
+    <definedName name="Acceptable">PageObjectModel!$M$2:$M$4</definedName>
     <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$23</definedName>
     <definedName name="AdditionalOnePage">PageObjectModel!#REF!</definedName>
     <definedName name="AdditionalTwoPage">PageObjectModel!#REF!</definedName>
-    <definedName name="Boolean">PageObjectModel!$H$2:$H$3</definedName>
+    <definedName name="Boolean">PageObjectModel!$L$2:$L$3</definedName>
     <definedName name="Browser">PageObjectModel!$C$2:$C$7</definedName>
     <definedName name="ContactPage">PageObjectModel!#REF!</definedName>
     <definedName name="CustomCoveragePage">PageObjectModel!#REF!</definedName>
@@ -48,14 +52,14 @@
     <definedName name="VehicleOwnedMonthsOptions">PageObjectModel!#REF!</definedName>
     <definedName name="VehicleUsage">PageObjectModel!#REF!</definedName>
     <definedName name="Violations">PageObjectModel!#REF!</definedName>
-    <definedName name="YesNo">PageObjectModel!$J$2:$J$4</definedName>
+    <definedName name="YesNo">PageObjectModel!$N$2:$N$4</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="136">
   <si>
     <t>Page</t>
   </si>
@@ -78,6 +82,18 @@
     <t>AnnotationImplementPage</t>
   </si>
   <si>
+    <t>CCMLoginPage</t>
+  </si>
+  <si>
+    <t>CCMMemberPage</t>
+  </si>
+  <si>
+    <t>CCMChronicPage</t>
+  </si>
+  <si>
+    <t>CCMEnrollmentPage</t>
+  </si>
+  <si>
     <t>Boolean</t>
   </si>
   <si>
@@ -105,6 +121,15 @@
     <t>RichTextBox</t>
   </si>
   <si>
+    <t>NextPageButton</t>
+  </si>
+  <si>
+    <t>CCMOrRPMPanel</t>
+  </si>
+  <si>
+    <t>DemographicsButton</t>
+  </si>
+  <si>
     <t>ACCEPT</t>
   </si>
   <si>
@@ -126,6 +151,15 @@
     <t>Selections[1]</t>
   </si>
   <si>
+    <t>Member40</t>
+  </si>
+  <si>
+    <t>CCMMemberTabs</t>
+  </si>
+  <si>
+    <t>PrimaryCareId</t>
+  </si>
+  <si>
     <t>DECLINE</t>
   </si>
   <si>
@@ -147,6 +181,9 @@
     <t>Selections[2]</t>
   </si>
   <si>
+    <t>GenderDropdown</t>
+  </si>
+  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -159,18 +196,27 @@
     <t>Selections[3]</t>
   </si>
   <si>
+    <t>ActiveOptions[1]</t>
+  </si>
+  <si>
     <t>select</t>
   </si>
   <si>
     <t>AddIcon</t>
   </si>
   <si>
+    <t>ActiveOptions[2]</t>
+  </si>
+  <si>
     <t>check</t>
   </si>
   <si>
     <t>Dropdowns[1]</t>
   </si>
   <si>
+    <t>ActiveOptions[3]</t>
+  </si>
+  <si>
     <t>doubleClick</t>
   </si>
   <si>
@@ -186,21 +232,12 @@
     <t>waitForVisible</t>
   </si>
   <si>
-    <t>ActiveOptions[1]</t>
-  </si>
-  <si>
     <t>waitForClickable</t>
   </si>
   <si>
-    <t>ActiveOptions[2]</t>
-  </si>
-  <si>
     <t>waitForHidden</t>
   </si>
   <si>
-    <t>ActiveOptions[3]</t>
-  </si>
-  <si>
     <t>clear</t>
   </si>
   <si>
@@ -291,6 +328,15 @@
     <t>http://192.168.198.202/annotation-tool/#/user/login</t>
   </si>
   <si>
+    <t>ChronicCare</t>
+  </si>
+  <si>
+    <t>chronic-care demo</t>
+  </si>
+  <si>
+    <t>http://192.168.198.202/chronic-care/#/login</t>
+  </si>
+  <si>
     <t>default</t>
   </si>
   <si>
@@ -327,7 +373,7 @@
     <t>Template</t>
   </si>
   <si>
-    <t>Login</t>
+    <t>AnnotationLogin</t>
   </si>
   <si>
     <t>ChooseAnnotaion</t>
@@ -336,6 +382,18 @@
     <t>ImplementAnnotation</t>
   </si>
   <si>
+    <t>CCMLogin</t>
+  </si>
+  <si>
+    <t>CCMMemberList</t>
+  </si>
+  <si>
+    <t>CCMChronic</t>
+  </si>
+  <si>
+    <t>CCMEnrollment</t>
+  </si>
+  <si>
     <t>TestGroup ID</t>
   </si>
   <si>
@@ -394,6 +452,21 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>Jenny@meddataquest.com</t>
+  </si>
+  <si>
+    <t>clickByJS</t>
+  </si>
+  <si>
+    <t>CCM</t>
+  </si>
+  <si>
+    <t>enrollment</t>
+  </si>
+  <si>
+    <t>hz 910</t>
   </si>
 </sst>
 </file>
@@ -402,9 +475,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -424,14 +497,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,22 +520,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -475,71 +548,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -559,12 +571,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -587,25 +660,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,157 +840,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,6 +851,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -791,6 +897,21 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -820,21 +941,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -845,194 +951,163 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1358,12 +1433,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1372,302 +1447,362 @@
     <col min="2" max="2" width="13.1238095238095" customWidth="1"/>
     <col min="3" max="3" width="9.87619047619048" customWidth="1"/>
     <col min="4" max="4" width="13.8761904761905" customWidth="1"/>
-    <col min="5" max="7" width="20.8571428571429" customWidth="1"/>
-    <col min="9" max="9" width="10.1238095238095" customWidth="1"/>
+    <col min="5" max="11" width="20.8571428571429" customWidth="1"/>
+    <col min="13" max="13" width="10.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:10">
-      <c r="A1" s="5" t="s">
+    <row r="1" s="6" customFormat="1" spans="1:14">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="b">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="b">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="D3" s="9"/>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="b">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
+        <v>37</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
+        <v>44</v>
+      </c>
+      <c r="K5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
+        <v>47</v>
+      </c>
+      <c r="K6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>50</v>
+      </c>
+      <c r="K7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1677,18 +1812,200 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="15.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="23.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C1:C2 C5:C1048576">
+      <formula1>PageObjectModel!$J:$J</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2 D3 D4">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="17.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="22.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5">
+      <c r="E4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C2 C3:C1048576">
+      <formula1>PageObjectModel!$K:$K</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
+      <formula1>PageObjectModel!$B:$B</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="28.6285714285714" customWidth="1"/>
     <col min="2" max="2" width="38.752380952381" customWidth="1"/>
@@ -1696,38 +2013,58 @@
     <col min="5" max="5" width="14.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:6">
-      <c r="A1" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="5" t="s">
+    <row r="1" s="6" customFormat="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>77</v>
+      <c r="D3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1741,6 +2078,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="http://192.168.198.202/annotation-tool/#/user/login" tooltip="http://192.168.198.202/annotation-tool/#/user/login"/>
+    <hyperlink ref="D3" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1753,10 +2091,10 @@
   <sheetPr/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1769,36 +2107,36 @@
     <col min="6" max="6" width="8.24761904761905" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:10">
-      <c r="A1" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>87</v>
+    <row r="1" s="6" customFormat="1" spans="1:10">
+      <c r="A1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1827,7 +2165,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -1842,34 +2180,34 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" spans="1:3">
-      <c r="A1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" s="6" customFormat="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>89</v>
+      <c r="C1" s="6" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1880,7 +2218,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1891,12 +2229,56 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1905,7 +2287,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
       <formula1>PageObjectModel!$A:$A</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 C3:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 C5 C6 C7 C8 C3:C4 C9:C1048576">
       <formula1>Boolean</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3:A1048576">
@@ -1924,7 +2306,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -1937,64 +2319,64 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E4" s="4">
         <v>12345678</v>
@@ -2002,16 +2384,16 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2051,104 +2433,104 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -2174,7 +2556,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2186,390 +2568,390 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>99</v>
+        <v>73</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2587,4 +2969,202 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="19.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="17.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="20.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="26.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="4">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2 D3 D4 D5">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 C3:C5">
+      <formula1>PageObjectModel!$E:$E</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="Jenny@meddataquest.com" tooltip="mailto:Jenny@meddataquest.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="20.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="9.57142857142857"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" spans="1:5">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C1:C2 C4:C1048576">
+      <formula1>PageObjectModel!$I:$I</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" tooltip="mailto:Jenny@meddataquest.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update cmm testcase and object model
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510"/>
+    <workbookView windowWidth="27765" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="139">
   <si>
     <t>Page</t>
   </si>
@@ -223,6 +223,9 @@
     <t>Dropdowns[2]</t>
   </si>
   <si>
+    <t>BirthDate</t>
+  </si>
+  <si>
     <t>hover</t>
   </si>
   <si>
@@ -304,6 +307,18 @@
     <t>takescreen</t>
   </si>
   <si>
+    <t>select_ccm</t>
+  </si>
+  <si>
+    <t>select_rpm</t>
+  </si>
+  <si>
+    <t>select_enrollment</t>
+  </si>
+  <si>
+    <t>select_first_date_of_next_month</t>
+  </si>
+  <si>
     <t>TestCase ID</t>
   </si>
   <si>
@@ -458,12 +473,6 @@
   </si>
   <si>
     <t>clickByJS</t>
-  </si>
-  <si>
-    <t>CCM</t>
-  </si>
-  <si>
-    <t>enrollment</t>
   </si>
   <si>
     <t>hz 910</t>
@@ -474,10 +483,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -512,6 +521,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
@@ -526,8 +549,55 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -541,7 +611,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -555,25 +633,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -586,58 +647,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -660,7 +669,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,13 +765,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -690,7 +777,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,145 +849,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -857,8 +866,28 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -878,15 +907,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -902,17 +922,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -932,146 +946,141 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1080,26 +1089,26 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
@@ -1107,7 +1116,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1433,12 +1441,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1461,7 +1469,7 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -1505,7 +1513,7 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
@@ -1549,7 +1557,7 @@
       <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="8"/>
       <c r="E3" t="s">
         <v>27</v>
       </c>
@@ -1661,25 +1669,31 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:7">
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
       <c r="B8" t="s">
         <v>52</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
       </c>
+      <c r="K8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G10" t="s">
         <v>45</v>
@@ -1687,7 +1701,7 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
         <v>48</v>
@@ -1695,7 +1709,7 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
         <v>51</v>
@@ -1703,106 +1717,126 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="2:7">
       <c r="B15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1818,87 +1852,82 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="15.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="23.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="21.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D$1:D$1048576">
+      <formula1>PageObjectModel!$B:$B</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C1:C2 C5:C1048576">
       <formula1>PageObjectModel!$J:$J</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2 D3 D4">
-      <formula1>ActionKeyWords</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4">
       <formula1>TestCaseID</formula1>
@@ -1912,13 +1941,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="17.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="22.2857142857143" customWidth="1"/>
@@ -1926,27 +1955,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -1955,37 +1984,63 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="5:5">
-      <c r="E4" t="s">
-        <v>135</v>
+      <c r="D5" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C2 C3:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C1:C2 C3:C4 C6:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2015,36 +2070,36 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -2052,16 +2107,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>91</v>
+      <c r="D3" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -2091,10 +2146,10 @@
   <sheetPr/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2109,34 +2164,34 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2150,7 +2205,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>60</v>
@@ -2165,7 +2220,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -2185,7 +2240,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -2196,18 +2251,18 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -2218,7 +2273,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -2229,7 +2284,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2240,7 +2295,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2251,7 +2306,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -2262,7 +2317,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -2273,7 +2328,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -2319,41 +2374,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -2362,15 +2417,15 @@
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -2384,10 +2439,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -2433,27 +2488,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2465,10 +2520,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -2479,24 +2534,24 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
@@ -2507,24 +2562,24 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -2568,195 +2623,195 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
@@ -2767,98 +2822,98 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -2866,10 +2921,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
         <v>48</v>
@@ -2880,10 +2935,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
@@ -2894,10 +2949,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -2908,50 +2963,50 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B23" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2977,7 +3032,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -2990,41 +3045,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -3033,15 +3088,15 @@
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -3055,10 +3110,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -3105,27 +3160,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -3136,16 +3191,16 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E3" s="2"/>
     </row>

</xml_diff>

<commit_message>
update cmm  obejct model, optimize log message
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
+    <workbookView windowWidth="27765" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="163">
   <si>
     <t>Page</t>
   </si>
@@ -181,7 +181,7 @@
     <t>Selections[2]</t>
   </si>
   <si>
-    <t>GenderDropdown</t>
+    <t>Gender</t>
   </si>
   <si>
     <t>N/A</t>
@@ -232,57 +232,102 @@
     <t>Dropdowns[3]</t>
   </si>
   <si>
+    <t>Organization</t>
+  </si>
+  <si>
     <t>waitForVisible</t>
   </si>
   <si>
+    <t>Facility</t>
+  </si>
+  <si>
     <t>waitForClickable</t>
   </si>
   <si>
+    <t>City</t>
+  </si>
+  <si>
     <t>waitForHidden</t>
   </si>
   <si>
+    <t>CityInput</t>
+  </si>
+  <si>
     <t>waitSpecificTime</t>
   </si>
   <si>
     <t>SelectedOptions[1]</t>
   </si>
   <si>
+    <t>State</t>
+  </si>
+  <si>
     <t>clear</t>
   </si>
   <si>
     <t>SelectedOptions[2]</t>
   </si>
   <si>
+    <t>AdvancedDirectivesOptions[1]</t>
+  </si>
+  <si>
     <t>get</t>
   </si>
   <si>
     <t>SelectedOptions[3]</t>
   </si>
   <si>
+    <t>AdvancedDirectivesOptions[2]</t>
+  </si>
+  <si>
     <t>size</t>
   </si>
   <si>
+    <t>AdvancedDirectivesOptions[3]</t>
+  </si>
+  <si>
     <t>[value]</t>
   </si>
   <si>
+    <t>HomePhoneNumber</t>
+  </si>
+  <si>
     <t>[text]</t>
   </si>
   <si>
+    <t>HomePhoneNumberExt</t>
+  </si>
+  <si>
     <t>[class]</t>
   </si>
   <si>
+    <t>CellNumber</t>
+  </si>
+  <si>
     <t>clickIfVisible</t>
   </si>
   <si>
+    <t>CellNumberExt</t>
+  </si>
+  <si>
     <t>waitTextToBePresented</t>
   </si>
   <si>
+    <t>HomePhoneNumberPerferred</t>
+  </si>
+  <si>
     <t>waitForCheck</t>
   </si>
   <si>
+    <t>CellNumberPerferred</t>
+  </si>
+  <si>
     <t>waitUtilSelected</t>
   </si>
   <si>
+    <t>SubmitButton</t>
+  </si>
+  <si>
     <t>clickAndHold</t>
   </si>
   <si>
@@ -322,6 +367,9 @@
     <t>select_first_date_of_next_month</t>
   </si>
   <si>
+    <t>[css](border-bottom-color)</t>
+  </si>
+  <si>
     <t>TestCase ID</t>
   </si>
   <si>
@@ -479,6 +527,27 @@
   </si>
   <si>
     <t>hz 910</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>ShuRuiTECH</t>
+  </si>
+  <si>
+    <t>West Lake Test</t>
+  </si>
+  <si>
+    <t>Hollywood</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>1231231234</t>
+  </si>
+  <si>
+    <t>rgba(245, 34, 45,1)</t>
   </si>
 </sst>
 </file>
@@ -486,10 +555,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -530,26 +599,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -561,14 +615,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -584,6 +645,14 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="等线"/>
@@ -591,15 +660,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,8 +684,23 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,25 +714,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -672,7 +741,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,7 +765,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,19 +807,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,133 +921,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -884,17 +953,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -914,15 +977,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -934,6 +988,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -953,107 +1018,111 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1062,28 +1131,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1092,19 +1161,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1114,9 +1183,9 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1444,12 +1513,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1686,165 +1755,215 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:11">
       <c r="B9" t="s">
         <v>55</v>
       </c>
       <c r="G9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
       <c r="B10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="2:7">
+      <c r="K10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
       <c r="B11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="K11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
       <c r="B12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="2:7">
+      <c r="K12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7">
+        <v>65</v>
+      </c>
+      <c r="K13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11">
       <c r="B14" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7">
+        <v>68</v>
+      </c>
+      <c r="K14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11">
       <c r="B15" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2">
+        <v>71</v>
+      </c>
+      <c r="K15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
+        <v>73</v>
+      </c>
+      <c r="K16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
       <c r="B17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
+        <v>75</v>
+      </c>
+      <c r="K17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11">
       <c r="B18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
+        <v>79</v>
+      </c>
+      <c r="K19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11">
       <c r="B20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
+        <v>81</v>
+      </c>
+      <c r="K20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11">
       <c r="B21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
+        <v>83</v>
+      </c>
+      <c r="K21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
+        <v>85</v>
+      </c>
+      <c r="K22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
       <c r="B23" t="s">
-        <v>73</v>
+        <v>87</v>
+      </c>
+      <c r="K23" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>86</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1860,7 +1979,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1872,47 +1991,47 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1935,55 +2054,57 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="17.5714285714286" customWidth="1"/>
-    <col min="3" max="3" width="22.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="31.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="32.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="10.5714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -1992,49 +2113,393 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" t="s">
+        <v>137</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>102</v>
+      </c>
+      <c r="E25" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26">
+        <v>1234567890</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C1:C2 C3:C4 C6:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C8 C21 C22 C1:C2 C3:C4 C6:C7 C9:C16 C17:C20 C23:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2048,7 +2513,7 @@
   <sheetPr/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
@@ -2064,36 +2529,36 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>94</v>
+      <c r="D2" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -2101,16 +2566,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>97</v>
+      <c r="D3" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -2140,10 +2605,10 @@
   <sheetPr/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2158,42 +2623,42 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -2205,7 +2670,7 @@
         <v>60</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -2214,7 +2679,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>3</v>
@@ -2245,18 +2710,18 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -2267,7 +2732,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -2278,7 +2743,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2289,7 +2754,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2300,7 +2765,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -2311,7 +2776,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -2322,7 +2787,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -2368,41 +2833,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -2410,16 +2875,16 @@
       <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>122</v>
+      <c r="E3" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -2427,16 +2892,16 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>12345678</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -2482,27 +2947,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -2510,14 +2975,14 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -2528,24 +2993,24 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>43</v>
@@ -2556,24 +3021,24 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -2617,195 +3082,195 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>76</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>125</v>
+        <v>91</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>131</v>
+        <v>91</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C12" t="s">
         <v>47</v>
@@ -2816,95 +3281,95 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C14" t="s">
         <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C18" t="s">
         <v>56</v>
@@ -2915,10 +3380,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C19" t="s">
         <v>48</v>
@@ -2929,10 +3394,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s">
         <v>50</v>
@@ -2943,10 +3408,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -2957,50 +3422,50 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>135</v>
+        <v>77</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C23" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>136</v>
+        <v>77</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3039,41 +3504,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -3081,16 +3546,16 @@
       <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>137</v>
+      <c r="E3" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -3098,16 +3563,16 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>12345678</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -3154,27 +3619,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -3185,18 +3650,18 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="E3" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="3">

</xml_diff>

<commit_message>
update template flow and optimize member finder fucntion
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="5" activeTab="10"/>
+    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -14,10 +14,11 @@
     <sheet name="AnnotationLoginPage" sheetId="22" r:id="rId5"/>
     <sheet name="AnnotationHomePage" sheetId="23" r:id="rId6"/>
     <sheet name="AnnotationImplementPage" sheetId="24" r:id="rId7"/>
-    <sheet name="CCMLoginPage" sheetId="25" r:id="rId8"/>
-    <sheet name="CCMMemberPage" sheetId="26" r:id="rId9"/>
-    <sheet name="CCMChronicPage" sheetId="27" r:id="rId10"/>
-    <sheet name="CCMEnrollmentPage" sheetId="28" r:id="rId11"/>
+    <sheet name="Login" sheetId="29" r:id="rId8"/>
+    <sheet name="CCMLoginPage" sheetId="25" r:id="rId9"/>
+    <sheet name="CCMMemberPage" sheetId="26" r:id="rId10"/>
+    <sheet name="CCMChronicPage" sheetId="27" r:id="rId11"/>
+    <sheet name="CCMEnrollmentPage" sheetId="28" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$M$2:$M$4</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="167">
   <si>
     <t>Page</t>
   </si>
@@ -109,7 +110,7 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>Searching</t>
+    <t>Login</t>
   </si>
   <si>
     <t>UserName</t>
@@ -181,6 +182,9 @@
     <t>Selections[2]</t>
   </si>
   <si>
+    <t>MembersList</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -331,9 +335,15 @@
     <t>clickAndHold</t>
   </si>
   <si>
+    <t>ErrorMessage[1]</t>
+  </si>
+  <si>
     <t>drogAndDropRichBox</t>
   </si>
   <si>
+    <t>ErrorMessage[2]</t>
+  </si>
+  <si>
     <t>selectPartialContextByIndex</t>
   </si>
   <si>
@@ -448,9 +458,6 @@
     <t>ImplementAnnotation</t>
   </si>
   <si>
-    <t>CCMLogin</t>
-  </si>
-  <si>
     <t>CCMMemberList</t>
   </si>
   <si>
@@ -523,7 +530,7 @@
     <t>Jenny@meddataquest.com</t>
   </si>
   <si>
-    <t>clickByJS</t>
+    <t>selectMemberByMID</t>
   </si>
   <si>
     <t>hz 910</t>
@@ -548,6 +555,12 @@
   </si>
   <si>
     <t>rgba(245, 34, 45,1)</t>
+  </si>
+  <si>
+    <t>Ext is wrong format!</t>
+  </si>
+  <si>
+    <t>Cell Number is required</t>
   </si>
 </sst>
 </file>
@@ -556,8 +569,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -599,6 +612,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -607,13 +657,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -629,42 +711,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -677,44 +727,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -747,6 +760,96 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -759,25 +862,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -789,139 +934,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -944,11 +957,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -958,6 +977,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,21 +1031,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1035,145 +1048,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1516,9 +1529,9 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1683,17 +1696,20 @@
       <c r="H4" t="s">
         <v>37</v>
       </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1701,16 +1717,16 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1718,13 +1734,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1732,13 +1748,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1746,224 +1762,230 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:11">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K18" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K19" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K22" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11">
       <c r="B24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
+        <v>90</v>
+      </c>
+      <c r="K24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11">
       <c r="B25" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="K25" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1984,6 +2006,91 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
+    <col min="1" max="1" width="20.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
+    <col min="4" max="4" width="25.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="9.57142857142857"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1" spans="1:5">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E3" s="3">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C1:C2 C4:C1048576">
+      <formula1>PageObjectModel!$I:$I</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" display="40" tooltip="mailto:Jenny@meddataquest.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <cols>
     <col min="1" max="1" width="15.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="23.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="21.2857142857143" customWidth="1"/>
@@ -1991,47 +2098,47 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2051,13 +2158,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2065,32 +2172,32 @@
     <col min="1" max="1" width="17.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="31.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="32.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="10.5714285714286"/>
+    <col min="5" max="5" width="11.7142857142857"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -2101,10 +2208,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -2113,46 +2220,46 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>35</v>
@@ -2160,13 +2267,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
@@ -2174,30 +2281,30 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
         <v>35</v>
@@ -2205,13 +2312,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -2219,47 +2326,47 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E12" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
         <v>35</v>
@@ -2267,30 +2374,30 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
@@ -2298,78 +2405,78 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E17" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
@@ -2380,154 +2487,188 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E21" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
         <v>78</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" t="s">
         <v>25</v>
       </c>
-      <c r="E22">
+      <c r="E23">
         <v>1234</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>111</v>
-      </c>
-      <c r="B26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
         <v>25</v>
       </c>
-      <c r="E27">
+      <c r="E29">
         <v>1234567890</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C29" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" t="s">
-        <v>97</v>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C8 C21 C22 C23 C29 C1:C2 C3:C4 C6:C7 C9:C16 C17:C20 C24:C28 C30:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5 C8 C21 C22 C23 C24 C28 C31 C1:C2 C3:C4 C6:C7 C9:C16 C17:C20 C25:C27 C29:C30 C32:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2541,10 +2682,10 @@
   <sheetPr/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="5"/>
@@ -2557,36 +2698,36 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -2594,16 +2735,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -2636,7 +2777,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2651,34 +2792,34 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2710,7 +2851,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2727,7 +2868,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="2"/>
@@ -2738,18 +2879,18 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -2760,7 +2901,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -2771,7 +2912,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2782,18 +2923,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -2804,7 +2945,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -2815,7 +2956,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -2861,41 +3002,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -2904,15 +3045,15 @@
         <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -2926,10 +3067,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -2975,27 +3116,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -3007,10 +3148,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -3021,27 +3162,27 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -3049,24 +3190,24 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -3110,198 +3251,198 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B9" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
         <v>14</v>
@@ -3309,98 +3450,98 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
         <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E15" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
         <v>14</v>
@@ -3408,13 +3549,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>14</v>
@@ -3422,13 +3563,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
         <v>14</v>
@@ -3436,13 +3577,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -3450,50 +3591,50 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3516,10 +3657,71 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="2">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 C1:XFD1">
+      <formula1>ContactPage</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="Jenny@meddataquest.com" tooltip="mailto:Jenny@meddataquest.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -3532,41 +3734,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -3575,15 +3777,15 @@
         <v>25</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -3597,10 +3799,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -3627,86 +3829,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
-  <cols>
-    <col min="1" max="1" width="20.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="9.57142857142857"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" ht="15" customHeight="1" spans="1:5">
-      <c r="A3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="3"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C1:C2 C4:C1048576">
-      <formula1>PageObjectModel!$I:$I</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
-      <formula1>ActionKeyWords</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3">
-      <formula1>TestCaseID</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" tooltip="mailto:Jenny@meddataquest.com"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add generatevaluebyregex, refactoring code
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="6" activeTab="11"/>
+    <workbookView windowWidth="27765" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="172">
   <si>
     <t>Page</t>
   </si>
@@ -554,7 +554,7 @@
     <t>MD</t>
   </si>
   <si>
-    <t>1231231234</t>
+    <t>[regex]((^[0-9]{3}-[0-9]{3}-[0-9]{4}$)|(^[0-9]{10}$))</t>
   </si>
   <si>
     <t>rgba(245, 34, 45,1)</t>
@@ -563,13 +563,19 @@
     <t>Ext is wrong format!</t>
   </si>
   <si>
+    <t>[regex]((^[0-9]{4}$))</t>
+  </si>
+  <si>
     <t>Cell Number is required</t>
   </si>
   <si>
+    <t>z@.com</t>
+  </si>
+  <si>
+    <t>Email is wrong format</t>
+  </si>
+  <si>
     <t>[regex](^[a-zA-Z0-9_.+-]+@[a-zA-Z0-9-]+\\.[a-zA-Z0-9-.]+$)</t>
-  </si>
-  <si>
-    <t>Email is wrong format</t>
   </si>
 </sst>
 </file>
@@ -577,8 +583,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -600,7 +606,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -608,9 +614,24 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -629,25 +650,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -659,45 +664,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -713,15 +682,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -739,6 +730,21 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -763,7 +769,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,7 +793,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,19 +811,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -811,13 +823,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,7 +841,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -841,13 +865,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -859,19 +895,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -883,43 +919,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,18 +950,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -960,8 +966,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -969,32 +975,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1016,10 +998,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1036,6 +1016,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1057,148 +1063,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1206,9 +1212,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2068,7 +2074,7 @@
       <c r="D3" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>40</v>
       </c>
     </row>
@@ -2173,10 +2179,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="$A26:$XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2184,7 +2190,7 @@
     <col min="1" max="1" width="17.5714285714286" customWidth="1"/>
     <col min="3" max="3" width="31.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="32.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="11.7142857142857"/>
+    <col min="5" max="5" width="58.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
@@ -2530,8 +2536,8 @@
       <c r="D22" t="s">
         <v>25</v>
       </c>
-      <c r="E22">
-        <v>1234</v>
+      <c r="E22" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2607,7 +2613,7 @@
         <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2640,8 +2646,8 @@
       <c r="D29" t="s">
         <v>25</v>
       </c>
-      <c r="E29" t="s">
-        <v>168</v>
+      <c r="E29" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
@@ -2658,10 +2664,10 @@
         <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
         <v>115</v>
       </c>
@@ -2669,10 +2675,13 @@
         <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>14</v>
+        <v>25</v>
+      </c>
+      <c r="E31" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2686,24 +2695,41 @@
         <v>89</v>
       </c>
       <c r="D32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
         <v>101</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C20 C21 C22 C23 C27 C28 C29 C30 C31 C32 C1:C2 C3:C4 C5:C6 C8:C15 C16:C19 C24:C26 C34:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C20 C21 C22 C23 C27 C28 C29 C30 C31 C32 C33 C1:C2 C3:C4 C5:C6 C8:C15 C16:C19 C24:C26 C34:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E29" r:id="rId1" display="z@.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2758,7 +2784,7 @@
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>114</v>
       </c>
       <c r="E2" t="s">
@@ -2775,7 +2801,7 @@
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>117</v>
       </c>
       <c r="E3" t="s">
@@ -2806,10 +2832,10 @@
   <sheetPr/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2862,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>30</v>
@@ -2880,7 +2906,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -3076,7 +3102,7 @@
       <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3311,7 +3337,7 @@
       <c r="D2" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -3723,7 +3749,7 @@
       <c r="B2" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>156</v>
       </c>
       <c r="D2" s="2">
@@ -3808,7 +3834,7 @@
       <c r="D3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>156</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update testcase with log diff
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="6" activeTab="11"/>
+    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="CCMMemberPage" sheetId="26" r:id="rId10"/>
     <sheet name="CCMChronicPage" sheetId="27" r:id="rId11"/>
     <sheet name="CCMEnrollmentPage" sheetId="28" r:id="rId12"/>
+    <sheet name="CCMChronicLogPage" sheetId="30" r:id="rId13"/>
   </sheets>
   <definedNames>
-    <definedName name="Acceptable">PageObjectModel!$M$2:$M$4</definedName>
+    <definedName name="Acceptable">PageObjectModel!$N$2:$N$4</definedName>
     <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$22</definedName>
     <definedName name="AdditionalOnePage">PageObjectModel!#REF!</definedName>
     <definedName name="AdditionalTwoPage">PageObjectModel!#REF!</definedName>
-    <definedName name="Boolean">PageObjectModel!$L$2:$L$3</definedName>
+    <definedName name="Boolean">PageObjectModel!$M$2:$M$3</definedName>
     <definedName name="Browser">PageObjectModel!$C$2:$C$7</definedName>
     <definedName name="ContactPage">PageObjectModel!#REF!</definedName>
     <definedName name="CustomCoveragePage">PageObjectModel!#REF!</definedName>
@@ -53,14 +54,14 @@
     <definedName name="VehicleOwnedMonthsOptions">PageObjectModel!#REF!</definedName>
     <definedName name="VehicleUsage">PageObjectModel!#REF!</definedName>
     <definedName name="Violations">PageObjectModel!#REF!</definedName>
-    <definedName name="YesNo">PageObjectModel!$N$2:$N$4</definedName>
+    <definedName name="YesNo">PageObjectModel!$O$2:$O$4</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="180">
   <si>
     <t>Page</t>
   </si>
@@ -95,6 +96,9 @@
     <t>CCMEnrollmentPage</t>
   </si>
   <si>
+    <t>CCMChronicLogPage</t>
+  </si>
+  <si>
     <t>Boolean</t>
   </si>
   <si>
@@ -128,405 +132,426 @@
     <t>CCMOrRPMPanel</t>
   </si>
   <si>
+    <t>CCMMemberTabs</t>
+  </si>
+  <si>
+    <t>LogList[1]</t>
+  </si>
+  <si>
+    <t>ACCEPT</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>MyTaskSubMenu</t>
+  </si>
+  <si>
+    <t>Selections[1]</t>
+  </si>
+  <si>
+    <t>Member40</t>
+  </si>
+  <si>
     <t>DemographicsButton</t>
   </si>
   <si>
-    <t>ACCEPT</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>enter</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>MyTaskSubMenu</t>
-  </si>
-  <si>
-    <t>Selections[1]</t>
-  </si>
-  <si>
-    <t>Member40</t>
-  </si>
-  <si>
-    <t>CCMMemberTabs</t>
+    <t>Birthdate</t>
+  </si>
+  <si>
+    <t>DECLINE</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>focus</t>
+  </si>
+  <si>
+    <t>ie</t>
+  </si>
+  <si>
+    <t>LoginButton</t>
+  </si>
+  <si>
+    <t>FirstTask</t>
+  </si>
+  <si>
+    <t>Selections[2]</t>
+  </si>
+  <si>
+    <t>MembersList</t>
   </si>
   <si>
     <t>PrimaryCareId</t>
   </si>
   <si>
-    <t>DECLINE</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>focus</t>
-  </si>
-  <si>
-    <t>ie</t>
-  </si>
-  <si>
-    <t>LoginButton</t>
-  </si>
-  <si>
-    <t>FirstTask</t>
-  </si>
-  <si>
-    <t>Selections[2]</t>
-  </si>
-  <si>
-    <t>MembersList</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>blur</t>
+  </si>
+  <si>
+    <t>TestTask</t>
+  </si>
+  <si>
+    <t>Selections[3]</t>
   </si>
   <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>blur</t>
-  </si>
-  <si>
-    <t>TestTask</t>
-  </si>
-  <si>
-    <t>Selections[3]</t>
+    <t>HomePhoneNumber</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>AddIcon</t>
   </si>
   <si>
     <t>ActiveOptions[1]</t>
   </si>
   <si>
-    <t>select</t>
-  </si>
-  <si>
-    <t>AddIcon</t>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Dropdowns[1]</t>
   </si>
   <si>
     <t>ActiveOptions[2]</t>
   </si>
   <si>
-    <t>check</t>
-  </si>
-  <si>
-    <t>Dropdowns[1]</t>
+    <t>doubleClick</t>
+  </si>
+  <si>
+    <t>Dropdowns[2]</t>
   </si>
   <si>
     <t>ActiveOptions[3]</t>
   </si>
   <si>
-    <t>doubleClick</t>
-  </si>
-  <si>
-    <t>Dropdowns[2]</t>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>Dropdowns[3]</t>
   </si>
   <si>
     <t>BirthDate</t>
   </si>
   <si>
-    <t>hover</t>
-  </si>
-  <si>
-    <t>Dropdowns[3]</t>
+    <t>waitForVisible</t>
   </si>
   <si>
     <t>Organization</t>
   </si>
   <si>
-    <t>waitForVisible</t>
+    <t>waitForClickable</t>
   </si>
   <si>
     <t>Facility</t>
   </si>
   <si>
-    <t>waitForClickable</t>
+    <t>waitForHidden</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>waitForHidden</t>
+    <t>waitSpecificTime</t>
+  </si>
+  <si>
+    <t>SelectedOptions[1]</t>
   </si>
   <si>
     <t>CityInput</t>
   </si>
   <si>
-    <t>waitSpecificTime</t>
-  </si>
-  <si>
-    <t>SelectedOptions[1]</t>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>SelectedOptions[2]</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>clear</t>
-  </si>
-  <si>
-    <t>SelectedOptions[2]</t>
+    <t>[value]</t>
+  </si>
+  <si>
+    <t>SelectedOptions[3]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[1]</t>
   </si>
   <si>
-    <t>[value]</t>
-  </si>
-  <si>
-    <t>SelectedOptions[3]</t>
+    <t>[text]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[2]</t>
   </si>
   <si>
-    <t>[text]</t>
+    <t>[class]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[3]</t>
   </si>
   <si>
-    <t>[class]</t>
-  </si>
-  <si>
-    <t>HomePhoneNumber</t>
-  </si>
-  <si>
     <t>clickIfVisible</t>
   </si>
   <si>
+    <t>waitTextToBePresented</t>
+  </si>
+  <si>
     <t>HomePhoneNumberExt</t>
   </si>
   <si>
-    <t>waitTextToBePresented</t>
+    <t>waitForCheck</t>
   </si>
   <si>
     <t>CellNumber</t>
   </si>
   <si>
-    <t>waitForCheck</t>
+    <t>waitUtilSelected</t>
   </si>
   <si>
     <t>CellNumberExt</t>
   </si>
   <si>
-    <t>waitUtilSelected</t>
+    <t>clickAndHold</t>
   </si>
   <si>
     <t>HomePhoneNumberPerferred</t>
   </si>
   <si>
-    <t>clickAndHold</t>
+    <t>drogAndDropRichBox</t>
   </si>
   <si>
     <t>CellNumberPerferred</t>
   </si>
   <si>
-    <t>drogAndDropRichBox</t>
+    <t>selectPartialContextByIndex</t>
   </si>
   <si>
     <t>SubmitButton</t>
   </si>
   <si>
-    <t>selectPartialContextByIndex</t>
+    <t>sendKey</t>
   </si>
   <si>
     <t>ErrorMessage</t>
   </si>
   <si>
-    <t>sendKey</t>
+    <t>sendKeyByRobot</t>
   </si>
   <si>
     <t>ErrorMessage[1]</t>
   </si>
   <si>
-    <t>sendKeyByRobot</t>
+    <t>rightClick</t>
   </si>
   <si>
     <t>ErrorMessage[2]</t>
   </si>
   <si>
-    <t>rightClick</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>[css](background-color)</t>
   </si>
   <si>
     <t>[attr](style)</t>
   </si>
   <si>
+    <t>[css](border-bottom-color)</t>
+  </si>
+  <si>
+    <t>takescreen</t>
+  </si>
+  <si>
+    <t>select_enrollment</t>
+  </si>
+  <si>
+    <t>select_chronic_log</t>
+  </si>
+  <si>
+    <t>select_ccm_if_visible</t>
+  </si>
+  <si>
+    <t>select_rpm_if_visible</t>
+  </si>
+  <si>
+    <t>select_first_date_of_next_month</t>
+  </si>
+  <si>
+    <t>[log_is_changed]</t>
+  </si>
+  <si>
+    <t>TestCase ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Site URL</t>
+  </si>
+  <si>
+    <t>Remote Hub</t>
+  </si>
+  <si>
+    <t>AnnotationTool</t>
+  </si>
+  <si>
+    <t>annotation tool</t>
+  </si>
+  <si>
+    <t>http://192.168.198.202/annotation-tool/#/user/login</t>
+  </si>
+  <si>
+    <t>ChronicCare_Demographics</t>
+  </si>
+  <si>
+    <t>chronic-care demo</t>
+  </si>
+  <si>
+    <t>http://192.168.198.202/chronic-care/#/login</t>
+  </si>
+  <si>
+    <t>ChronicCare_Enrollment</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>waitOrDelay</t>
+  </si>
+  <si>
+    <t>redirect</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>implict</t>
+  </si>
+  <si>
+    <t>explict</t>
+  </si>
+  <si>
+    <t>retry</t>
+  </si>
+  <si>
+    <t>sleepTime</t>
+  </si>
+  <si>
+    <t>FlowName</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>AnnotationLogin</t>
+  </si>
+  <si>
+    <t>ChooseAnnotaion</t>
+  </si>
+  <si>
+    <t>ImplementAnnotation</t>
+  </si>
+  <si>
+    <t>CCMMemberList</t>
+  </si>
+  <si>
+    <t>CCMChronic</t>
+  </si>
+  <si>
+    <t>CCMEnrollment</t>
+  </si>
+  <si>
+    <t>CCMChronicLog</t>
+  </si>
+  <si>
+    <t>TestGroup ID</t>
+  </si>
+  <si>
+    <t>Target Name</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>TS_01</t>
+  </si>
+  <si>
+    <t>dong</t>
+  </si>
+  <si>
+    <t>10,10,800,300</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>22,28</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>rgba(205, 79, 57, 1)</t>
+  </si>
+  <si>
+    <t>73,79</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>rgba(204, 152, 229,1)</t>
+  </si>
+  <si>
+    <t>114,123</t>
+  </si>
+  <si>
+    <t>25,35</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>rgba(206, 206, 206, 1)</t>
+  </si>
+  <si>
+    <t>InspPalpBreasts</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
     <t>takeScreen</t>
   </si>
   <si>
-    <t>select_ccm_if_visible</t>
-  </si>
-  <si>
-    <t>select_rpm_if_visible</t>
-  </si>
-  <si>
-    <t>select_enrollment</t>
-  </si>
-  <si>
-    <t>select_first_date_of_next_month</t>
-  </si>
-  <si>
-    <t>[css](border-bottom-color)</t>
-  </si>
-  <si>
-    <t>TestCase ID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Enabled</t>
-  </si>
-  <si>
-    <t>Site URL</t>
-  </si>
-  <si>
-    <t>Remote Hub</t>
-  </si>
-  <si>
-    <t>AnnotationTool</t>
-  </si>
-  <si>
-    <t>annotation tool</t>
-  </si>
-  <si>
-    <t>http://192.168.198.202/annotation-tool/#/user/login</t>
-  </si>
-  <si>
-    <t>ChronicCare</t>
-  </si>
-  <si>
-    <t>chronic-care demo</t>
-  </si>
-  <si>
-    <t>http://192.168.198.202/chronic-care/#/login</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>operation</t>
-  </si>
-  <si>
-    <t>waitOrDelay</t>
-  </si>
-  <si>
-    <t>redirect</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>implict</t>
-  </si>
-  <si>
-    <t>explict</t>
-  </si>
-  <si>
-    <t>retry</t>
-  </si>
-  <si>
-    <t>sleepTime</t>
-  </si>
-  <si>
-    <t>FlowName</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>AnnotationLogin</t>
-  </si>
-  <si>
-    <t>ChooseAnnotaion</t>
-  </si>
-  <si>
-    <t>ImplementAnnotation</t>
-  </si>
-  <si>
-    <t>CCMMemberList</t>
-  </si>
-  <si>
-    <t>CCMChronic</t>
-  </si>
-  <si>
-    <t>CCMEnrollment</t>
-  </si>
-  <si>
-    <t>TestGroup ID</t>
-  </si>
-  <si>
-    <t>Target Name</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>TS_01</t>
-  </si>
-  <si>
-    <t>dong</t>
-  </si>
-  <si>
-    <t>10,10,800,300</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>22,28</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>rgba(205, 79, 57, 1)</t>
-  </si>
-  <si>
-    <t>73,79</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>rgba(204, 152, 229,1)</t>
-  </si>
-  <si>
-    <t>114,123</t>
-  </si>
-  <si>
-    <t>25,35</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>rgba(206, 206, 206, 1)</t>
-  </si>
-  <si>
-    <t>InspPalpBreasts</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
     <t>Jenny@meddataquest.com</t>
   </si>
   <si>
@@ -573,6 +598,9 @@
   </si>
   <si>
     <t>[regex](^[a-zA-Z0-9_.+-]+@[a-zA-Z0-9-]+\\.[a-zA-Z0-9-.]+$)</t>
+  </si>
+  <si>
+    <t>TS_02</t>
   </si>
 </sst>
 </file>
@@ -580,10 +608,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -624,8 +652,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -639,9 +668,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -651,6 +679,14 @@
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -670,10 +706,39 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -686,15 +751,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -708,40 +766,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -772,7 +800,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -784,13 +848,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -802,49 +890,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -862,55 +944,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,31 +968,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -962,6 +990,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -970,16 +1009,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1003,16 +1042,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1032,113 +1071,102 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1147,37 +1175,37 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1186,22 +1214,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1538,12 +1566,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1552,11 +1580,11 @@
     <col min="2" max="2" width="13.1238095238095" customWidth="1"/>
     <col min="3" max="3" width="9.87619047619048" customWidth="1"/>
     <col min="4" max="4" width="13.8761904761905" customWidth="1"/>
-    <col min="5" max="11" width="20.8571428571429" customWidth="1"/>
-    <col min="13" max="13" width="10.1238095238095" customWidth="1"/>
+    <col min="5" max="12" width="20.8571428571429" customWidth="1"/>
+    <col min="14" max="14" width="10.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:14">
+    <row r="1" s="6" customFormat="1" spans="1:15">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1599,146 +1627,161 @@
       <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="b">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
-        <v>23</v>
-      </c>
       <c r="N2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>25</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
         <v>29</v>
       </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" t="b">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="b">
         <v>0</v>
       </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
       <c r="N3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" t="s">
-        <v>37</v>
-      </c>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>45</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1746,13 +1789,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1760,13 +1803,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1774,226 +1817,242 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="K8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="K10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="K11" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="K12" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="K13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="K14" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K16" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="K17" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="K18" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K19" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="K21" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="K22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K23" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="K24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K25" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K26" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
       <c r="B28" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+      <c r="K28" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>105</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2068,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -2022,47 +2081,47 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E3" s="4">
         <v>40</v>
@@ -2094,7 +2153,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -2106,47 +2165,47 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2169,10 +2228,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2185,295 +2244,295 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E15" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <v>123</v>
@@ -2481,143 +2540,143 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B26" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E26" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B27" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E27" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E28">
         <v>1234567890</v>
@@ -2625,81 +2684,95 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" t="s">
+        <v>146</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2707,13 +2780,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C20 C21 C22 C23 C27 C28 C29 C30 C31 C32 C33 C1:C2 C3:C4 C5:C6 C8:C15 C16:C19 C24:C26 C34:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9 A10 A11 A12 A13 A14 A15 A16 A17 A18 A19 A20 A21 A22 A23 A24 A25 A26 A27 A28 A29 A30 A31 A32 A33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2:A34">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2725,18 +2798,137 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="20.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="30.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="33.2857142857143" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5">
+      <formula1>PageObjectModel!$B:$B</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+      <formula1>PageObjectModel!$L:$L</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
+      <formula1>ActionKeyWords</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2:A5">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="28.6285714285714" customWidth="1"/>
     <col min="2" max="2" width="38.752380952381" customWidth="1"/>
@@ -2746,56 +2938,73 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2810,6 +3019,7 @@
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="http://192.168.198.202/annotation-tool/#/user/login" tooltip="http://192.168.198.202/annotation-tool/#/user/login"/>
     <hyperlink ref="D3" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
+    <hyperlink ref="D4" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2825,7 +3035,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2840,34 +3050,34 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2896,7 +3106,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -2911,15 +3121,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.5714285714286" customWidth="1"/>
@@ -2927,18 +3137,18 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -2949,7 +3159,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -2960,7 +3170,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2971,7 +3181,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -2982,7 +3192,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -2993,7 +3203,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -3004,12 +3214,23 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3037,7 +3258,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -3050,64 +3271,64 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
       <c r="E4" s="2">
         <v>12345678</v>
@@ -3115,16 +3336,16 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3164,104 +3385,104 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3299,390 +3520,390 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E13" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B20" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B22" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3708,39 +3929,39 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="1" max="1" width="21.4285714285714" customWidth="1"/>
     <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="D2" s="2">
         <v>12345678</v>
@@ -3769,7 +3990,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -3782,64 +4003,64 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
       </c>
       <c r="E4" s="2">
         <v>12345678</v>
@@ -3847,16 +4068,16 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update care plan status related testcase, update framework to handle component  filed reflect
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$N$2:$N$4</definedName>
-    <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$22</definedName>
+    <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$23</definedName>
     <definedName name="AdditionalOnePage">PageObjectModel!#REF!</definedName>
     <definedName name="AdditionalTwoPage">PageObjectModel!#REF!</definedName>
     <definedName name="Boolean">PageObjectModel!$M$2:$M$3</definedName>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="187">
   <si>
     <t>Page</t>
   </si>
@@ -192,6 +192,9 @@
     <t>MembersList</t>
   </si>
   <si>
+    <t>CarePlanProblem</t>
+  </si>
+  <si>
     <t>PrimaryCareId</t>
   </si>
   <si>
@@ -210,6 +213,9 @@
     <t>Selections[3]</t>
   </si>
   <si>
+    <t>LastPageNumberButton</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -222,6 +228,9 @@
     <t>AddIcon</t>
   </si>
   <si>
+    <t>LastMemberOfPage</t>
+  </si>
+  <si>
     <t>ActiveOptions[1]</t>
   </si>
   <si>
@@ -309,66 +318,72 @@
     <t>AdvancedDirectivesOptions[3]</t>
   </si>
   <si>
+    <t>clickifenabled</t>
+  </si>
+  <si>
     <t>clickIfVisible</t>
   </si>
   <si>
+    <t>HomePhoneNumberExt</t>
+  </si>
+  <si>
     <t>waitTextToBePresented</t>
   </si>
   <si>
-    <t>HomePhoneNumberExt</t>
+    <t>CellNumber</t>
   </si>
   <si>
     <t>waitForCheck</t>
   </si>
   <si>
-    <t>CellNumber</t>
+    <t>CellNumberExt</t>
   </si>
   <si>
     <t>waitUtilSelected</t>
   </si>
   <si>
-    <t>CellNumberExt</t>
+    <t>HomePhoneNumberPerferred</t>
   </si>
   <si>
     <t>clickAndHold</t>
   </si>
   <si>
-    <t>HomePhoneNumberPerferred</t>
+    <t>CellNumberPerferred</t>
   </si>
   <si>
     <t>drogAndDropRichBox</t>
   </si>
   <si>
-    <t>CellNumberPerferred</t>
+    <t>SubmitButton</t>
   </si>
   <si>
     <t>selectPartialContextByIndex</t>
   </si>
   <si>
-    <t>SubmitButton</t>
+    <t>ErrorMessage</t>
   </si>
   <si>
     <t>sendKey</t>
   </si>
   <si>
-    <t>ErrorMessage</t>
+    <t>ErrorMessage[1]</t>
   </si>
   <si>
     <t>sendKeyByRobot</t>
   </si>
   <si>
-    <t>ErrorMessage[1]</t>
+    <t>ErrorMessage[2]</t>
   </si>
   <si>
     <t>rightClick</t>
   </si>
   <si>
-    <t>ErrorMessage[2]</t>
-  </si>
-  <si>
     <t>[css](background-color)</t>
   </si>
   <si>
+    <t>ConsentValue</t>
+  </si>
+  <si>
     <t>[attr](style)</t>
   </si>
   <si>
@@ -381,6 +396,9 @@
     <t>select_enrollment</t>
   </si>
   <si>
+    <t>select_care_plan</t>
+  </si>
+  <si>
     <t>select_chronic_log</t>
   </si>
   <si>
@@ -558,6 +576,12 @@
     <t>selectMemberByMID</t>
   </si>
   <si>
+    <t>TS_02</t>
+  </si>
+  <si>
+    <t>No Data</t>
+  </si>
+  <si>
     <t>hz 910</t>
   </si>
   <si>
@@ -598,9 +622,6 @@
   </si>
   <si>
     <t>[regex](^[a-zA-Z0-9_.+-]+@[a-zA-Z0-9-]+\\.[a-zA-Z0-9-.]+$)</t>
-  </si>
-  <si>
-    <t>TS_02</t>
   </si>
 </sst>
 </file>
@@ -1566,12 +1587,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1748,20 +1769,23 @@
       <c r="I4" t="s">
         <v>42</v>
       </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1769,19 +1793,22 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
+        <v>50</v>
       </c>
       <c r="K5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1789,13 +1816,16 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="I6" t="s">
+        <v>55</v>
       </c>
       <c r="K6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1803,13 +1833,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1817,13 +1847,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1831,228 +1861,241 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="K11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G13" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K15" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K16" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K17" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="K18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K19" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K20" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="K21" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K22" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="K23" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K24" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="K27" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11">
       <c r="B29" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="K29" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>110</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2065,15 +2108,15 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.8571428571429" customWidth="1"/>
+    <col min="1" max="1" width="30.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="23.4285714285714" customWidth="1"/>
     <col min="4" max="4" width="25.2857142857143" customWidth="1"/>
     <col min="5" max="5" width="9.57142857142857"/>
@@ -2081,27 +2124,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -2112,30 +2155,59 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E3" s="4">
         <v>40</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1" spans="1:5">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C1:C2 C4:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C4 C5 C1:C2 C6:C1048576">
       <formula1>PageObjectModel!$I:$I</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2 D4 D5">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2150,73 +2222,118 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="15.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="33.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="23.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="21.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D2 D3:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+      <formula1>PageObjectModel!$J:$J</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D1:D2 D6:D1048576">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3 C1:C2 C4:C1048576">
-      <formula1>PageObjectModel!$J:$J</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2228,10 +2345,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2244,27 +2361,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -2275,44 +2392,44 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2320,13 +2437,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -2334,30 +2451,30 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
@@ -2365,13 +2482,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -2379,47 +2496,47 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -2427,30 +2544,30 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -2458,78 +2575,78 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -2540,92 +2657,92 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E20" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -2633,47 +2750,47 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E26" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -2684,64 +2801,64 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
         <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B31" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D31" t="s">
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -2749,30 +2866,61 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B34" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" t="s">
         <v>106</v>
+      </c>
+      <c r="D35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2780,13 +2928,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C20 C21 C22 C23 C27 C28 C29 C30 C31 C32 C33 C1:C2 C3:C4 C5:C6 C8:C15 C16:C19 C24:C26 C34:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2:A34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A35 A36 A2:A34">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2804,7 +2952,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -2817,27 +2965,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2848,16 +2996,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -2865,16 +3013,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -2882,16 +3030,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -2925,7 +3073,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -2938,36 +3086,36 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -2975,16 +3123,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -2992,16 +3140,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -3050,34 +3198,34 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3137,18 +3285,18 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3159,7 +3307,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3170,7 +3318,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3192,7 +3340,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -3203,7 +3351,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -3214,7 +3362,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3225,7 +3373,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -3271,41 +3419,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -3314,15 +3462,15 @@
         <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -3336,10 +3484,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -3385,27 +3533,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -3417,10 +3565,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -3431,27 +3579,27 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -3459,24 +3607,24 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -3520,198 +3668,198 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E7" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -3719,98 +3867,98 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -3818,13 +3966,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -3832,13 +3980,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -3846,13 +3994,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -3860,50 +4008,50 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3926,25 +4074,25 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="21.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="25.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
@@ -3955,21 +4103,35 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="D2" s="2">
         <v>12345678</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="2">
+        <v>12345678</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2 A3">
       <formula1>TestCaseID</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 C1:XFD1">
@@ -3978,6 +4140,7 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Jenny@meddataquest.com" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="C3" r:id="rId1" display="Jenny@meddataquest.com" tooltip="mailto:Jenny@meddataquest.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3990,12 +4153,12 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="19.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="28.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="17.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="20.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="26.2857142857143" customWidth="1"/>
@@ -4003,41 +4166,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -4046,15 +4209,15 @@
         <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -4068,10 +4231,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
update object model for enrollment flow
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
+    <workbookView windowWidth="27765" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="193">
   <si>
     <t>Page</t>
   </si>
@@ -195,210 +195,225 @@
     <t>CarePlanProblem</t>
   </si>
   <si>
+    <t>EnrollmentButton</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>blur</t>
+  </si>
+  <si>
+    <t>TestTask</t>
+  </si>
+  <si>
+    <t>Selections[3]</t>
+  </si>
+  <si>
+    <t>LastPageNumberButton</t>
+  </si>
+  <si>
     <t>PrimaryCareId</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>blur</t>
-  </si>
-  <si>
-    <t>TestTask</t>
-  </si>
-  <si>
-    <t>Selections[3]</t>
-  </si>
-  <si>
-    <t>LastPageNumberButton</t>
+    <t>HomePhoneNumber</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>AddIcon</t>
+  </si>
+  <si>
+    <t>LastMemberOfPage</t>
   </si>
   <si>
     <t>Gender</t>
   </si>
   <si>
-    <t>HomePhoneNumber</t>
-  </si>
-  <si>
-    <t>select</t>
-  </si>
-  <si>
-    <t>AddIcon</t>
-  </si>
-  <si>
-    <t>LastMemberOfPage</t>
+    <t>check</t>
+  </si>
+  <si>
+    <t>Dropdowns[1]</t>
   </si>
   <si>
     <t>ActiveOptions[1]</t>
   </si>
   <si>
-    <t>check</t>
-  </si>
-  <si>
-    <t>Dropdowns[1]</t>
+    <t>doubleClick</t>
+  </si>
+  <si>
+    <t>Dropdowns[2]</t>
   </si>
   <si>
     <t>ActiveOptions[2]</t>
   </si>
   <si>
-    <t>doubleClick</t>
-  </si>
-  <si>
-    <t>Dropdowns[2]</t>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>Dropdowns[3]</t>
   </si>
   <si>
     <t>ActiveOptions[3]</t>
   </si>
   <si>
-    <t>hover</t>
-  </si>
-  <si>
-    <t>Dropdowns[3]</t>
+    <t>waitForVisible</t>
   </si>
   <si>
     <t>BirthDate</t>
   </si>
   <si>
-    <t>waitForVisible</t>
+    <t>waitForClickable</t>
   </si>
   <si>
     <t>Organization</t>
   </si>
   <si>
-    <t>waitForClickable</t>
+    <t>waitForHidden</t>
   </si>
   <si>
     <t>Facility</t>
   </si>
   <si>
-    <t>waitForHidden</t>
+    <t>waitSpecificTime</t>
+  </si>
+  <si>
+    <t>SelectedOptions[1]</t>
   </si>
   <si>
     <t>City</t>
   </si>
   <si>
-    <t>waitSpecificTime</t>
-  </si>
-  <si>
-    <t>SelectedOptions[1]</t>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>SelectedOptions[2]</t>
   </si>
   <si>
     <t>CityInput</t>
   </si>
   <si>
-    <t>clear</t>
-  </si>
-  <si>
-    <t>SelectedOptions[2]</t>
+    <t>[value]</t>
+  </si>
+  <si>
+    <t>SelectedOptions[3]</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>[value]</t>
-  </si>
-  <si>
-    <t>SelectedOptions[3]</t>
+    <t>[text]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[1]</t>
   </si>
   <si>
-    <t>[text]</t>
+    <t>[class]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[2]</t>
   </si>
   <si>
-    <t>[class]</t>
+    <t>clickifenabled</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[3]</t>
   </si>
   <si>
-    <t>clickifenabled</t>
-  </si>
-  <si>
     <t>clickIfVisible</t>
   </si>
   <si>
+    <t>waitTextToBePresented</t>
+  </si>
+  <si>
     <t>HomePhoneNumberExt</t>
   </si>
   <si>
-    <t>waitTextToBePresented</t>
+    <t>waitForCheck</t>
   </si>
   <si>
     <t>CellNumber</t>
   </si>
   <si>
-    <t>waitForCheck</t>
+    <t>waitUtilSelected</t>
   </si>
   <si>
     <t>CellNumberExt</t>
   </si>
   <si>
-    <t>waitUtilSelected</t>
+    <t>clickAndHold</t>
   </si>
   <si>
     <t>HomePhoneNumberPerferred</t>
   </si>
   <si>
-    <t>clickAndHold</t>
+    <t>drogAndDropRichBox</t>
   </si>
   <si>
     <t>CellNumberPerferred</t>
   </si>
   <si>
-    <t>drogAndDropRichBox</t>
+    <t>selectPartialContextByIndex</t>
   </si>
   <si>
     <t>SubmitButton</t>
   </si>
   <si>
-    <t>selectPartialContextByIndex</t>
+    <t>sendKey</t>
   </si>
   <si>
     <t>ErrorMessage</t>
   </si>
   <si>
-    <t>sendKey</t>
+    <t>sendKeyByRobot</t>
   </si>
   <si>
     <t>ErrorMessage[1]</t>
   </si>
   <si>
-    <t>sendKeyByRobot</t>
+    <t>rightClick</t>
   </si>
   <si>
     <t>ErrorMessage[2]</t>
   </si>
   <si>
-    <t>rightClick</t>
-  </si>
-  <si>
     <t>[css](background-color)</t>
   </si>
   <si>
+    <t>[attr](style)</t>
+  </si>
+  <si>
     <t>ConsentValue</t>
   </si>
   <si>
-    <t>[attr](style)</t>
-  </si>
-  <si>
     <t>[css](border-bottom-color)</t>
   </si>
   <si>
+    <t>Consent</t>
+  </si>
+  <si>
     <t>takescreen</t>
   </si>
   <si>
+    <t>MemberStatus</t>
+  </si>
+  <si>
     <t>select_enrollment</t>
   </si>
   <si>
+    <t>EnrollmentDate</t>
+  </si>
+  <si>
     <t>select_care_plan</t>
   </si>
   <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t>select_chronic_log</t>
   </si>
   <si>
@@ -622,6 +637,9 @@
   </si>
   <si>
     <t>[regex](^[a-zA-Z0-9_.+-]+@[a-zA-Z0-9-]+\\.[a-zA-Z0-9-.]+$)</t>
+  </si>
+  <si>
+    <t>TS_03</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1272,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1268,6 +1286,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1589,10 +1608,10 @@
   <sheetPr/>
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1772,7 +1791,7 @@
       <c r="J4" t="s">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="9" t="s">
         <v>44</v>
       </c>
       <c r="L4" t="s">
@@ -1875,7 +1894,7 @@
         <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="K10" t="s">
         <v>67</v>
@@ -1886,7 +1905,7 @@
         <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K11" t="s">
         <v>69</v>
@@ -1897,7 +1916,7 @@
         <v>70</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K12" t="s">
         <v>71</v>
@@ -1957,15 +1976,15 @@
         <v>85</v>
       </c>
       <c r="K18" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K19" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -2037,65 +2056,80 @@
         <v>104</v>
       </c>
       <c r="K28" t="s">
-        <v>45</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
       <c r="B30" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="31" spans="2:2">
+      <c r="K30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
       <c r="B31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
+        <v>109</v>
+      </c>
+      <c r="K31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
       <c r="B32" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
+        <v>111</v>
+      </c>
+      <c r="K32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11">
       <c r="B33" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2">
+        <v>113</v>
+      </c>
+      <c r="K33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
       <c r="B34" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="K34" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2124,27 +2158,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -2155,16 +2189,16 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E3" s="4">
         <v>40</v>
@@ -2172,10 +2206,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>50</v>
@@ -2186,10 +2220,10 @@
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -2222,13 +2256,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="33.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="23.1428571428571" customWidth="1"/>
@@ -2237,83 +2271,83 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
@@ -2322,7 +2356,21 @@
         <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>172</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2333,7 +2381,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D1:D2 D6:D1048576">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2345,10 +2393,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2361,27 +2409,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -2392,44 +2440,44 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2437,13 +2485,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -2451,30 +2499,30 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
         <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
@@ -2482,13 +2530,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -2496,47 +2544,47 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
         <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
         <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -2544,30 +2592,30 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -2575,47 +2623,47 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
         <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C16" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
         <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
         <v>53</v>
@@ -2623,10 +2671,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
@@ -2635,18 +2683,18 @@
         <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -2657,64 +2705,64 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E20" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
         <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
         <v>75</v>
@@ -2722,13 +2770,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
         <v>53</v>
@@ -2736,13 +2784,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -2750,47 +2798,47 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E26" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C27" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D27" t="s">
         <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -2801,10 +2849,10 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
@@ -2813,32 +2861,32 @@
         <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B30" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D30" t="s">
         <v>81</v>
       </c>
       <c r="E30" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B31" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C31" t="s">
         <v>45</v>
@@ -2847,18 +2895,18 @@
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -2866,41 +2914,41 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B33" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
         <v>81</v>
@@ -2911,16 +2959,30 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" t="s">
+        <v>192</v>
+      </c>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2928,13 +2990,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C20 C21 C22 C23 C27 C28 C29 C30 C31 C32 C33 C1:C2 C3:C4 C5:C6 C8:C15 C16:C19 C24:C26 C34:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A35 A36 A2:A34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A35 A36 A37 A2:A34">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2965,27 +3027,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2996,16 +3058,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -3013,16 +3075,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -3030,16 +3092,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -3070,7 +3132,7 @@
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
@@ -3086,36 +3148,36 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -3123,16 +3185,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -3140,16 +3202,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -3198,34 +3260,34 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3285,18 +3347,18 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3307,7 +3369,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3318,7 +3380,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3340,7 +3402,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -3351,7 +3413,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -3362,7 +3424,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3373,7 +3435,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -3419,27 +3481,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -3450,10 +3512,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -3462,15 +3524,15 @@
         <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -3484,10 +3546,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -3533,27 +3595,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -3565,10 +3627,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -3579,10 +3641,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
@@ -3593,10 +3655,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
@@ -3607,10 +3669,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
@@ -3621,10 +3683,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -3668,27 +3730,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -3700,10 +3762,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -3712,15 +3774,15 @@
         <v>96</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -3729,15 +3791,15 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -3746,15 +3808,15 @@
         <v>98</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -3763,32 +3825,32 @@
         <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
@@ -3797,15 +3859,15 @@
         <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -3814,32 +3876,32 @@
         <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E10" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -3848,15 +3910,15 @@
         <v>98</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C12" t="s">
         <v>54</v>
@@ -3867,44 +3929,44 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -3913,15 +3975,15 @@
         <v>98</v>
       </c>
       <c r="E15" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B16" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -3930,32 +3992,32 @@
         <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E17" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
         <v>64</v>
@@ -3966,13 +4028,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B19" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -3980,10 +4042,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
         <v>58</v>
@@ -3994,13 +4056,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -4008,10 +4070,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
         <v>73</v>
@@ -4020,15 +4082,15 @@
         <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C23" t="s">
         <v>76</v>
@@ -4037,21 +4099,21 @@
         <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4089,10 +4151,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
@@ -4103,13 +4165,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D2" s="2">
         <v>12345678</v>
@@ -4117,13 +4179,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D3" s="2">
         <v>12345678</v>
@@ -4166,27 +4228,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
@@ -4197,10 +4259,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -4209,15 +4271,15 @@
         <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -4231,10 +4293,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
update ccm care plan testcase
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="7" activeTab="11"/>
+    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="7" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$N$2:$N$4</definedName>
-    <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$23</definedName>
+    <definedName name="ActionKeyWords">PageObjectModel!$B$2:$B$25</definedName>
     <definedName name="AdditionalOnePage">PageObjectModel!#REF!</definedName>
     <definedName name="AdditionalTwoPage">PageObjectModel!#REF!</definedName>
     <definedName name="Boolean">PageObjectModel!$M$2:$M$3</definedName>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="199">
   <si>
     <t>Page</t>
   </si>
@@ -216,6 +216,9 @@
     <t>LastPageNumberButton</t>
   </si>
   <si>
+    <t>CarePlanButton</t>
+  </si>
+  <si>
     <t>PrimaryCareId</t>
   </si>
   <si>
@@ -231,6 +234,9 @@
     <t>LastMemberOfPage</t>
   </si>
   <si>
+    <t>ProblemList</t>
+  </si>
+  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -318,102 +324,108 @@
     <t>AdvancedDirectivesOptions[2]</t>
   </si>
   <si>
+    <t>[visible]</t>
+  </si>
+  <si>
+    <t>AdvancedDirectivesOptions[3]</t>
+  </si>
+  <si>
+    <t>[size]</t>
+  </si>
+  <si>
     <t>clickifenabled</t>
   </si>
   <si>
-    <t>AdvancedDirectivesOptions[3]</t>
+    <t>HomePhoneNumberExt</t>
   </si>
   <si>
     <t>clickIfVisible</t>
   </si>
   <si>
+    <t>CellNumber</t>
+  </si>
+  <si>
     <t>waitTextToBePresented</t>
   </si>
   <si>
-    <t>HomePhoneNumberExt</t>
+    <t>CellNumberExt</t>
   </si>
   <si>
     <t>waitForCheck</t>
   </si>
   <si>
-    <t>CellNumber</t>
+    <t>HomePhoneNumberPerferred</t>
   </si>
   <si>
     <t>waitUtilSelected</t>
   </si>
   <si>
-    <t>CellNumberExt</t>
+    <t>CellNumberPerferred</t>
   </si>
   <si>
     <t>clickAndHold</t>
   </si>
   <si>
-    <t>HomePhoneNumberPerferred</t>
+    <t>SubmitButton</t>
   </si>
   <si>
     <t>drogAndDropRichBox</t>
   </si>
   <si>
-    <t>CellNumberPerferred</t>
+    <t>ErrorMessage</t>
   </si>
   <si>
     <t>selectPartialContextByIndex</t>
   </si>
   <si>
-    <t>SubmitButton</t>
+    <t>ErrorMessage[1]</t>
   </si>
   <si>
     <t>sendKey</t>
   </si>
   <si>
-    <t>ErrorMessage</t>
+    <t>ErrorMessage[2]</t>
   </si>
   <si>
     <t>sendKeyByRobot</t>
   </si>
   <si>
-    <t>ErrorMessage[1]</t>
-  </si>
-  <si>
     <t>rightClick</t>
   </si>
   <si>
-    <t>ErrorMessage[2]</t>
+    <t>ConsentValue</t>
   </si>
   <si>
     <t>[css](background-color)</t>
   </si>
   <si>
+    <t>Consent</t>
+  </si>
+  <si>
     <t>[attr](style)</t>
   </si>
   <si>
-    <t>ConsentValue</t>
+    <t>MemberStatus</t>
   </si>
   <si>
     <t>[css](border-bottom-color)</t>
   </si>
   <si>
-    <t>Consent</t>
+    <t>EnrollmentDate</t>
   </si>
   <si>
     <t>takescreen</t>
   </si>
   <si>
-    <t>MemberStatus</t>
+    <t>Note</t>
   </si>
   <si>
     <t>select_enrollment</t>
   </si>
   <si>
-    <t>EnrollmentDate</t>
-  </si>
-  <si>
     <t>select_care_plan</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>select_chronic_log</t>
   </si>
   <si>
@@ -595,6 +607,12 @@
   </si>
   <si>
     <t>No Data</t>
+  </si>
+  <si>
+    <t>TS_04</t>
+  </si>
+  <si>
+    <t>Create Care Plan</t>
   </si>
   <si>
     <t>hz 910</t>
@@ -1606,12 +1624,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1823,11 +1841,14 @@
       <c r="I5" t="s">
         <v>50</v>
       </c>
+      <c r="J5" t="s">
+        <v>51</v>
+      </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1835,16 +1856,19 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="J6" t="s">
+        <v>57</v>
       </c>
       <c r="K6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1852,13 +1876,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1866,13 +1890,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1880,188 +1904,188 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="K11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K14" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K17" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K18" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="K19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="K24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K25" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="K26" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="K27" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="K28" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="K29" t="s">
         <v>45</v>
@@ -2069,67 +2093,77 @@
     </row>
     <row r="30" spans="2:11">
       <c r="B30" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K30" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K31" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K32" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K33" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K34" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>121</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2145,7 +2179,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -2158,27 +2192,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -2189,16 +2223,16 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E3" s="4">
         <v>40</v>
@@ -2206,10 +2240,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>50</v>
@@ -2220,13 +2254,13 @@
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -2256,13 +2290,13 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="33.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="23.1428571428571" customWidth="1"/>
@@ -2271,117 +2305,154 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>133</v>
-      </c>
-      <c r="B6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
       <c r="D6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>87</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8 C1:C3 C4:C7 C9:C1048576">
       <formula1>PageObjectModel!$J:$J</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D1:D2 D6:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D8 D1:D2 D5:D7 D9:D1048576">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2 A3 A4 A5 A6 A7 A8 A9">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -2393,10 +2464,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2409,27 +2480,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -2440,44 +2511,44 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2485,13 +2556,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -2499,30 +2570,30 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
@@ -2530,13 +2601,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -2544,47 +2615,47 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
@@ -2592,30 +2663,30 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
         <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -2623,78 +2694,78 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E15" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E16" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -2705,92 +2776,92 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E20" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B24" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -2798,47 +2869,47 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D26" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E26" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -2849,10 +2920,10 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B29" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
         <v>45</v>
@@ -2861,32 +2932,32 @@
         <v>27</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D30" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B31" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
         <v>45</v>
@@ -2895,18 +2966,18 @@
         <v>27</v>
       </c>
       <c r="E31" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -2914,44 +2985,44 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D33" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C34" t="s">
         <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E35" t="s">
         <v>36</v>
@@ -2959,24 +3030,24 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C36" t="s">
         <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C37" t="s">
         <v>44</v>
@@ -2987,13 +3058,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B38" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -3001,13 +3072,13 @@
     </row>
     <row r="39" customFormat="1" spans="1:4">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B39" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C39" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D39" t="s">
         <v>15</v>
@@ -3015,44 +3086,58 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D41" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="42" customFormat="1" spans="1:4">
+      <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" t="s">
+        <v>198</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C20 C21 C22 C23 C27 C28 C29 C30 C31 C32 C33 C38 C39 C40 C1:C2 C3:C4 C5:C6 C8:C15 C16:C19 C24:C26 C34:C37 C41:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7 C20 C21 C22 C23 C27 C28 C29 C30 C31 C32 C33 C38 C39 C40 C41 C42 C1:C2 C3:C4 C5:C6 C8:C15 C16:C19 C24:C26 C34:C37 C43:C1048576">
       <formula1>PageObjectModel!$K:$K</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6 D7 D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25 D26 D27 D28 D29 D30 D31 D32 D33 D34 D35 D36 D37 D38 D39 D40 D41 D42">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A35 A36 A37 A38 A39 A40 A41 A2:A34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A35 A36 A37 A38 A39 A40 A41 A42 A2:A34">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -3070,7 +3155,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D9:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -3083,27 +3168,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -3114,16 +3199,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -3131,16 +3216,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -3148,16 +3233,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -3204,36 +3289,36 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -3241,16 +3326,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E3" t="s">
         <v>28</v>
@@ -3258,16 +3343,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -3316,34 +3401,34 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3403,18 +3488,18 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3425,7 +3510,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3436,7 +3521,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3458,7 +3543,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -3469,7 +3554,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -3480,7 +3565,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3491,7 +3576,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -3537,41 +3622,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -3580,15 +3665,15 @@
         <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -3602,10 +3687,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
@@ -3651,27 +3736,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -3683,10 +3768,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
@@ -3697,24 +3782,24 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
@@ -3725,24 +3810,24 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -3786,198 +3871,198 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E7" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E8" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -3985,98 +4070,98 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E13" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B14" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E14" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E15" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E16" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E17" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
         <v>15</v>
@@ -4084,13 +4169,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
         <v>15</v>
@@ -4098,13 +4183,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C20" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>
@@ -4112,13 +4197,13 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
         <v>15</v>
@@ -4126,50 +4211,50 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -4207,10 +4292,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>18</v>
@@ -4221,13 +4306,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D2" s="2">
         <v>12345678</v>
@@ -4235,13 +4320,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D3" s="2">
         <v>12345678</v>
@@ -4284,41 +4369,41 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
@@ -4327,15 +4412,15 @@
         <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -4349,10 +4434,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
update filepath for windows
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
+    <workbookView windowWidth="18165" windowHeight="7110" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -665,10 +665,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -703,7 +703,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -716,8 +716,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -732,10 +740,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -757,23 +773,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -784,14 +791,6 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -810,21 +809,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -851,12 +851,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -869,7 +863,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -881,157 +1025,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1047,6 +1047,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1054,20 +1065,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1087,32 +1110,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1128,141 +1125,144 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1271,22 +1271,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1629,7 +1629,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2292,8 +2292,8 @@
   <sheetPr/>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2466,8 +2466,8 @@
   <sheetPr/>
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -3155,7 +3155,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D9:D10"/>
+      <selection activeCell="C1" sqref="C$1:C$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -3273,10 +3273,10 @@
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -3315,7 +3315,7 @@
         <v>132</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>133</v>
@@ -3332,7 +3332,7 @@
         <v>135</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>136</v>
@@ -3349,7 +3349,7 @@
         <v>135</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>136</v>
@@ -3387,7 +3387,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -3478,7 +3478,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -3610,7 +3610,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -3859,8 +3859,8 @@
   <sheetPr/>
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -4281,14 +4281,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="25.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="12.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="19.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
@@ -4319,7 +4319,7 @@
         <v>12345678</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" ht="15" customHeight="1" spans="1:4">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -4357,7 +4357,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
update framework bug, component behavior has invoked twice.
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -666,9 +666,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -709,13 +709,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -731,7 +724,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -747,18 +739,18 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -778,9 +770,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -788,13 +787,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -808,9 +800,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -818,13 +825,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -851,13 +851,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,7 +881,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -887,25 +905,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -929,30 +929,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -965,13 +941,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -983,19 +971,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1013,25 +1019,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,13 +1078,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1114,21 +1118,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -1142,127 +1131,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1271,19 +1271,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2467,7 +2467,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A38" sqref="$A38:$XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -3276,7 +3276,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -3332,7 +3332,7 @@
         <v>135</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
update excel page model
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
+    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
     <sheet name="TestCases" sheetId="3" r:id="rId2"/>
     <sheet name="Config" sheetId="17" r:id="rId3"/>
     <sheet name="Flow" sheetId="19" r:id="rId4"/>
-    <sheet name="AnnotationLoginPage" sheetId="22" r:id="rId5"/>
-    <sheet name="AnnotationHomePage" sheetId="23" r:id="rId6"/>
-    <sheet name="AnnotationImplementPage" sheetId="24" r:id="rId7"/>
+    <sheet name="AnnotationLoginPage" sheetId="22" state="hidden" r:id="rId5"/>
+    <sheet name="AnnotationHomePage" sheetId="23" state="hidden" r:id="rId6"/>
+    <sheet name="AnnotationImplementPage" sheetId="24" state="hidden" r:id="rId7"/>
     <sheet name="Login" sheetId="29" r:id="rId8"/>
     <sheet name="CCMLoginPage" sheetId="25" r:id="rId9"/>
     <sheet name="CCMMemberPage" sheetId="26" r:id="rId10"/>
     <sheet name="CCMChronicPage" sheetId="27" r:id="rId11"/>
     <sheet name="CCMEnrollmentPage" sheetId="28" r:id="rId12"/>
     <sheet name="CCMChronicLogPage" sheetId="30" r:id="rId13"/>
+    <sheet name="CCMLoginPageModel" sheetId="31" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$N$2:$N$4</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="213">
   <si>
     <t>Page</t>
   </si>
@@ -108,6 +109,9 @@
     <t>YesNo</t>
   </si>
   <si>
+    <t>FindBy</t>
+  </si>
+  <si>
     <t>click</t>
   </si>
   <si>
@@ -144,6 +148,9 @@
     <t>YES</t>
   </si>
   <si>
+    <t>ById</t>
+  </si>
+  <si>
     <t>enter</t>
   </si>
   <si>
@@ -174,6 +181,9 @@
     <t>NO</t>
   </si>
   <si>
+    <t>ByCss</t>
+  </si>
+  <si>
     <t>focus</t>
   </si>
   <si>
@@ -204,6 +214,9 @@
     <t>N/A</t>
   </si>
   <si>
+    <t>ByXPath</t>
+  </si>
+  <si>
     <t>blur</t>
   </si>
   <si>
@@ -225,6 +238,9 @@
     <t>HomePhoneNumber</t>
   </si>
   <si>
+    <t>ByClassName</t>
+  </si>
+  <si>
     <t>select</t>
   </si>
   <si>
@@ -240,6 +256,9 @@
     <t>Gender</t>
   </si>
   <si>
+    <t>ByTag</t>
+  </si>
+  <si>
     <t>check</t>
   </si>
   <si>
@@ -249,6 +268,9 @@
     <t>ActiveOptions[1]</t>
   </si>
   <si>
+    <t>ByLinkText</t>
+  </si>
+  <si>
     <t>doubleClick</t>
   </si>
   <si>
@@ -258,6 +280,9 @@
     <t>ActiveOptions[2]</t>
   </si>
   <si>
+    <t>ByPartialLinkText</t>
+  </si>
+  <si>
     <t>hover</t>
   </si>
   <si>
@@ -267,6 +292,9 @@
     <t>ActiveOptions[3]</t>
   </si>
   <si>
+    <t>ByName</t>
+  </si>
+  <si>
     <t>waitForVisible</t>
   </si>
   <si>
@@ -369,189 +397,192 @@
     <t>SubmitButton</t>
   </si>
   <si>
+    <t>selectPartialContextByIndex</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>sendKey</t>
+  </si>
+  <si>
+    <t>ErrorMessage[1]</t>
+  </si>
+  <si>
+    <t>sendKeyByRobot</t>
+  </si>
+  <si>
+    <t>ErrorMessage[2]</t>
+  </si>
+  <si>
+    <t>rightClick</t>
+  </si>
+  <si>
+    <t>[css](background-color)</t>
+  </si>
+  <si>
+    <t>ConsentValue</t>
+  </si>
+  <si>
+    <t>[attr](style)</t>
+  </si>
+  <si>
+    <t>Consent</t>
+  </si>
+  <si>
+    <t>[css](border-bottom-color)</t>
+  </si>
+  <si>
+    <t>MemberStatus</t>
+  </si>
+  <si>
+    <t>takescreen</t>
+  </si>
+  <si>
+    <t>EnrollmentDate</t>
+  </si>
+  <si>
+    <t>select_enrollment</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>select_care_plan</t>
+  </si>
+  <si>
+    <t>select_chronic_log</t>
+  </si>
+  <si>
+    <t>select_ccm_if_visible</t>
+  </si>
+  <si>
+    <t>select_rpm_if_visible</t>
+  </si>
+  <si>
+    <t>select_first_date_of_next_month</t>
+  </si>
+  <si>
+    <t>[log_is_changed]</t>
+  </si>
+  <si>
+    <t>TestCase ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Site URL</t>
+  </si>
+  <si>
+    <t>Remote Hub</t>
+  </si>
+  <si>
+    <t>AnnotationTool</t>
+  </si>
+  <si>
+    <t>annotation tool</t>
+  </si>
+  <si>
+    <t>http://192.168.198.202/annotation-tool/#/user/login</t>
+  </si>
+  <si>
+    <t>ChronicCare_Demographics</t>
+  </si>
+  <si>
+    <t>chronic-care demo</t>
+  </si>
+  <si>
+    <t>http://192.168.198.202/chronic-care/#/login</t>
+  </si>
+  <si>
+    <t>ChronicCare_Enrollment</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>waitOrDelay</t>
+  </si>
+  <si>
+    <t>redirect</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>implict</t>
+  </si>
+  <si>
+    <t>explict</t>
+  </si>
+  <si>
+    <t>retry</t>
+  </si>
+  <si>
+    <t>sleepTime</t>
+  </si>
+  <si>
+    <t>FlowName</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>ExcelModel</t>
+  </si>
+  <si>
+    <t>AnnotationLogin</t>
+  </si>
+  <si>
+    <t>ChooseAnnotaion</t>
+  </si>
+  <si>
+    <t>ImplementAnnotation</t>
+  </si>
+  <si>
+    <t>CCMMemberList</t>
+  </si>
+  <si>
+    <t>CCMChronic</t>
+  </si>
+  <si>
+    <t>CCMEnrollment</t>
+  </si>
+  <si>
+    <t>CCMChronicLog</t>
+  </si>
+  <si>
+    <t>TestGroup ID</t>
+  </si>
+  <si>
+    <t>Target Name</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>TS_01</t>
+  </si>
+  <si>
+    <t>dong</t>
+  </si>
+  <si>
     <t>drogAndDropRichBox</t>
   </si>
   <si>
-    <t>ErrorMessage</t>
-  </si>
-  <si>
-    <t>selectPartialContextByIndex</t>
-  </si>
-  <si>
-    <t>ErrorMessage[1]</t>
-  </si>
-  <si>
-    <t>sendKey</t>
-  </si>
-  <si>
-    <t>ErrorMessage[2]</t>
-  </si>
-  <si>
-    <t>sendKeyByRobot</t>
-  </si>
-  <si>
-    <t>rightClick</t>
-  </si>
-  <si>
-    <t>ConsentValue</t>
-  </si>
-  <si>
-    <t>[css](background-color)</t>
-  </si>
-  <si>
-    <t>Consent</t>
-  </si>
-  <si>
-    <t>[attr](style)</t>
-  </si>
-  <si>
-    <t>MemberStatus</t>
-  </si>
-  <si>
-    <t>[css](border-bottom-color)</t>
-  </si>
-  <si>
-    <t>EnrollmentDate</t>
-  </si>
-  <si>
-    <t>takescreen</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>select_enrollment</t>
-  </si>
-  <si>
-    <t>select_care_plan</t>
-  </si>
-  <si>
-    <t>select_chronic_log</t>
-  </si>
-  <si>
-    <t>select_ccm_if_visible</t>
-  </si>
-  <si>
-    <t>select_rpm_if_visible</t>
-  </si>
-  <si>
-    <t>select_first_date_of_next_month</t>
-  </si>
-  <si>
-    <t>[log_is_changed]</t>
-  </si>
-  <si>
-    <t>TestCase ID</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Enabled</t>
-  </si>
-  <si>
-    <t>Site URL</t>
-  </si>
-  <si>
-    <t>Remote Hub</t>
-  </si>
-  <si>
-    <t>AnnotationTool</t>
-  </si>
-  <si>
-    <t>annotation tool</t>
-  </si>
-  <si>
-    <t>http://192.168.198.202/annotation-tool/#/user/login</t>
-  </si>
-  <si>
-    <t>ChronicCare_Demographics</t>
-  </si>
-  <si>
-    <t>chronic-care demo</t>
-  </si>
-  <si>
-    <t>http://192.168.198.202/chronic-care/#/login</t>
-  </si>
-  <si>
-    <t>ChronicCare_Enrollment</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>operation</t>
-  </si>
-  <si>
-    <t>waitOrDelay</t>
-  </si>
-  <si>
-    <t>redirect</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>implict</t>
-  </si>
-  <si>
-    <t>explict</t>
-  </si>
-  <si>
-    <t>retry</t>
-  </si>
-  <si>
-    <t>sleepTime</t>
-  </si>
-  <si>
-    <t>FlowName</t>
-  </si>
-  <si>
-    <t>Template</t>
-  </si>
-  <si>
-    <t>AnnotationLogin</t>
-  </si>
-  <si>
-    <t>ChooseAnnotaion</t>
-  </si>
-  <si>
-    <t>ImplementAnnotation</t>
-  </si>
-  <si>
-    <t>CCMMemberList</t>
-  </si>
-  <si>
-    <t>CCMChronic</t>
-  </si>
-  <si>
-    <t>CCMEnrollment</t>
-  </si>
-  <si>
-    <t>CCMChronicLog</t>
-  </si>
-  <si>
-    <t>TestGroup ID</t>
-  </si>
-  <si>
-    <t>Target Name</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>TS_01</t>
-  </si>
-  <si>
-    <t>dong</t>
-  </si>
-  <si>
     <t>10,10,800,300</t>
   </si>
   <si>
@@ -658,6 +689,18 @@
   </si>
   <si>
     <t>TS_03</t>
+  </si>
+  <si>
+    <t>FindBy Value</t>
+  </si>
+  <si>
+    <t>ShouldWait</t>
+  </si>
+  <si>
+    <t>ShouldDelay</t>
+  </si>
+  <si>
+    <t>ShouldBlur</t>
   </si>
 </sst>
 </file>
@@ -665,10 +708,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -709,11 +752,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -724,8 +766,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -733,6 +791,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -747,26 +821,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -786,17 +844,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -808,25 +865,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -851,7 +894,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,31 +954,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -899,25 +978,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,7 +996,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -947,43 +1020,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1001,30 +1038,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1032,6 +1045,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1063,6 +1106,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1074,6 +1132,26 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1093,30 +1171,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1131,108 +1185,97 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1241,28 +1284,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1271,19 +1314,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1624,12 +1667,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4:H8"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1638,11 +1681,13 @@
     <col min="2" max="2" width="13.1238095238095" customWidth="1"/>
     <col min="3" max="3" width="9.87619047619048" customWidth="1"/>
     <col min="4" max="4" width="13.8761904761905" customWidth="1"/>
-    <col min="5" max="12" width="20.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="10.1238095238095" customWidth="1"/>
+    <col min="5" max="7" width="20.8571428571429" hidden="1" customWidth="1"/>
+    <col min="8" max="12" width="20.8571428571429" customWidth="1"/>
+    <col min="13" max="13" width="14.5714285714286" customWidth="1"/>
+    <col min="14" max="14" width="16.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:15">
+    <row r="1" s="6" customFormat="1" spans="1:16">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1688,482 +1733,504 @@
       <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+        <v>38</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>49</v>
+      </c>
+      <c r="P4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>57</v>
+      </c>
+      <c r="P5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>63</v>
+      </c>
+      <c r="P6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="K7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>67</v>
+      </c>
+      <c r="P7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>71</v>
+      </c>
+      <c r="P8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="K9" t="s">
-        <v>67</v>
+        <v>75</v>
+      </c>
+      <c r="P9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="2:11">
       <c r="B10" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="2:11">
       <c r="B11" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="K11" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="2:11">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="K12" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="K13" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G14" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="K15" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="K16" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="2:11">
       <c r="B17" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="K17" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="K19" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="K20" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:11">
       <c r="B21" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="K21" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="2:11">
       <c r="B22" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="K22" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="K23" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:11">
       <c r="B24" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="K24" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="2:11">
       <c r="B25" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="K25" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="K26" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="K27" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="K28" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="2:11">
       <c r="B29" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="K29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="2:11">
       <c r="B30" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="K30" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="K31" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="K32" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="K33" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="K34" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2192,47 +2259,47 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="E3" s="4">
         <v>40</v>
@@ -2240,30 +2307,30 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4"/>
     </row>
@@ -2305,106 +2372,106 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2412,33 +2479,33 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E8" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -2480,295 +2547,295 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E11" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E15" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E19">
         <v>123</v>
@@ -2776,143 +2843,143 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D20" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C27" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D28" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E28">
         <v>1234567890</v>
@@ -2920,210 +2987,210 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E30" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C32" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D35" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="C37" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D38" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="1" spans="1:4">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="D40" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="C41" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" customFormat="1" spans="1:4">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3155,7 +3222,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -3168,47 +3235,47 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -3216,16 +3283,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -3233,16 +3300,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -3268,15 +3335,64 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.1428571428571" customWidth="1"/>
+    <col min="3" max="3" width="15.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="14.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="17.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="12.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
@@ -3289,73 +3405,73 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
       <c r="A1" s="6" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3387,7 +3503,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -3402,34 +3518,34 @@
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3458,7 +3574,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -3473,34 +3589,38 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="$A5:$XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:3">
+    <row r="1" s="6" customFormat="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>157</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3508,10 +3628,13 @@
       <c r="C2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3519,10 +3642,13 @@
       <c r="C3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3530,21 +3656,27 @@
       <c r="C4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -3552,10 +3684,13 @@
       <c r="C6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -3563,10 +3698,13 @@
       <c r="C7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3574,15 +3712,21 @@
       <c r="C8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3591,7 +3735,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
       <formula1>PageObjectModel!$A:$A</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 C5 C6 C7 C8 C3:C4 C9:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 D2 D3 D4 C5 D5 C6 D6 C7 D7 C8 D8 D9 C3:C4 C9:C1048576">
       <formula1>Boolean</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3:A1048576">
@@ -3623,64 +3767,64 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="2">
         <v>12345678</v>
@@ -3688,16 +3832,16 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3737,104 +3881,104 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3872,390 +4016,390 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="E15" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E16" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4281,7 +4425,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -4293,27 +4437,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D2" s="2">
         <v>12345678</v>
@@ -4321,13 +4465,13 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D3" s="2">
         <v>12345678</v>
@@ -4357,7 +4501,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
@@ -4370,64 +4514,64 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
       </c>
       <c r="E4" s="2">
         <v>12345678</v>
@@ -4435,16 +4579,16 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
get page clazz from excel
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="7" activeTab="13"/>
+    <workbookView windowWidth="27765" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="CCMEnrollmentPage" sheetId="28" r:id="rId12"/>
     <sheet name="CCMChronicLogPage" sheetId="30" r:id="rId13"/>
     <sheet name="CCMLoginPageModel" sheetId="31" r:id="rId14"/>
+    <sheet name="CCMChronicLogPageModel" sheetId="32" r:id="rId15"/>
+    <sheet name="CCMEnrollmentPageModel" sheetId="33" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$N$2:$N$4</definedName>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="277">
   <si>
     <t>Page</t>
   </si>
@@ -112,6 +114,9 @@
     <t>FindBy</t>
   </si>
   <si>
+    <t>Field Type</t>
+  </si>
+  <si>
     <t>click</t>
   </si>
   <si>
@@ -151,6 +156,9 @@
     <t>ById</t>
   </si>
   <si>
+    <t>Input</t>
+  </si>
+  <si>
     <t>enter</t>
   </si>
   <si>
@@ -184,6 +192,9 @@
     <t>ByCss</t>
   </si>
   <si>
+    <t>Button</t>
+  </si>
+  <si>
     <t>focus</t>
   </si>
   <si>
@@ -217,6 +228,9 @@
     <t>ByXPath</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>blur</t>
   </si>
   <si>
@@ -241,6 +255,9 @@
     <t>ByClassName</t>
   </si>
   <si>
+    <t>CheckBox</t>
+  </si>
+  <si>
     <t>select</t>
   </si>
   <si>
@@ -259,6 +276,9 @@
     <t>ByTag</t>
   </si>
   <si>
+    <t>Div</t>
+  </si>
+  <si>
     <t>check</t>
   </si>
   <si>
@@ -271,6 +291,9 @@
     <t>ByLinkText</t>
   </si>
   <si>
+    <t>DropDown</t>
+  </si>
+  <si>
     <t>doubleClick</t>
   </si>
   <si>
@@ -283,6 +306,9 @@
     <t>ByPartialLinkText</t>
   </si>
   <si>
+    <t>H</t>
+  </si>
+  <si>
     <t>hover</t>
   </si>
   <si>
@@ -295,24 +321,36 @@
     <t>ByName</t>
   </si>
   <si>
+    <t>Header</t>
+  </si>
+  <si>
     <t>waitForVisible</t>
   </si>
   <si>
     <t>BirthDate</t>
   </si>
   <si>
+    <t>Icon</t>
+  </si>
+  <si>
     <t>waitForClickable</t>
   </si>
   <si>
     <t>Organization</t>
   </si>
   <si>
+    <t>Image</t>
+  </si>
+  <si>
     <t>waitForHidden</t>
   </si>
   <si>
     <t>Facility</t>
   </si>
   <si>
+    <t>Lable</t>
+  </si>
+  <si>
     <t>waitSpecificTime</t>
   </si>
   <si>
@@ -322,6 +360,9 @@
     <t>City</t>
   </si>
   <si>
+    <t>Li</t>
+  </si>
+  <si>
     <t>clear</t>
   </si>
   <si>
@@ -331,6 +372,9 @@
     <t>CityInput</t>
   </si>
   <si>
+    <t>Link</t>
+  </si>
+  <si>
     <t>[value]</t>
   </si>
   <si>
@@ -340,69 +384,105 @@
     <t>State</t>
   </si>
   <si>
+    <t>Option</t>
+  </si>
+  <si>
     <t>[text]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[1]</t>
   </si>
   <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>[class]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[2]</t>
   </si>
   <si>
+    <t>RadioButton</t>
+  </si>
+  <si>
     <t>[visible]</t>
   </si>
   <si>
     <t>AdvancedDirectivesOptions[3]</t>
   </si>
   <si>
+    <t>Span</t>
+  </si>
+  <si>
     <t>[size]</t>
   </si>
   <si>
+    <t>Strong</t>
+  </si>
+  <si>
     <t>clickifenabled</t>
   </si>
   <si>
     <t>HomePhoneNumberExt</t>
   </si>
   <si>
+    <t>Textbox</t>
+  </si>
+  <si>
     <t>clickIfVisible</t>
   </si>
   <si>
     <t>CellNumber</t>
   </si>
   <si>
+    <t>Ul</t>
+  </si>
+  <si>
     <t>waitTextToBePresented</t>
   </si>
   <si>
     <t>CellNumberExt</t>
   </si>
   <si>
+    <t>List&lt;RadioButton&gt;</t>
+  </si>
+  <si>
     <t>waitForCheck</t>
   </si>
   <si>
     <t>HomePhoneNumberPerferred</t>
   </si>
   <si>
+    <t>List&lt;Div&gt;</t>
+  </si>
+  <si>
     <t>waitUtilSelected</t>
   </si>
   <si>
     <t>CellNumberPerferred</t>
   </si>
   <si>
+    <t>List&lt;Li&gt;</t>
+  </si>
+  <si>
     <t>clickAndHold</t>
   </si>
   <si>
     <t>SubmitButton</t>
   </si>
   <si>
+    <t>CCMDatePicker</t>
+  </si>
+  <si>
     <t>selectPartialContextByIndex</t>
   </si>
   <si>
     <t>ErrorMessage</t>
   </si>
   <si>
+    <t>CCMLogDiff</t>
+  </si>
+  <si>
     <t>sendKey</t>
   </si>
   <si>
@@ -418,6 +498,9 @@
     <t>rightClick</t>
   </si>
   <si>
+    <t>CCMMemberList</t>
+  </si>
+  <si>
     <t>[css](background-color)</t>
   </si>
   <si>
@@ -550,9 +633,6 @@
     <t>ImplementAnnotation</t>
   </si>
   <si>
-    <t>CCMMemberList</t>
-  </si>
-  <si>
     <t>CCMChronic</t>
   </si>
   <si>
@@ -701,6 +781,120 @@
   </si>
   <si>
     <t>ShouldBlur</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>GoNext</t>
+  </si>
+  <si>
+    <t>LogList</t>
+  </si>
+  <si>
+    <t>.//div[contains(@class,'chronicLog')]//table/tbody/tr</t>
+  </si>
+  <si>
+    <t>.//div[text()='Date of Birth']</t>
+  </si>
+  <si>
+    <t>.//div[text()='Email']</t>
+  </si>
+  <si>
+    <t>.//div[text()='Home Phone Number']</t>
+  </si>
+  <si>
+    <t>.//div[contains(@class,'ccmMember')]//ul[@role='menu']</t>
+  </si>
+  <si>
+    <t>.//div[@id='demographics']//button</t>
+  </si>
+  <si>
+    <t>.//div[@id='enrollment']//button</t>
+  </si>
+  <si>
+    <t>.//div[text()='Consent:']/parent::div//span</t>
+  </si>
+  <si>
+    <t>primary_care_id</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>ActiveOptions</t>
+  </si>
+  <si>
+    <t>.//div[contains(@class, 'ant-select-dropdown') and not(contains(@class,'ant-select-dropdown-hidden'))]//li</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>organization_id</t>
+  </si>
+  <si>
+    <t>facility_id</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>.//input[@id='city']</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>AdvancedDirectivesOptions</t>
+  </si>
+  <si>
+    <t>.//label[@title='Advanced Directives']/parent::div/parent::div//input</t>
+  </si>
+  <si>
+    <t>home_phone_number</t>
+  </si>
+  <si>
+    <t>home_phone_number_ext</t>
+  </si>
+  <si>
+    <t>cell_number</t>
+  </si>
+  <si>
+    <t>cell_number_ext</t>
+  </si>
+  <si>
+    <t>.//input[@value='home_phone_number']</t>
+  </si>
+  <si>
+    <t>.//input[@value='cell_number']</t>
+  </si>
+  <si>
+    <t>ant-form-explain</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>member_status</t>
+  </si>
+  <si>
+    <t>enrollment_date</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>ant-btn-primary</t>
   </si>
 </sst>
 </file>
@@ -873,7 +1067,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -883,6 +1077,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1079,12 +1291,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1188,85 +1415,85 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1275,7 +1502,7 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1287,25 +1514,25 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1314,34 +1541,38 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="41" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1667,12 +1898,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1687,550 +1918,637 @@
     <col min="14" max="14" width="16.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:16">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="10" customFormat="1" spans="1:17">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="D2" s="12" t="s">
+        <v>19</v>
+      </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>19</v>
-      </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" t="b">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="D3" s="12"/>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+        <v>41</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="M4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="O4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="P4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>53</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="P5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>62</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="K6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="P6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>69</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="K7" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="P7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>74</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="G8" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="K8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="P8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>79</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" t="s">
+        <v>83</v>
+      </c>
+      <c r="P9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" t="s">
         <v>73</v>
       </c>
-      <c r="G9" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" t="s">
-        <v>75</v>
-      </c>
-      <c r="P9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" t="s">
-        <v>67</v>
-      </c>
       <c r="K10" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" t="s">
-        <v>71</v>
-      </c>
       <c r="K11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11">
+        <v>90</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
       <c r="B12" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11">
+        <v>93</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
       <c r="B13" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="K13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11">
+        <v>97</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
       <c r="B14" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="K14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11">
+        <v>101</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
       <c r="B15" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="K15" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11">
+        <v>105</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
       <c r="B16" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="K16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11">
+        <v>108</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17">
       <c r="B17" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="K17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11">
+        <v>111</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17">
       <c r="B18" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="K18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11">
+        <v>114</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17">
       <c r="B19" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="K19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11">
+        <v>61</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17">
       <c r="B20" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="K20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11">
+        <v>119</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="K21" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11">
+        <v>122</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="K22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11">
+        <v>125</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="K23" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11">
+        <v>128</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
       <c r="B24" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="K24" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11">
+        <v>131</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="K25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11">
+        <v>134</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17">
       <c r="B26" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="K26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11">
+        <v>137</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17">
       <c r="B27" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="K27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11">
+        <v>140</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17">
       <c r="B28" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="K28" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11">
+        <v>142</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17">
       <c r="B29" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
       <c r="K29" t="s">
-        <v>48</v>
+        <v>51</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="2:11">
       <c r="B30" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="K30" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="2:11">
       <c r="B31" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="K31" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="2:11">
       <c r="B32" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="K32" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" t="s">
-        <v>124</v>
+        <v>151</v>
       </c>
       <c r="K33" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="K34" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="2:2">
       <c r="B38" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="2:2">
       <c r="B39" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="2:2">
       <c r="B40" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2259,80 +2577,80 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>189</v>
-      </c>
-      <c r="E3" s="4">
+        <v>215</v>
+      </c>
+      <c r="E3" s="8">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="E5" s="8"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -2372,106 +2690,106 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -2479,33 +2797,33 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>193</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B9" t="s">
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -2547,295 +2865,295 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>194</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>195</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D16" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>200</v>
+        <v>31</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E19">
         <v>123</v>
@@ -2843,143 +3161,143 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="E20" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>202</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>203</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B26" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C26" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>149</v>
       </c>
       <c r="E26" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B27" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
-        <v>204</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B28" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="D28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E28">
         <v>1234567890</v>
@@ -2987,210 +3305,210 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>205</v>
+        <v>31</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B30" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C31" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>207</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B33" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C33" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E35" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B36" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B37" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B38" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C38" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" customFormat="1" spans="1:4">
       <c r="A39" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B39" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B40" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="D41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" customFormat="1" spans="1:4">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B42" t="s">
-        <v>208</v>
+        <v>234</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3235,47 +3553,47 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -3283,16 +3601,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -3300,16 +3618,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -3338,43 +3656,671 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="13.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="15.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="14.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="17.1428571428571" customWidth="1"/>
-    <col min="6" max="6" width="12.5714285714286" customWidth="1"/>
+    <col min="1" max="2" width="13.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="15.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="14.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="17.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="12.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+      <formula1>PageObjectModel!$P:$P</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
+      <formula1>PageObjectModel!$Q:$Q</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="14.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="13.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="15.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="56.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>209</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>212</v>
+        <v>237</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+      <formula1>PageObjectModel!$P:$P</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
+      <formula1>PageObjectModel!$Q:$Q</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
+      <formula1>TestCaseID</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="28.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="19.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="11.2857142857143" customWidth="1"/>
+    <col min="4" max="4" width="55.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" s="2" customFormat="1" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" s="2" customFormat="1" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" s="2" customFormat="1" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" s="2" customFormat="1" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" s="2" customFormat="1" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" s="2" customFormat="1" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" s="2" customFormat="1" spans="1:7">
+      <c r="A16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G16" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" s="2" customFormat="1" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G17" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" s="2" customFormat="1" spans="1:7">
+      <c r="A18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G18" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" s="2" customFormat="1" spans="1:7">
+      <c r="A19" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G19" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" s="2" customFormat="1" spans="1:4">
+      <c r="A20" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
+      <c r="A21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" s="2" customFormat="1" spans="1:7">
+      <c r="A22" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="G22" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" s="2" customFormat="1" spans="1:4">
+      <c r="A23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" s="3" customFormat="1" spans="1:4">
+      <c r="A24" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" s="3" customFormat="1" spans="1:4">
+      <c r="A25" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" s="3" customFormat="1" spans="1:4">
+      <c r="A26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="27" s="3" customFormat="1" spans="1:4">
+      <c r="A27" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="28" s="4" customFormat="1" spans="1:4">
+      <c r="A28" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>276</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C1:C5 C6:C10 C29:C1048576">
+      <formula1>PageObjectModel!$P:$P</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B16 B17 B28 B1:B5 B6:B10 B12:B15 B18:B21 B22:B23 B24:B27 B29:B1048576">
+      <formula1>PageObjectModel!$Q:$Q</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
       <formula1>TestCaseID</formula1>
     </dataValidation>
@@ -3403,75 +4349,75 @@
     <col min="5" max="5" width="14.1238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:6">
-      <c r="A1" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="6" t="s">
+    <row r="1" s="10" customFormat="1" spans="1:6">
+      <c r="A1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>138</v>
+      <c r="F1" s="10" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>141</v>
+      <c r="D2" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>144</v>
+      <c r="D3" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>170</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>144</v>
+      <c r="D4" s="8" t="s">
+        <v>171</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -3500,10 +4446,10 @@
   <sheetPr/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -3516,36 +4462,36 @@
     <col min="6" max="6" width="8.24761904761905" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:10">
-      <c r="A1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>155</v>
+    <row r="1" s="10" customFormat="1" spans="1:10">
+      <c r="A1" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3556,7 +4502,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>30</v>
@@ -3574,7 +4520,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -3594,7 +4540,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="$A5:$XFD5"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -3604,23 +4550,23 @@
     <col min="4" max="4" width="12.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="6" customFormat="1" spans="1:4">
-      <c r="A1" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" s="10" customFormat="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>158</v>
+      <c r="C1" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -3634,7 +4580,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -3648,7 +4594,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3662,7 +4608,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -3676,7 +4622,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -3690,7 +4636,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -3704,7 +4650,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -3713,12 +4659,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -3727,7 +4673,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3767,81 +4713,81 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>171</v>
+        <v>31</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E4" s="6">
         <v>12345678</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3881,104 +4827,104 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -4016,390 +4962,390 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>173</v>
+        <v>198</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>139</v>
       </c>
-      <c r="B4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>113</v>
-      </c>
       <c r="E4" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>175</v>
+        <v>136</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="E6" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="E7" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B8" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>178</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="E9" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B10" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>181</v>
+        <v>136</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>182</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>115</v>
+        <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>183</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C18" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="D21" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>185</v>
+        <v>107</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>186</v>
+        <v>107</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="B24" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -4425,7 +5371,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -4437,43 +5383,43 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" s="2">
+        <v>196</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" s="6">
         <v>12345678</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="2">
+        <v>196</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="6">
         <v>12345678</v>
       </c>
     </row>
@@ -4514,81 +5460,81 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>188</v>
+        <v>31</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E4" s="6">
         <v>12345678</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add headless browser, update testcase
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" activeTab="2"/>
+    <workbookView windowWidth="27765" windowHeight="12510" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="279">
   <si>
     <t>Page</t>
   </si>
@@ -420,7 +420,7 @@
     <t>Strong</t>
   </si>
   <si>
-    <t>clickifenabled</t>
+    <t>clickIfEnabled</t>
   </si>
   <si>
     <t>HomePhoneNumberExt</t>
@@ -495,42 +495,45 @@
     <t>ErrorMessage[2]</t>
   </si>
   <si>
+    <t>clickByJS</t>
+  </si>
+  <si>
+    <t>CCMMemberList</t>
+  </si>
+  <si>
     <t>rightClick</t>
   </si>
   <si>
-    <t>CCMMemberList</t>
+    <t>ConsentValue</t>
   </si>
   <si>
     <t>[css](background-color)</t>
   </si>
   <si>
-    <t>ConsentValue</t>
+    <t>Consent</t>
   </si>
   <si>
     <t>[attr](style)</t>
   </si>
   <si>
-    <t>Consent</t>
+    <t>MemberStatus</t>
   </si>
   <si>
     <t>[css](border-bottom-color)</t>
   </si>
   <si>
-    <t>MemberStatus</t>
+    <t>EnrollmentDate</t>
   </si>
   <si>
     <t>takescreen</t>
   </si>
   <si>
-    <t>EnrollmentDate</t>
+    <t>Note</t>
   </si>
   <si>
     <t>select_enrollment</t>
   </si>
   <si>
-    <t>Note</t>
-  </si>
-  <si>
     <t>select_care_plan</t>
   </si>
   <si>
@@ -564,6 +567,9 @@
     <t>Remote Hub</t>
   </si>
   <si>
+    <t>Headless</t>
+  </si>
+  <si>
     <t>AnnotationTool</t>
   </si>
   <si>
@@ -828,73 +834,73 @@
     <t>gender</t>
   </si>
   <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>organization_id</t>
+  </si>
+  <si>
+    <t>facility_id</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>.//input[@id='city']</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>AdvancedDirectivesOptions</t>
+  </si>
+  <si>
+    <t>.//label[@title='Advanced Directives']/parent::div/parent::div//input</t>
+  </si>
+  <si>
+    <t>home_phone_number</t>
+  </si>
+  <si>
+    <t>home_phone_number_ext</t>
+  </si>
+  <si>
+    <t>cell_number</t>
+  </si>
+  <si>
+    <t>cell_number_ext</t>
+  </si>
+  <si>
+    <t>.//input[@value='home_phone_number']</t>
+  </si>
+  <si>
+    <t>.//input[@value='cell_number']</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>consent</t>
+  </si>
+  <si>
+    <t>member_status</t>
+  </si>
+  <si>
+    <t>enrollment_date</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>ant-btn-primary</t>
+  </si>
+  <si>
+    <t>ant-form-explain</t>
+  </si>
+  <si>
     <t>ActiveOptions</t>
   </si>
   <si>
     <t>.//div[contains(@class, 'ant-select-dropdown') and not(contains(@class,'ant-select-dropdown-hidden'))]//li</t>
-  </si>
-  <si>
-    <t>date_of_birth</t>
-  </si>
-  <si>
-    <t>organization_id</t>
-  </si>
-  <si>
-    <t>facility_id</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>.//input[@id='city']</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>AdvancedDirectivesOptions</t>
-  </si>
-  <si>
-    <t>.//label[@title='Advanced Directives']/parent::div/parent::div//input</t>
-  </si>
-  <si>
-    <t>home_phone_number</t>
-  </si>
-  <si>
-    <t>home_phone_number_ext</t>
-  </si>
-  <si>
-    <t>cell_number</t>
-  </si>
-  <si>
-    <t>cell_number_ext</t>
-  </si>
-  <si>
-    <t>.//input[@value='home_phone_number']</t>
-  </si>
-  <si>
-    <t>.//input[@value='cell_number']</t>
-  </si>
-  <si>
-    <t>ant-form-explain</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>consent</t>
-  </si>
-  <si>
-    <t>member_status</t>
-  </si>
-  <si>
-    <t>enrollment_date</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>ant-btn-primary</t>
   </si>
 </sst>
 </file>
@@ -903,9 +909,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -946,6 +952,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -960,31 +974,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1000,7 +992,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1008,7 +1000,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1023,7 +1030,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1037,8 +1044,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1051,19 +1066,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1106,7 +1112,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,25 +1208,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1148,145 +1286,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1333,51 +1339,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1398,6 +1363,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1412,97 +1403,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1511,28 +1517,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1541,19 +1547,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1565,7 +1571,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41" applyAlignment="1"/>
@@ -1898,12 +1904,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17"/>
+      <selection pane="bottomLeft" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2549,6 +2555,11 @@
     <row r="40" spans="2:2">
       <c r="B40" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2577,27 +2588,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -2608,16 +2619,16 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E3" s="8">
         <v>40</v>
@@ -2625,10 +2636,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>58</v>
@@ -2639,10 +2650,10 @@
     </row>
     <row r="5" ht="15" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
@@ -2678,7 +2689,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2690,69 +2701,69 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
@@ -2761,29 +2772,29 @@
         <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B6" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -2797,10 +2808,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
@@ -2809,15 +2820,15 @@
         <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C9" t="s">
         <v>67</v>
@@ -2852,7 +2863,7 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="$A38:$XFD38"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2865,27 +2876,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -2896,10 +2907,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -2908,29 +2919,29 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -2941,10 +2952,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>73</v>
@@ -2955,10 +2966,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
@@ -2967,15 +2978,15 @@
         <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
         <v>90</v>
@@ -2986,10 +2997,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
         <v>78</v>
@@ -3000,10 +3011,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
         <v>90</v>
@@ -3012,15 +3023,15 @@
         <v>107</v>
       </c>
       <c r="E10" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
         <v>93</v>
@@ -3029,15 +3040,15 @@
         <v>107</v>
       </c>
       <c r="E11" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
         <v>97</v>
@@ -3048,10 +3059,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
         <v>101</v>
@@ -3060,15 +3071,15 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
         <v>73</v>
@@ -3079,10 +3090,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
         <v>97</v>
@@ -3091,15 +3102,15 @@
         <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C16" t="s">
         <v>105</v>
@@ -3108,15 +3119,15 @@
         <v>107</v>
       </c>
       <c r="E16" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C17" t="s">
         <v>108</v>
@@ -3127,10 +3138,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C18" t="s">
         <v>61</v>
@@ -3139,15 +3150,15 @@
         <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C19" t="s">
         <v>119</v>
@@ -3161,27 +3172,27 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
         <v>119</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E20" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
         <v>140</v>
@@ -3190,15 +3201,15 @@
         <v>107</v>
       </c>
       <c r="E21" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C22" t="s">
         <v>119</v>
@@ -3207,15 +3218,15 @@
         <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C23" t="s">
         <v>122</v>
@@ -3226,10 +3237,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C24" t="s">
         <v>131</v>
@@ -3240,10 +3251,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C25" t="s">
         <v>134</v>
@@ -3254,27 +3265,27 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C26" t="s">
         <v>122</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E26" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C27" t="s">
         <v>140</v>
@@ -3283,15 +3294,15 @@
         <v>107</v>
       </c>
       <c r="E27" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C28" t="s">
         <v>122</v>
@@ -3305,10 +3316,10 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B29" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -3317,15 +3328,15 @@
         <v>31</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B30" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C30" t="s">
         <v>140</v>
@@ -3334,15 +3345,15 @@
         <v>107</v>
       </c>
       <c r="E30" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B31" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C31" t="s">
         <v>51</v>
@@ -3351,15 +3362,15 @@
         <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C32" t="s">
         <v>134</v>
@@ -3370,38 +3381,38 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C33" t="s">
         <v>134</v>
       </c>
       <c r="D33" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B35" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C35" t="s">
         <v>146</v>
@@ -3415,24 +3426,24 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B36" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
       </c>
       <c r="D36" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B37" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -3443,10 +3454,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C38" t="s">
         <v>148</v>
@@ -3457,10 +3468,10 @@
     </row>
     <row r="39" customFormat="1" spans="1:4">
       <c r="A39" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B39" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C39" t="s">
         <v>73</v>
@@ -3471,24 +3482,24 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B40" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C40" t="s">
         <v>152</v>
       </c>
       <c r="D40" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B41" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C41" t="s">
         <v>134</v>
@@ -3499,16 +3510,16 @@
     </row>
     <row r="42" customFormat="1" spans="1:4">
       <c r="A42" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B42" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
       </c>
       <c r="D42" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3553,27 +3564,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -3584,16 +3595,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -3601,16 +3612,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -3618,16 +3629,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E5" t="b">
         <v>1</v>
@@ -3659,7 +3670,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="$A6:$XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -3673,7 +3684,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -3682,16 +3693,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3705,7 +3716,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3719,7 +3730,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3733,12 +3744,12 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -3747,15 +3758,18 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E5 E6:E1048576 F1:F5 F6:F1048576 G1:G5 G6:G1048576">
+      <formula1>PageObjectModel!$M:$M</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C5 C6:C1048576">
       <formula1>PageObjectModel!$P:$P</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 B6:B1048576">
       <formula1>PageObjectModel!$Q:$Q</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
@@ -3773,7 +3787,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -3786,7 +3800,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -3795,21 +3809,21 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
         <v>129</v>
@@ -3818,7 +3832,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3832,7 +3846,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3846,10 +3860,10 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1" spans="1:4">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -3860,15 +3874,18 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E5 E6:E1048576 F1:F5 F6:F1048576 G1:G5 G6:G1048576">
+      <formula1>PageObjectModel!$M:$M</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C5 C6:C1048576">
       <formula1>PageObjectModel!$P:$P</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 B6:B1048576">
       <formula1>PageObjectModel!$Q:$Q</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
@@ -3885,21 +3902,23 @@
   <sheetPr/>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="28.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="19.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="11.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="18.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="55.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="10.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="12.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -3908,16 +3927,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3931,7 +3950,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3945,7 +3964,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3959,7 +3978,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3973,7 +3992,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -3987,7 +4006,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
@@ -4001,40 +4020,40 @@
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>254</v>
+        <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>135</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>70</v>
@@ -4043,12 +4062,12 @@
         <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>70</v>
@@ -4057,68 +4076,71 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>105</v>
+        <v>262</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" s="2" customFormat="1" spans="1:7">
+      <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="15" s="2" customFormat="1" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
+      </c>
+      <c r="G15" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>30</v>
@@ -4127,7 +4149,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -4135,7 +4157,7 @@
     </row>
     <row r="17" s="2" customFormat="1" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>30</v>
@@ -4144,7 +4166,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>1</v>
@@ -4152,7 +4174,7 @@
     </row>
     <row r="18" s="2" customFormat="1" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>30</v>
@@ -4161,32 +4183,29 @@
         <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" spans="1:7">
+    <row r="19" s="2" customFormat="1" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="G19" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" s="2" customFormat="1" spans="1:4">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>112</v>
@@ -4195,130 +4214,136 @@
         <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="21" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>112</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="22" s="2" customFormat="1" spans="1:7">
-      <c r="A22" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="G22" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" s="2" customFormat="1" spans="1:4">
-      <c r="A23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="2" t="s">
+    </row>
+    <row r="22" s="3" customFormat="1" spans="1:4">
+      <c r="A22" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="23" s="3" customFormat="1" spans="1:4">
+      <c r="A23" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="26" s="3" customFormat="1" spans="1:4">
-      <c r="A26" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="27" s="3" customFormat="1" spans="1:4">
-      <c r="A27" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="3" t="s">
+    <row r="26" s="4" customFormat="1" spans="1:6">
+      <c r="A26" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>275</v>
+      </c>
+      <c r="F26" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" s="4" customFormat="1" spans="1:7">
+      <c r="A27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G27" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="28" s="4" customFormat="1" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>134</v>
+        <v>277</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C1:C5 C6:C10 C29:C1048576">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E27 F27 G27 E28 F28 G28 E1:E7 E8:E20 E21:E26 E29:E1048576 F1:F7 F8:F20 F21:F26 F29:F1048576 G1:G7 G8:G20 G21:G26 G29:G1048576">
+      <formula1>PageObjectModel!$M:$M</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25 C26 C27 C28 C1:C5 C6:C7 C8:C9 C29:C1048576">
       <formula1>PageObjectModel!$P:$P</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11 B16 B17 B28 B1:B5 B6:B10 B12:B15 B18:B21 B22:B23 B24:B27 B29:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10 B15 B16 B21 B26 B27 B28 B1:B5 B6:B7 B8:B9 B11:B14 B17:B20 B22:B25 B29:B1048576">
       <formula1>PageObjectModel!$Q:$Q</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
@@ -4333,91 +4358,98 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="28.6285714285714" customWidth="1"/>
     <col min="2" max="2" width="38.752380952381" customWidth="1"/>
     <col min="4" max="4" width="49" customWidth="1"/>
     <col min="5" max="5" width="14.1238095238095" customWidth="1"/>
+    <col min="6" max="6" width="11.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="1" spans="1:6">
+    <row r="1" s="10" customFormat="1" spans="1:7">
       <c r="A1" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E3" t="s">
         <v>18</v>
       </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" t="s">
         <v>172</v>
-      </c>
-      <c r="B4" t="s">
-        <v>170</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4425,14 +4457,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 E2 E3:E1048576">
       <formula1>Browser</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2:C3 C4:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 G4 C2:C3 C4:C1048576 G2:G3">
       <formula1>Boolean</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="http://192.168.198.202/annotation-tool/#/user/login" tooltip="http://192.168.198.202/annotation-tool/#/user/login"/>
     <hyperlink ref="D3" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
-    <hyperlink ref="F3" r:id="rId3"/>
     <hyperlink ref="D4" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4446,10 +4477,10 @@
   <sheetPr/>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -4464,34 +4495,34 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:10">
       <c r="A1" s="10" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4520,7 +4551,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -4552,21 +4583,21 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:4">
       <c r="A1" s="10" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -4580,7 +4611,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -4594,7 +4625,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -4614,7 +4645,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -4636,7 +4667,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -4650,7 +4681,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -4664,7 +4695,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -4713,27 +4744,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -4744,10 +4775,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -4756,15 +4787,15 @@
         <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -4778,10 +4809,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -4827,27 +4858,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -4859,10 +4890,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -4873,10 +4904,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
@@ -4887,10 +4918,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -4901,10 +4932,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -4915,10 +4946,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -4962,27 +4993,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -4994,27 +5025,27 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -5023,15 +5054,15 @@
         <v>139</v>
       </c>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -5040,15 +5071,15 @@
         <v>136</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -5057,32 +5088,32 @@
         <v>141</v>
       </c>
       <c r="E6" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -5091,15 +5122,15 @@
         <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -5108,32 +5139,32 @@
         <v>141</v>
       </c>
       <c r="E9" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -5142,15 +5173,15 @@
         <v>136</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -5161,44 +5192,44 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -5207,15 +5238,15 @@
         <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -5224,32 +5255,32 @@
         <v>141</v>
       </c>
       <c r="E16" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C18" t="s">
         <v>82</v>
@@ -5260,10 +5291,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C19" t="s">
         <v>78</v>
@@ -5274,10 +5305,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C20" t="s">
         <v>72</v>
@@ -5288,10 +5319,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C21" t="s">
         <v>78</v>
@@ -5302,10 +5333,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C22" t="s">
         <v>96</v>
@@ -5314,15 +5345,15 @@
         <v>107</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B23" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C23" t="s">
         <v>100</v>
@@ -5331,21 +5362,21 @@
         <v>107</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -5383,10 +5414,10 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -5397,13 +5428,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D2" s="6">
         <v>12345678</v>
@@ -5411,13 +5442,13 @@
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D3" s="6">
         <v>12345678</v>
@@ -5460,27 +5491,27 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -5491,10 +5522,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -5503,15 +5534,15 @@
         <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -5525,10 +5556,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
update parallelMode for testSuites
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510"/>
+    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -2028,7 +2028,7 @@
   <sheetPr/>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
@@ -5094,10 +5094,10 @@
   <sheetPr/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -5140,7 +5140,7 @@
         <v>176</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>177</v>

</xml_diff>

<commit_message>
update parallel running code, refactor code
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27765" windowHeight="12510" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12510" firstSheet="16" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
     <sheet name="TestCases" sheetId="3" r:id="rId2"/>
     <sheet name="Config" sheetId="17" r:id="rId3"/>
     <sheet name="Flow" sheetId="19" r:id="rId4"/>
-    <sheet name="AnnotationLoginPage" sheetId="22" state="hidden" r:id="rId5"/>
-    <sheet name="AnnotationHomePage" sheetId="23" state="hidden" r:id="rId6"/>
+    <sheet name="AnnotationLoginPage" sheetId="22" r:id="rId5"/>
+    <sheet name="AnnotationHomePage" sheetId="23" r:id="rId6"/>
     <sheet name="AnnotationImplementPage" sheetId="24" r:id="rId7"/>
     <sheet name="Login" sheetId="29" r:id="rId8"/>
     <sheet name="CCMLoginPage" sheetId="25" state="hidden" r:id="rId9"/>
@@ -25,9 +25,9 @@
     <sheet name="CCMEnrollmentPageModel" sheetId="33" r:id="rId16"/>
     <sheet name="CCMChronicPageModel" sheetId="35" r:id="rId17"/>
     <sheet name="CCMMemberPageModel" sheetId="36" r:id="rId18"/>
-    <sheet name="AnnotationHomePageModel" sheetId="37" state="hidden" r:id="rId19"/>
-    <sheet name="AnnotationImplementPageModel" sheetId="38" state="hidden" r:id="rId20"/>
-    <sheet name="AnnotationLoginPageModel" sheetId="39" state="hidden" r:id="rId21"/>
+    <sheet name="AnnotationHomePageModel" sheetId="37" r:id="rId19"/>
+    <sheet name="AnnotationImplementPageModel" sheetId="38" r:id="rId20"/>
+    <sheet name="AnnotationLoginPageModel" sheetId="39" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$N$2:$N$4</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="316">
   <si>
     <t>Page</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t>sleepTime</t>
+  </si>
+  <si>
+    <t>parallel</t>
   </si>
   <si>
     <t>FlowName</t>
@@ -1021,10 +1024,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1059,21 +1062,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1087,16 +1091,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1110,6 +1113,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -1118,11 +1128,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1135,31 +1152,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1179,10 +1174,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1237,7 +1240,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1249,19 +1294,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1273,7 +1312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1285,25 +1324,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1315,49 +1384,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1369,13 +1402,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1387,31 +1414,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1443,8 +1446,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1454,21 +1457,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1488,17 +1476,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1520,15 +1502,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1537,97 +1510,127 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1639,25 +1642,25 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1669,19 +1672,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2744,16 +2747,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2761,7 +2764,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -2775,13 +2778,13 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E3" s="8">
         <v>41</v>
@@ -2792,7 +2795,7 @@
         <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>58</v>
@@ -2806,7 +2809,7 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
@@ -2821,7 +2824,7 @@
         <v>182</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -2835,13 +2838,13 @@
         <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E7" s="8">
         <v>40</v>
@@ -2889,16 +2892,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2906,7 +2909,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2920,7 +2923,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -2934,7 +2937,7 @@
         <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -2948,7 +2951,7 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
@@ -2957,7 +2960,7 @@
         <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2965,7 +2968,7 @@
         <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -2979,7 +2982,7 @@
         <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -2996,7 +2999,7 @@
         <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
@@ -3005,7 +3008,7 @@
         <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3013,7 +3016,7 @@
         <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C9" t="s">
         <v>67</v>
@@ -3030,7 +3033,7 @@
         <v>182</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -3044,7 +3047,7 @@
         <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
         <v>73</v>
@@ -3061,7 +3064,7 @@
         <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
         <v>85</v>
@@ -3070,7 +3073,7 @@
         <v>113</v>
       </c>
       <c r="E12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" ht="12" customHeight="1" spans="1:5">
@@ -3078,7 +3081,7 @@
         <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
         <v>73</v>
@@ -3095,7 +3098,7 @@
         <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
         <v>85</v>
@@ -3104,7 +3107,7 @@
         <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" ht="12" customHeight="1" spans="1:5">
@@ -3112,7 +3115,7 @@
         <v>182</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
         <v>73</v>
@@ -3129,7 +3132,7 @@
         <v>182</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
         <v>85</v>
@@ -3138,7 +3141,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3180,16 +3183,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3197,7 +3200,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -3211,7 +3214,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -3220,7 +3223,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3228,7 +3231,7 @@
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>90</v>
@@ -3242,7 +3245,7 @@
         <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -3256,7 +3259,7 @@
         <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>74</v>
@@ -3270,7 +3273,7 @@
         <v>178</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
@@ -3279,7 +3282,7 @@
         <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3287,7 +3290,7 @@
         <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
         <v>93</v>
@@ -3301,7 +3304,7 @@
         <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
         <v>80</v>
@@ -3315,7 +3318,7 @@
         <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
         <v>93</v>
@@ -3324,7 +3327,7 @@
         <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3332,7 +3335,7 @@
         <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
         <v>96</v>
@@ -3341,7 +3344,7 @@
         <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3349,7 +3352,7 @@
         <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
         <v>100</v>
@@ -3363,7 +3366,7 @@
         <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
         <v>104</v>
@@ -3372,7 +3375,7 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3380,7 +3383,7 @@
         <v>178</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
         <v>74</v>
@@ -3394,7 +3397,7 @@
         <v>178</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
         <v>100</v>
@@ -3403,7 +3406,7 @@
         <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3411,7 +3414,7 @@
         <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
         <v>108</v>
@@ -3420,7 +3423,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3428,7 +3431,7 @@
         <v>178</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
         <v>111</v>
@@ -3442,7 +3445,7 @@
         <v>178</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
         <v>61</v>
@@ -3451,7 +3454,7 @@
         <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3459,7 +3462,7 @@
         <v>178</v>
       </c>
       <c r="B19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C19" t="s">
         <v>122</v>
@@ -3476,7 +3479,7 @@
         <v>178</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C20" t="s">
         <v>122</v>
@@ -3485,7 +3488,7 @@
         <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3493,7 +3496,7 @@
         <v>178</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C21" t="s">
         <v>143</v>
@@ -3502,7 +3505,7 @@
         <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3510,7 +3513,7 @@
         <v>178</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C22" t="s">
         <v>122</v>
@@ -3519,7 +3522,7 @@
         <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3527,7 +3530,7 @@
         <v>178</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
         <v>125</v>
@@ -3541,7 +3544,7 @@
         <v>178</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s">
         <v>134</v>
@@ -3555,7 +3558,7 @@
         <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C25" t="s">
         <v>137</v>
@@ -3569,7 +3572,7 @@
         <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C26" t="s">
         <v>125</v>
@@ -3578,7 +3581,7 @@
         <v>158</v>
       </c>
       <c r="E26" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3586,7 +3589,7 @@
         <v>178</v>
       </c>
       <c r="B27" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C27" t="s">
         <v>143</v>
@@ -3595,7 +3598,7 @@
         <v>110</v>
       </c>
       <c r="E27" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3603,7 +3606,7 @@
         <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C28" t="s">
         <v>125</v>
@@ -3620,7 +3623,7 @@
         <v>178</v>
       </c>
       <c r="B29" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -3629,7 +3632,7 @@
         <v>31</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
@@ -3637,7 +3640,7 @@
         <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C30" t="s">
         <v>143</v>
@@ -3646,7 +3649,7 @@
         <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
@@ -3654,7 +3657,7 @@
         <v>178</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C31" t="s">
         <v>51</v>
@@ -3663,7 +3666,7 @@
         <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3671,7 +3674,7 @@
         <v>178</v>
       </c>
       <c r="B32" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C32" t="s">
         <v>137</v>
@@ -3685,13 +3688,13 @@
         <v>178</v>
       </c>
       <c r="B33" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C33" t="s">
         <v>137</v>
       </c>
       <c r="D33" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3699,7 +3702,7 @@
         <v>178</v>
       </c>
       <c r="B34" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
@@ -3713,7 +3716,7 @@
         <v>181</v>
       </c>
       <c r="B35" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C35" t="s">
         <v>150</v>
@@ -3730,7 +3733,7 @@
         <v>181</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
@@ -3744,7 +3747,7 @@
         <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -3758,7 +3761,7 @@
         <v>181</v>
       </c>
       <c r="B38" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C38" t="s">
         <v>152</v>
@@ -3772,7 +3775,7 @@
         <v>181</v>
       </c>
       <c r="B39" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C39" t="s">
         <v>74</v>
@@ -3786,7 +3789,7 @@
         <v>181</v>
       </c>
       <c r="B40" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C40" t="s">
         <v>157</v>
@@ -3800,7 +3803,7 @@
         <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C41" t="s">
         <v>137</v>
@@ -3814,7 +3817,7 @@
         <v>181</v>
       </c>
       <c r="B42" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -3868,16 +3871,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3885,7 +3888,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -3899,7 +3902,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -3916,7 +3919,7 @@
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
@@ -3933,7 +3936,7 @@
         <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
         <v>61</v>
@@ -3985,7 +3988,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -3994,16 +3997,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4017,7 +4020,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4031,7 +4034,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4045,12 +4048,12 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -4059,7 +4062,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -4101,7 +4104,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4110,21 +4113,21 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s">
         <v>132</v>
@@ -4133,7 +4136,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4147,7 +4150,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4161,7 +4164,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
@@ -4175,7 +4178,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -4219,7 +4222,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4228,16 +4231,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4251,7 +4254,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4265,7 +4268,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4279,7 +4282,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4293,7 +4296,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -4307,7 +4310,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
@@ -4321,7 +4324,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
@@ -4335,7 +4338,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
@@ -4349,7 +4352,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
@@ -4363,7 +4366,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
@@ -4377,7 +4380,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:4">
@@ -4391,7 +4394,7 @@
         <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="1:4">
@@ -4405,12 +4408,12 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>129</v>
@@ -4419,7 +4422,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" spans="1:7">
@@ -4433,7 +4436,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>1</v>
@@ -4450,7 +4453,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -4467,7 +4470,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>1</v>
@@ -4484,7 +4487,7 @@
         <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -4501,7 +4504,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
@@ -4515,7 +4518,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
@@ -4529,7 +4532,7 @@
         <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:4">
@@ -4543,7 +4546,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" spans="1:4">
@@ -4557,7 +4560,7 @@
         <v>29</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:4">
@@ -4571,7 +4574,7 @@
         <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:4">
@@ -4585,7 +4588,7 @@
         <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="26" s="4" customFormat="1" spans="1:6">
@@ -4599,7 +4602,7 @@
         <v>62</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F26" s="4" t="b">
         <v>1</v>
@@ -4616,7 +4619,7 @@
         <v>62</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -4624,7 +4627,7 @@
     </row>
     <row r="28" s="4" customFormat="1" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>135</v>
@@ -4633,7 +4636,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -4677,7 +4680,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4686,16 +4689,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4709,7 +4712,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -4726,7 +4729,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
@@ -4740,7 +4743,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:4">
@@ -4754,7 +4757,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -4768,7 +4771,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4782,7 +4785,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4796,7 +4799,7 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4810,7 +4813,7 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -4854,7 +4857,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4863,16 +4866,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4886,7 +4889,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4900,7 +4903,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4914,7 +4917,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4928,7 +4931,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4942,7 +4945,7 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -4986,7 +4989,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4995,16 +4998,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5018,7 +5021,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5032,7 +5035,7 @@
         <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5046,7 +5049,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -5063,7 +5066,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -5094,10 +5097,10 @@
   <sheetPr/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -5140,7 +5143,7 @@
         <v>176</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>177</v>
@@ -5169,7 +5172,7 @@
         <v>18</v>
       </c>
       <c r="G3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5251,7 +5254,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -5260,16 +5263,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5283,7 +5286,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -5291,7 +5294,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B3" t="s">
         <v>141</v>
@@ -5300,7 +5303,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5314,12 +5317,12 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B5" t="s">
         <v>132</v>
@@ -5328,12 +5331,12 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
         <v>135</v>
@@ -5342,12 +5345,12 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B7" t="s">
         <v>132</v>
@@ -5356,7 +5359,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -5384,8 +5387,8 @@
   <sheetPr/>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="6"/>
@@ -5400,7 +5403,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -5409,16 +5412,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5432,7 +5435,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5446,10 +5449,10 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1" spans="1:4">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -5460,18 +5463,18 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 F1 G1 E2:E1048576 F2:F1048576 G2:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1 F1 G1 E2:E4 E5:E7 E8:E1048576 F2:F4 F5:F7 F8:F1048576 G2:G4 G5:G7 G8:G1048576">
       <formula1>PageObjectModel!$M:$M</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2:C4 C5:C7 C8:C1048576">
       <formula1>PageObjectModel!$P:$P</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 B2:B4 B5:B7 B8:B1048576">
       <formula1>PageObjectModel!$Q:$Q</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
@@ -5486,12 +5489,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L$1:L$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -5502,9 +5505,10 @@
     <col min="4" max="4" width="10.1428571428571" customWidth="1"/>
     <col min="5" max="5" width="6.87619047619048" customWidth="1"/>
     <col min="6" max="6" width="8.24761904761905" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="1" spans="1:10">
+    <row r="1" s="10" customFormat="1" spans="1:11">
       <c r="A1" s="10" t="s">
         <v>184</v>
       </c>
@@ -5535,8 +5539,11 @@
       <c r="J1" s="10" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5566,6 +5573,9 @@
       </c>
       <c r="J2">
         <v>5</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5582,7 +5592,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -5594,21 +5604,21 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:4">
       <c r="A1" s="10" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -5622,7 +5632,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -5636,7 +5646,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -5678,7 +5688,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -5692,7 +5702,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -5706,7 +5716,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -5720,13 +5730,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B$1:B$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B9 B10:B1048576">
       <formula1>PageObjectModel!$A:$A</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 D2 D3 D4 C5 D5 C6 D6 C7 D7 C8 D8 D9 C3:C4 C9:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 D2 D3 D4 C5 D5 C6 D6 C7 D7 C8 D8 C9 D9 C3:C4 C10:C1048576">
       <formula1>Boolean</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3:A9 A10:A1048576">
       <formula1>Flow</formula1>
     </dataValidation>
   </dataValidations>
@@ -5758,16 +5768,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5775,7 +5785,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -5789,7 +5799,7 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -5798,7 +5808,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5806,7 +5816,7 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -5823,7 +5833,7 @@
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -5872,16 +5882,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5889,7 +5899,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -5904,7 +5914,7 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -5918,7 +5928,7 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
@@ -5932,7 +5942,7 @@
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -5946,7 +5956,7 @@
         <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -5960,7 +5970,7 @@
         <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -6007,16 +6017,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -6024,7 +6034,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -6039,7 +6049,7 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -6048,7 +6058,7 @@
         <v>145</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6056,7 +6066,7 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -6065,7 +6075,7 @@
         <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6073,7 +6083,7 @@
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -6082,7 +6092,7 @@
         <v>145</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -6090,7 +6100,7 @@
         <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -6099,7 +6109,7 @@
         <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -6107,7 +6117,7 @@
         <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -6116,7 +6126,7 @@
         <v>154</v>
       </c>
       <c r="E7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -6124,7 +6134,7 @@
         <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -6133,7 +6143,7 @@
         <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -6141,7 +6151,7 @@
         <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -6150,7 +6160,7 @@
         <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -6158,7 +6168,7 @@
         <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -6167,7 +6177,7 @@
         <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6175,7 +6185,7 @@
         <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -6184,7 +6194,7 @@
         <v>145</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6192,7 +6202,7 @@
         <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -6206,7 +6216,7 @@
         <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
@@ -6215,7 +6225,7 @@
         <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6223,7 +6233,7 @@
         <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
@@ -6232,7 +6242,7 @@
         <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6240,7 +6250,7 @@
         <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -6249,7 +6259,7 @@
         <v>145</v>
       </c>
       <c r="E15" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -6257,7 +6267,7 @@
         <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -6266,7 +6276,7 @@
         <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6274,7 +6284,7 @@
         <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
@@ -6283,7 +6293,7 @@
         <v>154</v>
       </c>
       <c r="E17" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -6291,7 +6301,7 @@
         <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
         <v>84</v>
@@ -6305,7 +6315,7 @@
         <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C19" t="s">
         <v>80</v>
@@ -6319,7 +6329,7 @@
         <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C20" t="s">
         <v>72</v>
@@ -6333,7 +6343,7 @@
         <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C21" t="s">
         <v>80</v>
@@ -6347,7 +6357,7 @@
         <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C22" t="s">
         <v>99</v>
@@ -6356,7 +6366,7 @@
         <v>110</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6364,7 +6374,7 @@
         <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
         <v>103</v>
@@ -6373,7 +6383,7 @@
         <v>110</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -6381,13 +6391,13 @@
         <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -6428,7 +6438,7 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -6442,10 +6452,10 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D2" s="6">
         <v>12345678</v>
@@ -6456,10 +6466,10 @@
         <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D3" s="6">
         <v>12345678</v>
@@ -6470,10 +6480,10 @@
         <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D4" s="6">
         <v>12345678</v>
@@ -6520,16 +6530,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6537,7 +6547,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -6551,7 +6561,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -6560,7 +6570,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6568,7 +6578,7 @@
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -6585,7 +6595,7 @@
         <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
update parallel running testcase
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12510" firstSheet="16" activeTab="20"/>
+    <workbookView windowWidth="28800" windowHeight="12510" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
     <sheet name="TestCases" sheetId="3" r:id="rId2"/>
     <sheet name="Config" sheetId="17" r:id="rId3"/>
     <sheet name="Flow" sheetId="19" r:id="rId4"/>
-    <sheet name="AnnotationLoginPage" sheetId="22" r:id="rId5"/>
-    <sheet name="AnnotationHomePage" sheetId="23" r:id="rId6"/>
-    <sheet name="AnnotationImplementPage" sheetId="24" r:id="rId7"/>
+    <sheet name="AnnotationLoginPage" sheetId="22" state="hidden" r:id="rId5"/>
+    <sheet name="AnnotationHomePage" sheetId="23" state="hidden" r:id="rId6"/>
+    <sheet name="AnnotationImplementPage" sheetId="24" state="hidden" r:id="rId7"/>
     <sheet name="Login" sheetId="29" r:id="rId8"/>
     <sheet name="CCMLoginPage" sheetId="25" state="hidden" r:id="rId9"/>
     <sheet name="CCMMemberPage" sheetId="26" r:id="rId10"/>
@@ -25,9 +25,9 @@
     <sheet name="CCMEnrollmentPageModel" sheetId="33" r:id="rId16"/>
     <sheet name="CCMChronicPageModel" sheetId="35" r:id="rId17"/>
     <sheet name="CCMMemberPageModel" sheetId="36" r:id="rId18"/>
-    <sheet name="AnnotationHomePageModel" sheetId="37" r:id="rId19"/>
-    <sheet name="AnnotationImplementPageModel" sheetId="38" r:id="rId20"/>
-    <sheet name="AnnotationLoginPageModel" sheetId="39" r:id="rId21"/>
+    <sheet name="AnnotationHomePageModel" sheetId="37" state="hidden" r:id="rId19"/>
+    <sheet name="AnnotationImplementPageModel" sheetId="38" state="hidden" r:id="rId20"/>
+    <sheet name="AnnotationLoginPageModel" sheetId="39" state="hidden" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="Acceptable">PageObjectModel!$N$2:$N$4</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="318">
   <si>
     <t>Page</t>
   </si>
@@ -746,7 +746,13 @@
     <t>takeScreen</t>
   </si>
   <si>
+    <t>selenium_ccm_2@shuruitech.com</t>
+  </si>
+  <si>
     <t>Jenny@meddataquest.com</t>
+  </si>
+  <si>
+    <t>selenium_ccm_1@shuruitech.com</t>
   </si>
   <si>
     <t>selectMemberByMID</t>
@@ -1024,10 +1030,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1068,11 +1074,102 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1092,98 +1189,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1246,36 +1252,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1294,7 +1270,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1306,7 +1312,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1318,13 +1360,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1336,55 +1408,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1396,25 +1420,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1445,9 +1451,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1455,8 +1463,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1479,33 +1487,7 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1540,97 +1522,121 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1639,28 +1645,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1669,22 +1675,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2731,7 +2737,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="4"/>
@@ -2784,10 +2790,10 @@
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E3" s="8">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2844,10 +2850,10 @@
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E7" s="8">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2863,8 +2869,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="41" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="E7" r:id="rId1" display="40" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="E3" r:id="rId1" display="51" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="E7" r:id="rId1" display="50" tooltip="mailto:Jenny@meddataquest.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2877,7 +2883,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A9" sqref="$A9:$XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2951,7 +2957,7 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
@@ -2960,7 +2966,7 @@
         <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2968,7 +2974,7 @@
         <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -2982,7 +2988,7 @@
         <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -2999,7 +3005,7 @@
         <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
@@ -3008,7 +3014,7 @@
         <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3016,7 +3022,7 @@
         <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C9" t="s">
         <v>67</v>
@@ -3073,7 +3079,7 @@
         <v>113</v>
       </c>
       <c r="E12" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" ht="12" customHeight="1" spans="1:5">
@@ -3107,7 +3113,7 @@
         <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" ht="12" customHeight="1" spans="1:5">
@@ -3141,7 +3147,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3229,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3282,7 +3288,7 @@
         <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3327,7 +3333,7 @@
         <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3344,7 +3350,7 @@
         <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3375,7 +3381,7 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3406,7 +3412,7 @@
         <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3423,7 +3429,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3454,7 +3460,7 @@
         <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3488,7 +3494,7 @@
         <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3505,7 +3511,7 @@
         <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3522,7 +3528,7 @@
         <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3581,7 +3587,7 @@
         <v>158</v>
       </c>
       <c r="E26" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3598,7 +3604,7 @@
         <v>110</v>
       </c>
       <c r="E27" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3632,7 +3638,7 @@
         <v>31</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
@@ -3649,7 +3655,7 @@
         <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
@@ -3666,7 +3672,7 @@
         <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3747,7 +3753,7 @@
         <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -3761,7 +3767,7 @@
         <v>181</v>
       </c>
       <c r="B38" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C38" t="s">
         <v>152</v>
@@ -3775,7 +3781,7 @@
         <v>181</v>
       </c>
       <c r="B39" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C39" t="s">
         <v>74</v>
@@ -3789,7 +3795,7 @@
         <v>181</v>
       </c>
       <c r="B40" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C40" t="s">
         <v>157</v>
@@ -3803,7 +3809,7 @@
         <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C41" t="s">
         <v>137</v>
@@ -3817,7 +3823,7 @@
         <v>181</v>
       </c>
       <c r="B42" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -3997,16 +4003,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4020,7 +4026,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4034,7 +4040,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4048,12 +4054,12 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -4062,7 +4068,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -4113,21 +4119,21 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B2" t="s">
         <v>132</v>
@@ -4136,7 +4142,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4150,7 +4156,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4164,7 +4170,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
@@ -4178,7 +4184,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -4231,16 +4237,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4254,7 +4260,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4268,7 +4274,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4282,7 +4288,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4296,7 +4302,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -4310,7 +4316,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
@@ -4324,7 +4330,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
@@ -4338,7 +4344,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
@@ -4352,7 +4358,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
@@ -4366,7 +4372,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
@@ -4380,7 +4386,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:4">
@@ -4394,7 +4400,7 @@
         <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="1:4">
@@ -4408,12 +4414,12 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>129</v>
@@ -4422,7 +4428,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" spans="1:7">
@@ -4436,7 +4442,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>1</v>
@@ -4453,7 +4459,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -4470,7 +4476,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>1</v>
@@ -4487,7 +4493,7 @@
         <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -4504,7 +4510,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
@@ -4518,7 +4524,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
@@ -4532,7 +4538,7 @@
         <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:4">
@@ -4546,7 +4552,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" spans="1:4">
@@ -4560,7 +4566,7 @@
         <v>29</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:4">
@@ -4574,7 +4580,7 @@
         <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:4">
@@ -4588,7 +4594,7 @@
         <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" s="4" customFormat="1" spans="1:6">
@@ -4602,7 +4608,7 @@
         <v>62</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="F26" s="4" t="b">
         <v>1</v>
@@ -4619,7 +4625,7 @@
         <v>62</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -4627,7 +4633,7 @@
     </row>
     <row r="28" s="4" customFormat="1" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>135</v>
@@ -4636,7 +4642,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -4665,7 +4671,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -4689,16 +4695,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4712,7 +4718,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -4729,7 +4735,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
@@ -4743,7 +4749,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:4">
@@ -4757,7 +4763,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -4771,7 +4777,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4785,7 +4791,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4799,7 +4805,7 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4813,7 +4819,7 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -4842,7 +4848,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="6"/>
@@ -4866,16 +4872,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4889,7 +4895,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4903,7 +4909,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4917,7 +4923,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4931,7 +4937,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4945,7 +4951,7 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -4998,16 +5004,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5021,7 +5027,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5035,7 +5041,7 @@
         <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5049,7 +5055,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -5066,7 +5072,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -5097,10 +5103,10 @@
   <sheetPr/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -5143,7 +5149,7 @@
         <v>176</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>177</v>
@@ -5200,7 +5206,7 @@
         <v>183</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>180</v>
@@ -5209,7 +5215,7 @@
         <v>18</v>
       </c>
       <c r="G5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -5223,8 +5229,8 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="http://192.168.198.202/annotation-tool/#/user/login" tooltip="http://192.168.198.202/annotation-tool/#/user/login"/>
+    <hyperlink ref="D4" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
     <hyperlink ref="D3" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
-    <hyperlink ref="D4" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
     <hyperlink ref="D5" r:id="rId2" display="http://192.168.198.202/chronic-care/#/login"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5263,16 +5269,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5286,7 +5292,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -5294,7 +5300,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B3" t="s">
         <v>141</v>
@@ -5303,7 +5309,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5317,12 +5323,12 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B5" t="s">
         <v>132</v>
@@ -5331,12 +5337,12 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B6" t="s">
         <v>135</v>
@@ -5345,12 +5351,12 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B7" t="s">
         <v>132</v>
@@ -5359,7 +5365,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -5387,7 +5393,7 @@
   <sheetPr/>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -5412,16 +5418,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5435,7 +5441,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5449,7 +5455,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:4">
@@ -5463,7 +5469,7 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -5494,7 +5500,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L$1:L$1048576"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -5569,7 +5575,7 @@
         <v>10</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -6423,7 +6429,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="3"/>
@@ -6469,7 +6475,7 @@
         <v>208</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D3" s="6">
         <v>12345678</v>
@@ -6482,8 +6488,8 @@
       <c r="B4" t="s">
         <v>208</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>225</v>
+      <c r="C4" s="8" t="s">
+        <v>227</v>
       </c>
       <c r="D4" s="6">
         <v>12345678</v>
@@ -6499,9 +6505,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Jenny@meddataquest.com" tooltip="mailto:Jenny@meddataquest.com"/>
     <hyperlink ref="C3" r:id="rId1" display="Jenny@meddataquest.com" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="C4" r:id="rId1" display="Jenny@meddataquest.com" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="C4" r:id="rId2" display="selenium_ccm_1@shuruitech.com" tooltip="mailto:selenium_ccm_1@shuruitech.com"/>
+    <hyperlink ref="C2" r:id="rId3" display="selenium_ccm_2@shuruitech.com" tooltip="mailto:selenium_ccm_2@shuruitech.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -6570,7 +6576,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>

<commit_message>
update logger, update parallel running code, other refactoring...
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="319">
   <si>
     <t>Page</t>
   </si>
@@ -654,6 +654,9 @@
   </si>
   <si>
     <t>parallel</t>
+  </si>
+  <si>
+    <t>threadCount</t>
   </si>
   <si>
     <t>FlowName</t>
@@ -2753,16 +2756,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2770,7 +2773,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -2784,13 +2787,13 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E3" s="8">
         <v>51</v>
@@ -2801,7 +2804,7 @@
         <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>58</v>
@@ -2815,7 +2818,7 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
@@ -2830,7 +2833,7 @@
         <v>182</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -2844,13 +2847,13 @@
         <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
         <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E7" s="8">
         <v>50</v>
@@ -2883,7 +2886,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="$A9:$XFD9"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2898,16 +2901,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2915,7 +2918,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2929,7 +2932,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -2943,7 +2946,7 @@
         <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -2957,7 +2960,7 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
@@ -2966,7 +2969,7 @@
         <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2974,7 +2977,7 @@
         <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -2988,7 +2991,7 @@
         <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -3005,7 +3008,7 @@
         <v>181</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C8" t="s">
         <v>59</v>
@@ -3014,7 +3017,7 @@
         <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3022,7 +3025,7 @@
         <v>181</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C9" t="s">
         <v>67</v>
@@ -3039,7 +3042,7 @@
         <v>182</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>24</v>
@@ -3053,7 +3056,7 @@
         <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
         <v>73</v>
@@ -3070,7 +3073,7 @@
         <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
         <v>85</v>
@@ -3079,7 +3082,7 @@
         <v>113</v>
       </c>
       <c r="E12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" ht="12" customHeight="1" spans="1:5">
@@ -3087,7 +3090,7 @@
         <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C13" t="s">
         <v>73</v>
@@ -3096,7 +3099,7 @@
         <v>161</v>
       </c>
       <c r="E13">
-        <v>5.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3104,7 +3107,7 @@
         <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
         <v>85</v>
@@ -3113,7 +3116,7 @@
         <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" ht="12" customHeight="1" spans="1:5">
@@ -3121,7 +3124,7 @@
         <v>182</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
         <v>73</v>
@@ -3130,7 +3133,7 @@
         <v>161</v>
       </c>
       <c r="E15">
-        <v>30.1</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3138,7 +3141,7 @@
         <v>182</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
         <v>85</v>
@@ -3147,7 +3150,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3173,12 +3176,12 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="32.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="31.1428571428571" customWidth="1"/>
     <col min="4" max="4" width="32.4285714285714" customWidth="1"/>
     <col min="5" max="5" width="58.7142857142857" customWidth="1"/>
@@ -3189,16 +3192,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3206,7 +3209,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -3220,7 +3223,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -3229,7 +3232,7 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3237,7 +3240,7 @@
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>90</v>
@@ -3251,7 +3254,7 @@
         <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -3265,7 +3268,7 @@
         <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>74</v>
@@ -3279,7 +3282,7 @@
         <v>178</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
@@ -3288,7 +3291,7 @@
         <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3296,7 +3299,7 @@
         <v>178</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C8" t="s">
         <v>93</v>
@@ -3310,7 +3313,7 @@
         <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
         <v>80</v>
@@ -3324,7 +3327,7 @@
         <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>93</v>
@@ -3333,7 +3336,7 @@
         <v>110</v>
       </c>
       <c r="E10" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3341,7 +3344,7 @@
         <v>178</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
         <v>96</v>
@@ -3350,7 +3353,7 @@
         <v>110</v>
       </c>
       <c r="E11" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3358,7 +3361,7 @@
         <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
         <v>100</v>
@@ -3372,7 +3375,7 @@
         <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C13" t="s">
         <v>104</v>
@@ -3381,7 +3384,7 @@
         <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3389,7 +3392,7 @@
         <v>178</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
         <v>74</v>
@@ -3403,7 +3406,7 @@
         <v>178</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
         <v>100</v>
@@ -3412,7 +3415,7 @@
         <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3420,7 +3423,7 @@
         <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
         <v>108</v>
@@ -3429,7 +3432,7 @@
         <v>110</v>
       </c>
       <c r="E16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3437,7 +3440,7 @@
         <v>178</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
         <v>111</v>
@@ -3451,7 +3454,7 @@
         <v>178</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s">
         <v>61</v>
@@ -3460,7 +3463,7 @@
         <v>31</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3468,7 +3471,7 @@
         <v>178</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
         <v>122</v>
@@ -3485,7 +3488,7 @@
         <v>178</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
         <v>122</v>
@@ -3494,7 +3497,7 @@
         <v>158</v>
       </c>
       <c r="E20" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3502,7 +3505,7 @@
         <v>178</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C21" t="s">
         <v>143</v>
@@ -3511,7 +3514,7 @@
         <v>110</v>
       </c>
       <c r="E21" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3519,7 +3522,7 @@
         <v>178</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
         <v>122</v>
@@ -3528,7 +3531,7 @@
         <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3536,7 +3539,7 @@
         <v>178</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C23" t="s">
         <v>125</v>
@@ -3550,7 +3553,7 @@
         <v>178</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C24" t="s">
         <v>134</v>
@@ -3564,7 +3567,7 @@
         <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C25" t="s">
         <v>137</v>
@@ -3578,7 +3581,7 @@
         <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C26" t="s">
         <v>125</v>
@@ -3587,7 +3590,7 @@
         <v>158</v>
       </c>
       <c r="E26" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3595,7 +3598,7 @@
         <v>178</v>
       </c>
       <c r="B27" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C27" t="s">
         <v>143</v>
@@ -3604,7 +3607,7 @@
         <v>110</v>
       </c>
       <c r="E27" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3612,7 +3615,7 @@
         <v>178</v>
       </c>
       <c r="B28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C28" t="s">
         <v>125</v>
@@ -3629,7 +3632,7 @@
         <v>178</v>
       </c>
       <c r="B29" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -3638,7 +3641,7 @@
         <v>31</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
@@ -3646,7 +3649,7 @@
         <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C30" t="s">
         <v>143</v>
@@ -3655,7 +3658,7 @@
         <v>110</v>
       </c>
       <c r="E30" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
@@ -3663,7 +3666,7 @@
         <v>178</v>
       </c>
       <c r="B31" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C31" t="s">
         <v>51</v>
@@ -3672,7 +3675,7 @@
         <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -3680,7 +3683,7 @@
         <v>178</v>
       </c>
       <c r="B32" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s">
         <v>137</v>
@@ -3694,13 +3697,13 @@
         <v>178</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C33" t="s">
         <v>137</v>
       </c>
       <c r="D33" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3708,7 +3711,7 @@
         <v>178</v>
       </c>
       <c r="B34" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C34" t="s">
         <v>25</v>
@@ -3722,7 +3725,7 @@
         <v>181</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C35" t="s">
         <v>150</v>
@@ -3739,7 +3742,7 @@
         <v>181</v>
       </c>
       <c r="B36" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C36" t="s">
         <v>25</v>
@@ -3753,7 +3756,7 @@
         <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -3767,7 +3770,7 @@
         <v>181</v>
       </c>
       <c r="B38" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C38" t="s">
         <v>152</v>
@@ -3781,7 +3784,7 @@
         <v>181</v>
       </c>
       <c r="B39" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C39" t="s">
         <v>74</v>
@@ -3795,7 +3798,7 @@
         <v>181</v>
       </c>
       <c r="B40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C40" t="s">
         <v>157</v>
@@ -3809,7 +3812,7 @@
         <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C41" t="s">
         <v>137</v>
@@ -3823,7 +3826,7 @@
         <v>181</v>
       </c>
       <c r="B42" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -3858,15 +3861,15 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="20.2857142857143" customWidth="1"/>
+    <col min="1" max="1" width="24.8571428571429" customWidth="1"/>
     <col min="2" max="2" width="13.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="30.2857142857143" customWidth="1"/>
     <col min="4" max="4" width="33.2857142857143" customWidth="1"/>
@@ -3877,16 +3880,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3894,7 +3897,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
@@ -3908,7 +3911,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
@@ -3925,7 +3928,7 @@
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>51</v>
@@ -3942,7 +3945,7 @@
         <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>61</v>
@@ -3954,18 +3957,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3 D4 D5 D6">
       <formula1>PageObjectModel!$B:$B</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C$1:C$1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6 C1:C5 C7:C1048576">
       <formula1>PageObjectModel!$L:$L</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 D2">
       <formula1>ActionKeyWords</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A2:A5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A6 A2:A5">
       <formula1>TestCaseID</formula1>
     </dataValidation>
   </dataValidations>
@@ -3994,7 +4014,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4003,16 +4023,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4026,7 +4046,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4040,7 +4060,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4054,12 +4074,12 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B5" t="s">
         <v>42</v>
@@ -4068,7 +4088,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -4110,7 +4130,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4119,21 +4139,21 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
         <v>132</v>
@@ -4142,7 +4162,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4156,7 +4176,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4170,7 +4190,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
@@ -4184,7 +4204,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -4228,7 +4248,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4237,16 +4257,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4260,7 +4280,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4274,7 +4294,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4288,7 +4308,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4302,7 +4322,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -4316,7 +4336,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
@@ -4330,7 +4350,7 @@
         <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
@@ -4344,7 +4364,7 @@
         <v>29</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
@@ -4358,7 +4378,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
@@ -4372,7 +4392,7 @@
         <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
@@ -4386,7 +4406,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:4">
@@ -4400,7 +4420,7 @@
         <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="1:4">
@@ -4414,12 +4434,12 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>129</v>
@@ -4428,7 +4448,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" spans="1:7">
@@ -4442,7 +4462,7 @@
         <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>1</v>
@@ -4459,7 +4479,7 @@
         <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -4476,7 +4496,7 @@
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>1</v>
@@ -4493,7 +4513,7 @@
         <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -4510,7 +4530,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
@@ -4524,7 +4544,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
@@ -4538,7 +4558,7 @@
         <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:4">
@@ -4552,7 +4572,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" spans="1:4">
@@ -4566,7 +4586,7 @@
         <v>29</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:4">
@@ -4580,7 +4600,7 @@
         <v>29</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:4">
@@ -4594,7 +4614,7 @@
         <v>29</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" s="4" customFormat="1" spans="1:6">
@@ -4608,7 +4628,7 @@
         <v>62</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F26" s="4" t="b">
         <v>1</v>
@@ -4625,7 +4645,7 @@
         <v>62</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -4633,7 +4653,7 @@
     </row>
     <row r="28" s="4" customFormat="1" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>135</v>
@@ -4642,7 +4662,7 @@
         <v>53</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -4686,7 +4706,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4695,16 +4715,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4718,7 +4738,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -4735,7 +4755,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
@@ -4749,7 +4769,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:4">
@@ -4763,7 +4783,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -4777,7 +4797,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -4791,7 +4811,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4805,7 +4825,7 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -4819,7 +4839,7 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -4863,7 +4883,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -4872,16 +4892,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4895,7 +4915,7 @@
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4909,7 +4929,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4923,7 +4943,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -4937,7 +4957,7 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -4951,7 +4971,7 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -4995,7 +5015,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -5004,16 +5024,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5027,7 +5047,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5041,7 +5061,7 @@
         <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5055,7 +5075,7 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -5072,7 +5092,7 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -5106,7 +5126,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -5149,7 +5169,7 @@
         <v>176</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>177</v>
@@ -5181,7 +5201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -5189,13 +5209,16 @@
         <v>179</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>180</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -5206,7 +5229,7 @@
         <v>183</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>180</v>
@@ -5260,7 +5283,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -5269,16 +5292,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5292,7 +5315,7 @@
         <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -5300,7 +5323,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B3" t="s">
         <v>141</v>
@@ -5309,7 +5332,7 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5323,12 +5346,12 @@
         <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B5" t="s">
         <v>132</v>
@@ -5337,12 +5360,12 @@
         <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B6" t="s">
         <v>135</v>
@@ -5351,12 +5374,12 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B7" t="s">
         <v>132</v>
@@ -5365,7 +5388,7 @@
         <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5409,7 +5432,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
@@ -5418,16 +5441,16 @@
         <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5441,7 +5464,7 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5455,7 +5478,7 @@
         <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:4">
@@ -5469,7 +5492,7 @@
         <v>69</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -5495,12 +5518,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -5514,7 +5537,7 @@
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="1" spans="1:11">
+    <row r="1" s="10" customFormat="1" spans="1:12">
       <c r="A1" s="10" t="s">
         <v>184</v>
       </c>
@@ -5548,8 +5571,11 @@
       <c r="K1" s="10" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5582,6 +5608,9 @@
       </c>
       <c r="K2" t="b">
         <v>1</v>
+      </c>
+      <c r="L2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5610,21 +5639,21 @@
   <sheetData>
     <row r="1" s="10" customFormat="1" spans="1:4">
       <c r="A1" s="10" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -5638,7 +5667,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -5652,7 +5681,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -5694,7 +5723,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -5708,7 +5737,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -5722,7 +5751,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -5774,16 +5803,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5791,7 +5820,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -5805,7 +5834,7 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -5814,7 +5843,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5822,7 +5851,7 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -5839,7 +5868,7 @@
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -5888,16 +5917,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5905,7 +5934,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -5920,7 +5949,7 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -5934,7 +5963,7 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
@@ -5948,7 +5977,7 @@
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -5962,7 +5991,7 @@
         <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
@@ -5976,7 +6005,7 @@
         <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
@@ -6023,16 +6052,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -6040,7 +6069,7 @@
         <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -6055,7 +6084,7 @@
         <v>175</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -6064,7 +6093,7 @@
         <v>145</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6072,7 +6101,7 @@
         <v>175</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -6081,7 +6110,7 @@
         <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -6089,7 +6118,7 @@
         <v>175</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
@@ -6098,7 +6127,7 @@
         <v>145</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -6106,7 +6135,7 @@
         <v>175</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -6115,7 +6144,7 @@
         <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -6123,7 +6152,7 @@
         <v>175</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -6132,7 +6161,7 @@
         <v>154</v>
       </c>
       <c r="E7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -6140,7 +6169,7 @@
         <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -6149,7 +6178,7 @@
         <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -6157,7 +6186,7 @@
         <v>175</v>
       </c>
       <c r="B9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -6166,7 +6195,7 @@
         <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -6174,7 +6203,7 @@
         <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -6183,7 +6212,7 @@
         <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -6191,7 +6220,7 @@
         <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -6200,7 +6229,7 @@
         <v>145</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6208,7 +6237,7 @@
         <v>175</v>
       </c>
       <c r="B12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -6222,7 +6251,7 @@
         <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C13" t="s">
         <v>47</v>
@@ -6231,7 +6260,7 @@
         <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6239,7 +6268,7 @@
         <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
@@ -6248,7 +6277,7 @@
         <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6256,7 +6285,7 @@
         <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
@@ -6265,7 +6294,7 @@
         <v>145</v>
       </c>
       <c r="E15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -6273,7 +6302,7 @@
         <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
         <v>22</v>
@@ -6282,7 +6311,7 @@
         <v>148</v>
       </c>
       <c r="E16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6290,7 +6319,7 @@
         <v>175</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
         <v>47</v>
@@ -6299,7 +6328,7 @@
         <v>154</v>
       </c>
       <c r="E17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -6307,7 +6336,7 @@
         <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C18" t="s">
         <v>84</v>
@@ -6321,7 +6350,7 @@
         <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C19" t="s">
         <v>80</v>
@@ -6335,7 +6364,7 @@
         <v>175</v>
       </c>
       <c r="B20" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C20" t="s">
         <v>72</v>
@@ -6349,7 +6378,7 @@
         <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C21" t="s">
         <v>80</v>
@@ -6363,7 +6392,7 @@
         <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C22" t="s">
         <v>99</v>
@@ -6372,7 +6401,7 @@
         <v>110</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -6380,7 +6409,7 @@
         <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C23" t="s">
         <v>103</v>
@@ -6389,7 +6418,7 @@
         <v>110</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -6397,13 +6426,13 @@
         <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C24" t="s">
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -6444,7 +6473,7 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -6458,10 +6487,10 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="D2" s="6">
         <v>12345678</v>
@@ -6472,10 +6501,10 @@
         <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D3" s="6">
         <v>12345678</v>
@@ -6486,10 +6515,10 @@
         <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D4" s="6">
         <v>12345678</v>
@@ -6536,16 +6565,16 @@
         <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6553,7 +6582,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -6567,7 +6596,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -6576,7 +6605,7 @@
         <v>31</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6584,7 +6613,7 @@
         <v>178</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -6601,7 +6630,7 @@
         <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
reafactoring sleep or wait code
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="8310" firstSheet="1" activeTab="12"/>
+    <workbookView windowWidth="28800" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="345">
   <si>
     <t>Page</t>
   </si>
@@ -643,6 +643,9 @@
     <t>Headless</t>
   </si>
   <si>
+    <t>Priority</t>
+  </si>
+  <si>
     <t>AnnotationTool</t>
   </si>
   <si>
@@ -685,21 +688,12 @@
     <t>default</t>
   </si>
   <si>
-    <t>operation</t>
-  </si>
-  <si>
     <t>waitOrDelay</t>
   </si>
   <si>
     <t>redirect</t>
   </si>
   <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
     <t>implict</t>
   </si>
   <si>
@@ -707,9 +701,6 @@
   </si>
   <si>
     <t>retry</t>
-  </si>
-  <si>
-    <t>sleepTime</t>
   </si>
   <si>
     <t>parallel</t>
@@ -1122,10 +1113,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1160,7 +1151,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1168,13 +1159,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1188,6 +1172,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -1196,25 +1202,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1229,61 +1263,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1344,13 +1335,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1362,19 +1371,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1386,19 +1383,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1410,13 +1395,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1434,13 +1419,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1458,61 +1503,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1550,8 +1541,56 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1586,39 +1625,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1629,112 +1635,97 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1743,28 +1734,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1773,22 +1764,22 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2138,7 +2129,7 @@
   <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
     </sheetView>
@@ -2924,24 +2915,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" hidden="1" spans="1:4">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2952,16 +2943,16 @@
     </row>
     <row r="3" ht="15" hidden="1" customHeight="1" spans="1:5">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E3" s="7">
         <v>51</v>
@@ -2969,10 +2960,10 @@
     </row>
     <row r="4" hidden="1" spans="1:4">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
@@ -2983,10 +2974,10 @@
     </row>
     <row r="5" ht="15" hidden="1" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>70</v>
@@ -2998,10 +2989,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>84</v>
@@ -3012,16 +3003,16 @@
     </row>
     <row r="7" ht="15" customHeight="1" spans="1:5">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E7" s="7">
         <v>89</v>
@@ -3029,10 +3020,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>84</v>
@@ -3043,12 +3034,11 @@
     </row>
     <row r="9" ht="15" customHeight="1" spans="1:5">
       <c r="A9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
-      </c>
-      <c r="C9"/>
+        <v>225</v>
+      </c>
       <c r="D9" t="s">
         <v>170</v>
       </c>
@@ -3058,16 +3048,16 @@
     </row>
     <row r="10" ht="15" customHeight="1" spans="1:5">
       <c r="A10" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E10" s="7">
         <v>89</v>
@@ -3075,10 +3065,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
         <v>84</v>
@@ -3089,16 +3079,16 @@
     </row>
     <row r="12" ht="15" customHeight="1" spans="1:5">
       <c r="A12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E12" s="7">
         <v>90</v>
@@ -3106,10 +3096,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C13" t="s">
         <v>84</v>
@@ -3120,16 +3110,16 @@
     </row>
     <row r="14" ht="15" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E14" s="7">
         <v>90</v>
@@ -3137,10 +3127,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>84</v>
@@ -3151,16 +3141,16 @@
     </row>
     <row r="16" ht="15" customHeight="1" spans="1:5">
       <c r="A16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E16" s="7">
         <v>91</v>
@@ -3168,10 +3158,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s">
         <v>84</v>
@@ -3182,16 +3172,16 @@
     </row>
     <row r="18" ht="15" customHeight="1" spans="1:5">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B18" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E18" s="7">
         <v>91</v>
@@ -3229,7 +3219,7 @@
   <sheetPr/>
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
@@ -3245,24 +3235,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" ht="17" hidden="1" customHeight="1" spans="1:4">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -3273,10 +3263,10 @@
     </row>
     <row r="3" ht="24" hidden="1" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -3287,10 +3277,10 @@
     </row>
     <row r="4" ht="17" hidden="1" customHeight="1" spans="1:4">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -3301,10 +3291,10 @@
     </row>
     <row r="5" ht="21" hidden="1" customHeight="1" spans="1:5">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
@@ -3313,15 +3303,15 @@
         <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" ht="23" hidden="1" customHeight="1" spans="1:4">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -3332,10 +3322,10 @@
     </row>
     <row r="7" ht="20" hidden="1" customHeight="1" spans="1:5">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C7" t="s">
         <v>63</v>
@@ -3349,10 +3339,10 @@
     </row>
     <row r="8" ht="24" hidden="1" customHeight="1" spans="1:5">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C8" t="s">
         <v>63</v>
@@ -3361,15 +3351,15 @@
         <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" ht="18" hidden="1" customHeight="1" spans="1:5">
       <c r="A9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s">
         <v>71</v>
@@ -3383,10 +3373,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -3397,10 +3387,10 @@
     </row>
     <row r="11" ht="12" customHeight="1" spans="1:5">
       <c r="A11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D11" t="s">
         <v>170</v>
@@ -3411,10 +3401,10 @@
     </row>
     <row r="12" ht="12" customHeight="1" spans="1:5">
       <c r="A12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>91</v>
@@ -3423,15 +3413,15 @@
         <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>96</v>
@@ -3440,15 +3430,15 @@
         <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" ht="12" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D14" t="s">
         <v>170</v>
@@ -3459,10 +3449,10 @@
     </row>
     <row r="15" ht="12" customHeight="1" spans="1:5">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>91</v>
@@ -3471,15 +3461,15 @@
         <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>96</v>
@@ -3488,15 +3478,15 @@
         <v>117</v>
       </c>
       <c r="E16" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" ht="12" customHeight="1" spans="1:5">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D17" t="s">
         <v>170</v>
@@ -3507,10 +3497,10 @@
     </row>
     <row r="18" ht="12" customHeight="1" spans="1:5">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -3519,15 +3509,15 @@
         <v>117</v>
       </c>
       <c r="E18" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
         <v>96</v>
@@ -3536,15 +3526,15 @@
         <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D20" t="s">
         <v>170</v>
@@ -3555,10 +3545,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D21" t="s">
         <v>169</v>
@@ -3566,10 +3556,10 @@
     </row>
     <row r="22" ht="12" customHeight="1" spans="1:5">
       <c r="A22" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
@@ -3578,15 +3568,15 @@
         <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
         <v>96</v>
@@ -3595,15 +3585,15 @@
         <v>117</v>
       </c>
       <c r="E23" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="1:4">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B24" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D24" t="s">
         <v>168</v>
@@ -3611,10 +3601,10 @@
     </row>
     <row r="25" s="6" customFormat="1" ht="12" customHeight="1" spans="1:4">
       <c r="A25" s="6" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>85</v>
@@ -3625,10 +3615,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B26" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C26" t="s">
         <v>96</v>
@@ -3637,15 +3627,15 @@
         <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B27" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D27" t="s">
         <v>170</v>
@@ -3656,10 +3646,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D28" t="s">
         <v>169</v>
@@ -3667,10 +3657,10 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
         <v>96</v>
@@ -3679,15 +3669,15 @@
         <v>117</v>
       </c>
       <c r="E29" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D30" t="s">
         <v>170</v>
@@ -3698,10 +3688,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D31" t="s">
         <v>169</v>
@@ -3709,10 +3699,10 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C32" t="s">
         <v>96</v>
@@ -3721,15 +3711,15 @@
         <v>117</v>
       </c>
       <c r="E32" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D33" t="s">
         <v>170</v>
@@ -3740,10 +3730,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D34" t="s">
         <v>169</v>
@@ -3751,10 +3741,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C35" t="s">
         <v>96</v>
@@ -3768,10 +3758,10 @@
     </row>
     <row r="36" customFormat="1" spans="1:4">
       <c r="A36" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B36" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D36" t="s">
         <v>168</v>
@@ -3779,10 +3769,10 @@
     </row>
     <row r="37" s="6" customFormat="1" spans="1:4">
       <c r="A37" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>55</v>
@@ -3793,10 +3783,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -3807,10 +3797,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D39" t="s">
         <v>170</v>
@@ -3821,10 +3811,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B40" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C40" t="s">
         <v>85</v>
@@ -3835,10 +3825,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B41" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C41" t="s">
         <v>26</v>
@@ -3849,10 +3839,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B42" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -3863,10 +3853,10 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B43" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D43" t="s">
         <v>170</v>
@@ -3877,10 +3867,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B44" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C44" t="s">
         <v>85</v>
@@ -3891,10 +3881,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B45" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
@@ -3942,24 +3932,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3970,10 +3960,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -3982,15 +3972,15 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>97</v>
@@ -4001,10 +3991,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>72</v>
@@ -4015,10 +4005,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>79</v>
@@ -4029,10 +4019,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>72</v>
@@ -4041,15 +4031,15 @@
         <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>100</v>
@@ -4060,10 +4050,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
         <v>86</v>
@@ -4074,10 +4064,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>100</v>
@@ -4086,15 +4076,15 @@
         <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
         <v>103</v>
@@ -4103,15 +4093,15 @@
         <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>107</v>
@@ -4122,10 +4112,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>111</v>
@@ -4134,15 +4124,15 @@
         <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
         <v>79</v>
@@ -4153,10 +4143,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>107</v>
@@ -4165,15 +4155,15 @@
         <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>115</v>
@@ -4182,15 +4172,15 @@
         <v>117</v>
       </c>
       <c r="E16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
         <v>118</v>
@@ -4201,10 +4191,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
         <v>65</v>
@@ -4213,15 +4203,15 @@
         <v>33</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
         <v>129</v>
@@ -4235,10 +4225,10 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B20" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C20" t="s">
         <v>129</v>
@@ -4247,15 +4237,15 @@
         <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
         <v>150</v>
@@ -4264,15 +4254,15 @@
         <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
         <v>129</v>
@@ -4281,15 +4271,15 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
         <v>132</v>
@@ -4300,10 +4290,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C24" t="s">
         <v>141</v>
@@ -4314,10 +4304,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C25" t="s">
         <v>144</v>
@@ -4328,10 +4318,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C26" t="s">
         <v>132</v>
@@ -4340,15 +4330,15 @@
         <v>165</v>
       </c>
       <c r="E26" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C27" t="s">
         <v>150</v>
@@ -4357,15 +4347,15 @@
         <v>117</v>
       </c>
       <c r="E27" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C28" t="s">
         <v>132</v>
@@ -4379,10 +4369,10 @@
     </row>
     <row r="29" ht="12" customHeight="1" spans="1:5">
       <c r="A29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
         <v>54</v>
@@ -4391,15 +4381,15 @@
         <v>33</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
       <c r="A30" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C30" t="s">
         <v>150</v>
@@ -4408,15 +4398,15 @@
         <v>117</v>
       </c>
       <c r="E30" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
       <c r="A31" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C31" t="s">
         <v>54</v>
@@ -4425,15 +4415,15 @@
         <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C32" t="s">
         <v>144</v>
@@ -4444,24 +4434,24 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C33" t="s">
         <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
@@ -4472,10 +4462,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B35" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C35" t="s">
         <v>157</v>
@@ -4489,10 +4479,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B36" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C36" t="s">
         <v>26</v>
@@ -4503,10 +4493,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B37" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C37" t="s">
         <v>53</v>
@@ -4517,10 +4507,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B38" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C38" t="s">
         <v>159</v>
@@ -4531,10 +4521,10 @@
     </row>
     <row r="39" customFormat="1" spans="1:4">
       <c r="A39" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B39" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C39" t="s">
         <v>79</v>
@@ -4545,10 +4535,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C40" t="s">
         <v>164</v>
@@ -4559,10 +4549,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B41" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C41" t="s">
         <v>144</v>
@@ -4573,10 +4563,10 @@
     </row>
     <row r="42" customFormat="1" spans="1:4">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B42" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C42" t="s">
         <v>26</v>
@@ -4613,7 +4603,7 @@
   <sheetPr/>
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -4630,24 +4620,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -4656,15 +4646,15 @@
         <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -4673,15 +4663,15 @@
         <v>183</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D4" t="s">
         <v>168</v>
@@ -4690,10 +4680,10 @@
     </row>
     <row r="5" s="6" customFormat="1" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>55</v>
@@ -4705,10 +4695,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -4717,15 +4707,15 @@
         <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -4734,15 +4724,15 @@
         <v>183</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D8" t="s">
         <v>168</v>
@@ -4750,10 +4740,10 @@
     </row>
     <row r="9" s="6" customFormat="1" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>55</v>
@@ -4809,24 +4799,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -4837,10 +4827,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -4854,10 +4844,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -4871,10 +4861,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
@@ -4888,10 +4878,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
         <v>168</v>
@@ -4940,7 +4930,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -4949,16 +4939,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4972,7 +4962,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4986,7 +4976,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5000,12 +4990,12 @@
         <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
@@ -5014,7 +5004,7 @@
         <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5058,7 +5048,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5067,16 +5057,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5090,7 +5080,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5104,7 +5094,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5118,7 +5108,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5132,7 +5122,7 @@
         <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5146,7 +5136,7 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5160,7 +5150,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -5204,7 +5194,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5213,16 +5203,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5236,7 +5226,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5250,7 +5240,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5264,7 +5254,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5278,7 +5268,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -5292,7 +5282,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
@@ -5306,7 +5296,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
@@ -5320,7 +5310,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
@@ -5334,7 +5324,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
@@ -5348,7 +5338,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
@@ -5362,7 +5352,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:4">
@@ -5376,7 +5366,7 @@
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="1:4">
@@ -5390,12 +5380,12 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>136</v>
@@ -5404,7 +5394,7 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" spans="1:7">
@@ -5418,7 +5408,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>1</v>
@@ -5435,7 +5425,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -5452,7 +5442,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>1</v>
@@ -5469,7 +5459,7 @@
         <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -5486,7 +5476,7 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
@@ -5500,7 +5490,7 @@
         <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
@@ -5514,7 +5504,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:4">
@@ -5528,7 +5518,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" spans="1:4">
@@ -5542,7 +5532,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:4">
@@ -5556,7 +5546,7 @@
         <v>31</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:4">
@@ -5570,7 +5560,7 @@
         <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" s="4" customFormat="1" spans="1:6">
@@ -5584,7 +5574,7 @@
         <v>66</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="F26" s="4" t="b">
         <v>1</v>
@@ -5601,7 +5591,7 @@
         <v>66</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -5609,7 +5599,7 @@
     </row>
     <row r="28" s="4" customFormat="1" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>142</v>
@@ -5618,7 +5608,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:4">
@@ -5632,7 +5622,7 @@
         <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5679,7 +5669,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5688,16 +5678,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5711,7 +5701,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -5728,7 +5718,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
@@ -5742,7 +5732,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:4">
@@ -5756,7 +5746,7 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -5770,7 +5760,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5784,7 +5774,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5798,12 +5788,12 @@
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B9" t="s">
         <v>145</v>
@@ -5812,7 +5802,7 @@
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5826,7 +5816,7 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5870,7 +5860,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5879,16 +5869,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5902,7 +5892,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:4">
@@ -5916,7 +5906,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5945,15 +5935,15 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="45.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="38.752380952381" customWidth="1"/>
@@ -5962,7 +5952,7 @@
     <col min="6" max="6" width="11.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" spans="1:7">
+    <row r="1" s="12" customFormat="1" spans="1:8">
       <c r="A1" s="12" t="s">
         <v>184</v>
       </c>
@@ -5984,19 +5974,22 @@
       <c r="G1" s="12" t="s">
         <v>189</v>
       </c>
+      <c r="H1" s="12" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -6007,16 +6000,16 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -6027,16 +6020,16 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -6045,18 +6038,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -6064,19 +6057,22 @@
       <c r="G5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -6084,19 +6080,22 @@
       <c r="G6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -6104,25 +6103,31 @@
       <c r="G7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E8" t="s">
         <v>19</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6168,7 +6173,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6177,21 +6182,21 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B2" t="s">
         <v>139</v>
@@ -6200,7 +6205,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6214,7 +6219,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6228,7 +6233,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
@@ -6242,7 +6247,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:4">
@@ -6256,7 +6261,7 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -6303,7 +6308,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6312,16 +6317,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6335,7 +6340,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6349,7 +6354,7 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6363,7 +6368,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -6380,7 +6385,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -6427,7 +6432,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6436,16 +6441,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6459,7 +6464,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -6467,7 +6472,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B3" t="s">
         <v>148</v>
@@ -6476,7 +6481,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6490,12 +6495,12 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B5" t="s">
         <v>139</v>
@@ -6504,12 +6509,12 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B6" t="s">
         <v>142</v>
@@ -6518,12 +6523,12 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B7" t="s">
         <v>139</v>
@@ -6532,7 +6537,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -6576,7 +6581,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6585,16 +6590,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6608,7 +6613,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6622,7 +6627,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:4">
@@ -6636,7 +6641,7 @@
         <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -6662,102 +6667,79 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="9.37142857142857" customWidth="1"/>
-    <col min="2" max="2" width="9.5047619047619" customWidth="1"/>
-    <col min="3" max="3" width="11.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="10.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="6.87619047619048" customWidth="1"/>
-    <col min="6" max="6" width="8.24761904761905" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="2" max="2" width="11.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="10.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="1" spans="1:12">
+    <row r="1" s="12" customFormat="1" spans="1:8">
       <c r="A1" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="I1" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-      <c r="E2">
-        <v>60</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
       <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>Boolean</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
@@ -6783,21 +6765,21 @@
   <sheetData>
     <row r="1" s="12" customFormat="1" spans="1:4">
       <c r="A1" s="12" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -6811,7 +6793,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -6825,7 +6807,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -6867,7 +6849,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -6881,7 +6863,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -6895,7 +6877,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -6947,24 +6929,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -6975,10 +6957,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -6987,15 +6969,15 @@
         <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -7009,10 +6991,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
@@ -7061,24 +7043,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -7090,10 +7072,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
@@ -7104,10 +7086,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
@@ -7118,10 +7100,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>60</v>
@@ -7132,10 +7114,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
@@ -7146,10 +7128,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -7196,24 +7178,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -7225,10 +7207,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -7237,15 +7219,15 @@
         <v>152</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -7254,15 +7236,15 @@
         <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -7271,15 +7253,15 @@
         <v>152</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -7288,15 +7270,15 @@
         <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -7305,15 +7287,15 @@
         <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -7322,15 +7304,15 @@
         <v>152</v>
       </c>
       <c r="E8" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -7339,15 +7321,15 @@
         <v>155</v>
       </c>
       <c r="E9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>
@@ -7356,15 +7338,15 @@
         <v>161</v>
       </c>
       <c r="E10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -7373,15 +7355,15 @@
         <v>152</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>69</v>
@@ -7392,10 +7374,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -7404,15 +7386,15 @@
         <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
         <v>61</v>
@@ -7421,15 +7403,15 @@
         <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -7438,15 +7420,15 @@
         <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -7455,15 +7437,15 @@
         <v>155</v>
       </c>
       <c r="E16" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
         <v>50</v>
@@ -7472,15 +7454,15 @@
         <v>161</v>
       </c>
       <c r="E17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
@@ -7491,10 +7473,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
         <v>86</v>
@@ -7505,10 +7487,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C20" t="s">
         <v>76</v>
@@ -7519,10 +7501,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
         <v>86</v>
@@ -7533,10 +7515,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B22" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
         <v>106</v>
@@ -7545,15 +7527,15 @@
         <v>117</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B23" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
         <v>110</v>
@@ -7562,18 +7544,18 @@
         <v>117</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B24" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D24" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -7615,7 +7597,7 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
@@ -7626,13 +7608,13 @@
     </row>
     <row r="2" hidden="1" spans="1:4">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D2" s="9">
         <v>12345678</v>
@@ -7640,13 +7622,13 @@
     </row>
     <row r="3" ht="15" hidden="1" customHeight="1" spans="1:4">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D3" s="9">
         <v>12345678</v>
@@ -7654,13 +7636,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D4" s="9">
         <v>12345678</v>
@@ -7668,13 +7650,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D5" s="9">
         <v>12345678</v>
@@ -7682,13 +7664,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D6" s="9">
         <v>12345678</v>
@@ -7696,13 +7678,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D7" s="9">
         <v>12345678</v>
@@ -7752,24 +7734,24 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -7780,10 +7762,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -7792,15 +7774,15 @@
         <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -7814,10 +7796,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
define xmltest orders programmatically
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="347">
   <si>
     <t>Page</t>
   </si>
@@ -725,6 +725,15 @@
   </si>
   <si>
     <t>ImplementAnnotation</t>
+  </si>
+  <si>
+    <t>CCMChronic</t>
+  </si>
+  <si>
+    <t>CCMEnrollment</t>
+  </si>
+  <si>
+    <t>CCMChronicLog</t>
   </si>
   <si>
     <t>TestGroup ID</t>
@@ -2912,16 +2921,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" hidden="1" spans="1:4">
@@ -2929,7 +2938,7 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -2943,13 +2952,13 @@
         <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E3" s="7">
         <v>51</v>
@@ -2960,7 +2969,7 @@
         <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>62</v>
@@ -2974,7 +2983,7 @@
         <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>70</v>
@@ -2989,7 +2998,7 @@
         <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>84</v>
@@ -3003,13 +3012,13 @@
         <v>198</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E7" s="7">
         <v>89</v>
@@ -3020,7 +3029,7 @@
         <v>200</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>84</v>
@@ -3034,7 +3043,7 @@
         <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D9" t="s">
         <v>170</v>
@@ -3048,13 +3057,13 @@
         <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E10" s="7">
         <v>89</v>
@@ -3065,7 +3074,7 @@
         <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
         <v>84</v>
@@ -3079,13 +3088,13 @@
         <v>202</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E12" s="7">
         <v>90</v>
@@ -3096,7 +3105,7 @@
         <v>202</v>
       </c>
       <c r="B13" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C13" t="s">
         <v>84</v>
@@ -3110,13 +3119,13 @@
         <v>202</v>
       </c>
       <c r="B14" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
         <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E14" s="7">
         <v>90</v>
@@ -3127,7 +3136,7 @@
         <v>203</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>84</v>
@@ -3141,13 +3150,13 @@
         <v>203</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E16" s="7">
         <v>91</v>
@@ -3158,7 +3167,7 @@
         <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s">
         <v>84</v>
@@ -3172,13 +3181,13 @@
         <v>203</v>
       </c>
       <c r="B18" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C18" t="s">
         <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E18" s="7">
         <v>91</v>
@@ -3232,16 +3241,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" ht="17" hidden="1" customHeight="1" spans="1:4">
@@ -3249,7 +3258,7 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -3263,7 +3272,7 @@
         <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -3277,7 +3286,7 @@
         <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>26</v>
@@ -3291,7 +3300,7 @@
         <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
@@ -3300,7 +3309,7 @@
         <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" ht="23" hidden="1" customHeight="1" spans="1:4">
@@ -3308,7 +3317,7 @@
         <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -3322,13 +3331,13 @@
         <v>197</v>
       </c>
       <c r="B7" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C7" t="s">
         <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -3339,7 +3348,7 @@
         <v>197</v>
       </c>
       <c r="B8" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C8" t="s">
         <v>63</v>
@@ -3348,7 +3357,7 @@
         <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row r="9" ht="18" hidden="1" customHeight="1" spans="1:5">
@@ -3356,7 +3365,7 @@
         <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C9" t="s">
         <v>71</v>
@@ -3373,7 +3382,7 @@
         <v>198</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -3387,7 +3396,7 @@
         <v>198</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D11" t="s">
         <v>170</v>
@@ -3401,7 +3410,7 @@
         <v>198</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>91</v>
@@ -3410,7 +3419,7 @@
         <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3418,16 +3427,16 @@
         <v>198</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="E13" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" ht="12" customHeight="1" spans="1:5">
@@ -3435,7 +3444,7 @@
         <v>198</v>
       </c>
       <c r="B14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D14" t="s">
         <v>170</v>
@@ -3449,7 +3458,7 @@
         <v>198</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>91</v>
@@ -3458,7 +3467,7 @@
         <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3466,7 +3475,7 @@
         <v>198</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>96</v>
@@ -3475,7 +3484,7 @@
         <v>117</v>
       </c>
       <c r="E16" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" ht="12" customHeight="1" spans="1:5">
@@ -3483,7 +3492,7 @@
         <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D17" t="s">
         <v>170</v>
@@ -3497,7 +3506,7 @@
         <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
         <v>91</v>
@@ -3506,7 +3515,7 @@
         <v>117</v>
       </c>
       <c r="E18" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3514,7 +3523,7 @@
         <v>198</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
         <v>96</v>
@@ -3523,7 +3532,7 @@
         <v>117</v>
       </c>
       <c r="E19" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3531,7 +3540,7 @@
         <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D20" t="s">
         <v>170</v>
@@ -3545,7 +3554,7 @@
         <v>198</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D21" t="s">
         <v>169</v>
@@ -3556,7 +3565,7 @@
         <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
         <v>91</v>
@@ -3565,7 +3574,7 @@
         <v>117</v>
       </c>
       <c r="E22" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3573,7 +3582,7 @@
         <v>198</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
         <v>96</v>
@@ -3582,7 +3591,7 @@
         <v>117</v>
       </c>
       <c r="E23" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="1:4">
@@ -3590,7 +3599,7 @@
         <v>198</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D24" t="s">
         <v>168</v>
@@ -3601,7 +3610,7 @@
         <v>198</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>85</v>
@@ -3615,7 +3624,7 @@
         <v>200</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C26" t="s">
         <v>96</v>
@@ -3624,7 +3633,7 @@
         <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3632,7 +3641,7 @@
         <v>200</v>
       </c>
       <c r="B27" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D27" t="s">
         <v>170</v>
@@ -3646,7 +3655,7 @@
         <v>200</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D28" t="s">
         <v>169</v>
@@ -3657,7 +3666,7 @@
         <v>200</v>
       </c>
       <c r="B29" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
         <v>96</v>
@@ -3666,7 +3675,7 @@
         <v>117</v>
       </c>
       <c r="E29" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3674,7 +3683,7 @@
         <v>200</v>
       </c>
       <c r="B30" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D30" t="s">
         <v>170</v>
@@ -3688,7 +3697,7 @@
         <v>200</v>
       </c>
       <c r="B31" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D31" t="s">
         <v>169</v>
@@ -3699,7 +3708,7 @@
         <v>200</v>
       </c>
       <c r="B32" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C32" t="s">
         <v>96</v>
@@ -3708,7 +3717,7 @@
         <v>117</v>
       </c>
       <c r="E32" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3716,7 +3725,7 @@
         <v>200</v>
       </c>
       <c r="B33" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D33" t="s">
         <v>170</v>
@@ -3730,7 +3739,7 @@
         <v>200</v>
       </c>
       <c r="B34" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D34" t="s">
         <v>169</v>
@@ -3741,7 +3750,7 @@
         <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C35" t="s">
         <v>96</v>
@@ -3758,7 +3767,7 @@
         <v>200</v>
       </c>
       <c r="B36" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D36" t="s">
         <v>168</v>
@@ -3769,7 +3778,7 @@
         <v>200</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>55</v>
@@ -3783,7 +3792,7 @@
         <v>202</v>
       </c>
       <c r="B38" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C38" t="s">
         <v>25</v>
@@ -3797,7 +3806,7 @@
         <v>202</v>
       </c>
       <c r="B39" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D39" t="s">
         <v>170</v>
@@ -3811,7 +3820,7 @@
         <v>202</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C40" t="s">
         <v>85</v>
@@ -3825,7 +3834,7 @@
         <v>202</v>
       </c>
       <c r="B41" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C41" t="s">
         <v>26</v>
@@ -3839,7 +3848,7 @@
         <v>203</v>
       </c>
       <c r="B42" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C42" t="s">
         <v>25</v>
@@ -3853,7 +3862,7 @@
         <v>203</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D43" t="s">
         <v>170</v>
@@ -3867,7 +3876,7 @@
         <v>203</v>
       </c>
       <c r="B44" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C44" t="s">
         <v>85</v>
@@ -3881,7 +3890,7 @@
         <v>203</v>
       </c>
       <c r="B45" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C45" t="s">
         <v>26</v>
@@ -3929,16 +3938,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3946,7 +3955,7 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3960,7 +3969,7 @@
         <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -3969,7 +3978,7 @@
         <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3977,7 +3986,7 @@
         <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>97</v>
@@ -3991,7 +4000,7 @@
         <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>72</v>
@@ -4005,7 +4014,7 @@
         <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>79</v>
@@ -4019,7 +4028,7 @@
         <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>72</v>
@@ -4028,7 +4037,7 @@
         <v>117</v>
       </c>
       <c r="E7" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4036,7 +4045,7 @@
         <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>100</v>
@@ -4050,7 +4059,7 @@
         <v>194</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
         <v>86</v>
@@ -4064,7 +4073,7 @@
         <v>194</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>100</v>
@@ -4073,7 +4082,7 @@
         <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4081,7 +4090,7 @@
         <v>194</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
         <v>103</v>
@@ -4090,7 +4099,7 @@
         <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4098,7 +4107,7 @@
         <v>194</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>107</v>
@@ -4112,7 +4121,7 @@
         <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>111</v>
@@ -4121,7 +4130,7 @@
         <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4129,7 +4138,7 @@
         <v>194</v>
       </c>
       <c r="B14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
         <v>79</v>
@@ -4143,7 +4152,7 @@
         <v>194</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>107</v>
@@ -4152,7 +4161,7 @@
         <v>117</v>
       </c>
       <c r="E15" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4160,7 +4169,7 @@
         <v>194</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>115</v>
@@ -4169,7 +4178,7 @@
         <v>117</v>
       </c>
       <c r="E16" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4177,7 +4186,7 @@
         <v>194</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
         <v>118</v>
@@ -4191,7 +4200,7 @@
         <v>194</v>
       </c>
       <c r="B18" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
         <v>65</v>
@@ -4200,7 +4209,7 @@
         <v>33</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4208,7 +4217,7 @@
         <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
         <v>129</v>
@@ -4225,7 +4234,7 @@
         <v>194</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C20" t="s">
         <v>129</v>
@@ -4234,7 +4243,7 @@
         <v>165</v>
       </c>
       <c r="E20" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4242,7 +4251,7 @@
         <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
         <v>150</v>
@@ -4251,7 +4260,7 @@
         <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -4259,7 +4268,7 @@
         <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
         <v>129</v>
@@ -4268,7 +4277,7 @@
         <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4276,7 +4285,7 @@
         <v>194</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
         <v>132</v>
@@ -4290,7 +4299,7 @@
         <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C24" t="s">
         <v>141</v>
@@ -4304,7 +4313,7 @@
         <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C25" t="s">
         <v>144</v>
@@ -4318,7 +4327,7 @@
         <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C26" t="s">
         <v>132</v>
@@ -4327,7 +4336,7 @@
         <v>165</v>
       </c>
       <c r="E26" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4335,7 +4344,7 @@
         <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C27" t="s">
         <v>150</v>
@@ -4344,7 +4353,7 @@
         <v>117</v>
       </c>
       <c r="E27" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -4352,7 +4361,7 @@
         <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C28" t="s">
         <v>132</v>
@@ -4369,7 +4378,7 @@
         <v>194</v>
       </c>
       <c r="B29" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C29" t="s">
         <v>54</v>
@@ -4378,7 +4387,7 @@
         <v>33</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
@@ -4386,7 +4395,7 @@
         <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C30" t="s">
         <v>150</v>
@@ -4395,7 +4404,7 @@
         <v>117</v>
       </c>
       <c r="E30" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
@@ -4403,7 +4412,7 @@
         <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C31" t="s">
         <v>54</v>
@@ -4412,7 +4421,7 @@
         <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4420,7 +4429,7 @@
         <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C32" t="s">
         <v>144</v>
@@ -4434,13 +4443,13 @@
         <v>194</v>
       </c>
       <c r="B33" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C33" t="s">
         <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -4448,7 +4457,7 @@
         <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C34" t="s">
         <v>26</v>
@@ -4462,7 +4471,7 @@
         <v>197</v>
       </c>
       <c r="B35" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C35" t="s">
         <v>157</v>
@@ -4479,7 +4488,7 @@
         <v>197</v>
       </c>
       <c r="B36" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C36" t="s">
         <v>26</v>
@@ -4493,7 +4502,7 @@
         <v>197</v>
       </c>
       <c r="B37" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C37" t="s">
         <v>53</v>
@@ -4507,7 +4516,7 @@
         <v>197</v>
       </c>
       <c r="B38" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C38" t="s">
         <v>159</v>
@@ -4521,7 +4530,7 @@
         <v>197</v>
       </c>
       <c r="B39" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C39" t="s">
         <v>79</v>
@@ -4535,7 +4544,7 @@
         <v>197</v>
       </c>
       <c r="B40" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C40" t="s">
         <v>164</v>
@@ -4549,7 +4558,7 @@
         <v>197</v>
       </c>
       <c r="B41" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C41" t="s">
         <v>144</v>
@@ -4563,7 +4572,7 @@
         <v>197</v>
       </c>
       <c r="B42" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C42" t="s">
         <v>26</v>
@@ -4617,16 +4626,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4634,7 +4643,7 @@
         <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
@@ -4643,7 +4652,7 @@
         <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4651,7 +4660,7 @@
         <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
@@ -4660,7 +4669,7 @@
         <v>183</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4668,7 +4677,7 @@
         <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D4" t="s">
         <v>168</v>
@@ -4680,7 +4689,7 @@
         <v>202</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>55</v>
@@ -4695,7 +4704,7 @@
         <v>203</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -4704,7 +4713,7 @@
         <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4712,7 +4721,7 @@
         <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -4721,7 +4730,7 @@
         <v>183</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4729,7 +4738,7 @@
         <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="D8" t="s">
         <v>168</v>
@@ -4740,7 +4749,7 @@
         <v>203</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>55</v>
@@ -4796,16 +4805,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4813,7 +4822,7 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -4827,7 +4836,7 @@
         <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -4844,7 +4853,7 @@
         <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>
@@ -4861,7 +4870,7 @@
         <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>65</v>
@@ -4878,7 +4887,7 @@
         <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D6" t="s">
         <v>168</v>
@@ -4927,7 +4936,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -4936,16 +4945,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4959,7 +4968,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -4973,7 +4982,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4987,12 +4996,12 @@
         <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
@@ -5001,7 +5010,7 @@
         <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -5045,7 +5054,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5054,16 +5063,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5077,7 +5086,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -5094,7 +5103,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -5111,7 +5120,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5125,7 +5134,7 @@
         <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5139,7 +5148,7 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5153,7 +5162,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -5200,7 +5209,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5209,16 +5218,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5232,7 +5241,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5246,7 +5255,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5260,7 +5269,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5274,7 +5283,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -5288,7 +5297,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
@@ -5302,7 +5311,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
@@ -5316,7 +5325,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
@@ -5330,7 +5339,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
@@ -5344,7 +5353,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
@@ -5358,7 +5367,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:4">
@@ -5372,7 +5381,7 @@
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="1:4">
@@ -5386,12 +5395,12 @@
         <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>136</v>
@@ -5400,7 +5409,7 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" spans="1:7">
@@ -5414,7 +5423,7 @@
         <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>1</v>
@@ -5431,7 +5440,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -5448,7 +5457,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>1</v>
@@ -5465,7 +5474,7 @@
         <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -5482,7 +5491,7 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
@@ -5496,7 +5505,7 @@
         <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
@@ -5510,7 +5519,7 @@
         <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:4">
@@ -5524,7 +5533,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" spans="1:4">
@@ -5538,7 +5547,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:4">
@@ -5552,7 +5561,7 @@
         <v>31</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:4">
@@ -5566,7 +5575,7 @@
         <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" s="4" customFormat="1" spans="1:6">
@@ -5580,7 +5589,7 @@
         <v>66</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F26" s="4" t="b">
         <v>1</v>
@@ -5597,7 +5606,7 @@
         <v>66</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -5605,7 +5614,7 @@
     </row>
     <row r="28" s="4" customFormat="1" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>142</v>
@@ -5614,7 +5623,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:4">
@@ -5628,7 +5637,7 @@
         <v>57</v>
       </c>
       <c r="D29" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5675,7 +5684,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5684,16 +5693,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5707,7 +5716,7 @@
         <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -5724,7 +5733,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
@@ -5738,7 +5747,7 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:4">
@@ -5752,7 +5761,7 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -5766,7 +5775,7 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5780,7 +5789,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5794,12 +5803,12 @@
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B9" t="s">
         <v>145</v>
@@ -5808,7 +5817,7 @@
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5822,7 +5831,7 @@
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5866,7 +5875,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -5875,16 +5884,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5898,7 +5907,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:4">
@@ -5912,7 +5921,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -5946,7 +5955,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="$A7:$XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -6179,7 +6188,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6188,21 +6197,21 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B2" t="s">
         <v>139</v>
@@ -6211,7 +6220,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6225,7 +6234,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6239,7 +6248,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
@@ -6253,7 +6262,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:4">
@@ -6267,7 +6276,7 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -6314,7 +6323,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6323,16 +6332,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6346,7 +6355,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6360,7 +6369,7 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6374,7 +6383,7 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -6391,7 +6400,7 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -6438,7 +6447,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6447,16 +6456,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6470,7 +6479,7 @@
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -6478,7 +6487,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B3" t="s">
         <v>148</v>
@@ -6487,7 +6496,7 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6501,12 +6510,12 @@
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B5" t="s">
         <v>139</v>
@@ -6515,12 +6524,12 @@
         <v>57</v>
       </c>
       <c r="D5" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B6" t="s">
         <v>142</v>
@@ -6529,12 +6538,12 @@
         <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B7" t="s">
         <v>139</v>
@@ -6543,7 +6552,7 @@
         <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -6587,7 +6596,7 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -6596,16 +6605,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6619,7 +6628,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6633,7 +6642,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:4">
@@ -6647,7 +6656,7 @@
         <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -6678,7 +6687,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -6737,7 +6746,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6754,15 +6763,15 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="22.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="27.5714285714286" customWidth="1"/>
@@ -6839,15 +6848,85 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B5 B6:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B9 B10:B1048576">
       <formula1>PageObjectModel!$A:$A</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 D2 D3 D4 C5 D5 C3:C4 C6:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1 C2 D2 D3 D4 C5 D5 C6 D6 C7 D7 C8 D8 C9 D9 C10 D10 C3:C4 C11:C1048576">
       <formula1>Boolean</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3:A5 A6:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1 A3:A9 A10:A1048576">
       <formula1>Flow</formula1>
     </dataValidation>
   </dataValidations>
@@ -6879,16 +6958,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6896,7 +6975,7 @@
         <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -6910,7 +6989,7 @@
         <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -6919,7 +6998,7 @@
         <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6927,7 +7006,7 @@
         <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -6944,7 +7023,7 @@
         <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>
@@ -6993,16 +7072,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -7010,7 +7089,7 @@
         <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -7025,7 +7104,7 @@
         <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
@@ -7039,7 +7118,7 @@
         <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
@@ -7053,7 +7132,7 @@
         <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>60</v>
@@ -7067,7 +7146,7 @@
         <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
@@ -7081,7 +7160,7 @@
         <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -7128,16 +7207,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -7145,7 +7224,7 @@
         <v>191</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
@@ -7160,7 +7239,7 @@
         <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
@@ -7169,7 +7248,7 @@
         <v>152</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7177,7 +7256,7 @@
         <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -7186,7 +7265,7 @@
         <v>155</v>
       </c>
       <c r="E4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7194,7 +7273,7 @@
         <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -7203,7 +7282,7 @@
         <v>152</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -7211,7 +7290,7 @@
         <v>191</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -7220,7 +7299,7 @@
         <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -7228,7 +7307,7 @@
         <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C7" t="s">
         <v>37</v>
@@ -7237,7 +7316,7 @@
         <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -7245,7 +7324,7 @@
         <v>191</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
@@ -7254,7 +7333,7 @@
         <v>152</v>
       </c>
       <c r="E8" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -7262,7 +7341,7 @@
         <v>191</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -7271,7 +7350,7 @@
         <v>155</v>
       </c>
       <c r="E9" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -7279,7 +7358,7 @@
         <v>191</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C10" t="s">
         <v>50</v>
@@ -7288,7 +7367,7 @@
         <v>161</v>
       </c>
       <c r="E10" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -7296,7 +7375,7 @@
         <v>191</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -7305,7 +7384,7 @@
         <v>152</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -7313,7 +7392,7 @@
         <v>191</v>
       </c>
       <c r="B12" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
         <v>69</v>
@@ -7327,7 +7406,7 @@
         <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -7336,7 +7415,7 @@
         <v>161</v>
       </c>
       <c r="E13" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -7344,7 +7423,7 @@
         <v>191</v>
       </c>
       <c r="B14" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C14" t="s">
         <v>61</v>
@@ -7353,7 +7432,7 @@
         <v>161</v>
       </c>
       <c r="E14" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -7361,7 +7440,7 @@
         <v>191</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
         <v>23</v>
@@ -7370,7 +7449,7 @@
         <v>152</v>
       </c>
       <c r="E15" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -7378,7 +7457,7 @@
         <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -7387,7 +7466,7 @@
         <v>155</v>
       </c>
       <c r="E16" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -7395,7 +7474,7 @@
         <v>191</v>
       </c>
       <c r="B17" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C17" t="s">
         <v>50</v>
@@ -7404,7 +7483,7 @@
         <v>161</v>
       </c>
       <c r="E17" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -7412,7 +7491,7 @@
         <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
@@ -7426,7 +7505,7 @@
         <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C19" t="s">
         <v>86</v>
@@ -7440,7 +7519,7 @@
         <v>191</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C20" t="s">
         <v>76</v>
@@ -7454,7 +7533,7 @@
         <v>191</v>
       </c>
       <c r="B21" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C21" t="s">
         <v>86</v>
@@ -7468,7 +7547,7 @@
         <v>191</v>
       </c>
       <c r="B22" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
         <v>106</v>
@@ -7477,7 +7556,7 @@
         <v>117</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -7485,7 +7564,7 @@
         <v>191</v>
       </c>
       <c r="B23" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s">
         <v>110</v>
@@ -7494,7 +7573,7 @@
         <v>117</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -7502,10 +7581,10 @@
         <v>191</v>
       </c>
       <c r="B24" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="D24" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -7547,7 +7626,7 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>21</v>
@@ -7561,10 +7640,10 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D2" s="9">
         <v>12345678</v>
@@ -7575,10 +7654,10 @@
         <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D3" s="9">
         <v>12345678</v>
@@ -7589,10 +7668,10 @@
         <v>198</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D4" s="9">
         <v>12345678</v>
@@ -7603,10 +7682,10 @@
         <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D5" s="9">
         <v>12345678</v>
@@ -7617,10 +7696,10 @@
         <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D6" s="9">
         <v>12345678</v>
@@ -7631,10 +7710,10 @@
         <v>203</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="D7" s="9">
         <v>12345678</v>
@@ -7684,16 +7763,16 @@
         <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7701,7 +7780,7 @@
         <v>194</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -7715,7 +7794,7 @@
         <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -7724,7 +7803,7 @@
         <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7732,7 +7811,7 @@
         <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -7749,7 +7828,7 @@
         <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
update timing testcases, update listener
</commit_message>
<xml_diff>
--- a/demo/testData/testCase.xlsx
+++ b/demo/testData/testCase.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12510" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="12510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PageObjectModel" sheetId="5" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="Flow" sheetId="19" r:id="rId4"/>
     <sheet name="AnnotationLoginPage" sheetId="22" state="hidden" r:id="rId5"/>
     <sheet name="AnnotationHomePage" sheetId="23" state="hidden" r:id="rId6"/>
-    <sheet name="AnnotationImplementPage" sheetId="24" r:id="rId7"/>
+    <sheet name="AnnotationImplementPage" sheetId="24" state="hidden" r:id="rId7"/>
     <sheet name="Login" sheetId="29" r:id="rId8"/>
     <sheet name="CCMLoginPage" sheetId="25" state="hidden" r:id="rId9"/>
     <sheet name="CCMMemberPage" sheetId="26" r:id="rId10"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1329" uniqueCount="352">
   <si>
     <t>Page</t>
   </si>
@@ -331,7 +331,7 @@
     <t>Dropdowns[1]</t>
   </si>
   <si>
-    <t>PageNumberButtons[4]</t>
+    <t>PageNumberButtons[5]</t>
   </si>
   <si>
     <t>ReminderButtons[1]</t>
@@ -823,7 +823,16 @@
     <t>selectMemberByMID</t>
   </si>
   <si>
+    <t>8ELN0090</t>
+  </si>
+  <si>
+    <t>9ELN0091</t>
+  </si>
+  <si>
     <t>TS_02</t>
+  </si>
+  <si>
+    <t>3ELN0092</t>
   </si>
   <si>
     <t>No Data</t>
@@ -1125,10 +1134,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1163,7 +1172,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1177,6 +1214,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
@@ -1185,22 +1246,8 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1215,15 +1262,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1238,53 +1284,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1347,7 +1356,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1359,31 +1446,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1395,61 +1458,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1467,19 +1482,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1491,25 +1500,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1521,7 +1524,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1553,41 +1562,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1618,6 +1609,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1633,111 +1633,120 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1746,28 +1755,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1776,26 +1785,26 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1819,7 +1828,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="41"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2144,7 +2152,7 @@
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="S7" sqref="S7"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2274,7 +2282,7 @@
       <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2925,7 +2933,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -3040,8 +3048,8 @@
       <c r="D7" t="s">
         <v>249</v>
       </c>
-      <c r="E7" s="7">
-        <v>89</v>
+      <c r="E7" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3085,8 +3093,8 @@
       <c r="D10" t="s">
         <v>249</v>
       </c>
-      <c r="E10" s="7">
-        <v>89</v>
+      <c r="E10" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3116,8 +3124,8 @@
       <c r="D12" t="s">
         <v>249</v>
       </c>
-      <c r="E12" s="7">
-        <v>90</v>
+      <c r="E12" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3125,7 +3133,7 @@
         <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C13" t="s">
         <v>86</v>
@@ -3139,7 +3147,7 @@
         <v>205</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
@@ -3147,8 +3155,8 @@
       <c r="D14" t="s">
         <v>249</v>
       </c>
-      <c r="E14" s="7">
-        <v>90</v>
+      <c r="E14" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3178,8 +3186,8 @@
       <c r="D16" t="s">
         <v>249</v>
       </c>
-      <c r="E16" s="7">
-        <v>91</v>
+      <c r="E16" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3187,7 +3195,7 @@
         <v>206</v>
       </c>
       <c r="B17" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C17" t="s">
         <v>86</v>
@@ -3201,7 +3209,7 @@
         <v>206</v>
       </c>
       <c r="B18" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C18" t="s">
         <v>53</v>
@@ -3209,8 +3217,8 @@
       <c r="D18" t="s">
         <v>249</v>
       </c>
-      <c r="E18" s="7">
-        <v>91</v>
+      <c r="E18" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3227,13 +3235,11 @@
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" display="51" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="E7" r:id="rId1" display="89" tooltip="mailto:Jenny@meddataquest.com"/>
     <hyperlink ref="E9" r:id="rId1" display="1.2" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="E10" r:id="rId1" display="89" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="E12" r:id="rId1" display="90" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="E18" r:id="rId1" display="91" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="E14" r:id="rId1" display="90" tooltip="mailto:Jenny@meddataquest.com"/>
-    <hyperlink ref="E16" r:id="rId1" display="91" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="E12" r:id="rId1" display="9ELN0091" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="E16" r:id="rId1" display="3ELN0092" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="E14" r:id="rId1" display="9ELN0091" tooltip="mailto:Jenny@meddataquest.com"/>
+    <hyperlink ref="E18" r:id="rId1" display="3ELN0092" tooltip="mailto:Jenny@meddataquest.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3320,7 +3326,7 @@
         <v>200</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C5" t="s">
         <v>54</v>
@@ -3329,7 +3335,7 @@
         <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" ht="23" hidden="1" customHeight="1" spans="1:4">
@@ -3337,7 +3343,7 @@
         <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
         <v>27</v>
@@ -3351,13 +3357,13 @@
         <v>200</v>
       </c>
       <c r="B7" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -3368,7 +3374,7 @@
         <v>200</v>
       </c>
       <c r="B8" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C8" t="s">
         <v>65</v>
@@ -3377,7 +3383,7 @@
         <v>119</v>
       </c>
       <c r="E8" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" ht="18" hidden="1" customHeight="1" spans="1:5">
@@ -3385,7 +3391,7 @@
         <v>200</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C9" t="s">
         <v>73</v>
@@ -3439,7 +3445,7 @@
         <v>119</v>
       </c>
       <c r="E12" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3456,7 +3462,7 @@
         <v>123</v>
       </c>
       <c r="E13" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" ht="12" customHeight="1" spans="1:5">
@@ -3487,7 +3493,7 @@
         <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3504,7 +3510,7 @@
         <v>119</v>
       </c>
       <c r="E16" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" ht="12" customHeight="1" spans="1:5">
@@ -3535,7 +3541,7 @@
         <v>119</v>
       </c>
       <c r="E18" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3552,7 +3558,7 @@
         <v>119</v>
       </c>
       <c r="E19" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3594,7 +3600,7 @@
         <v>119</v>
       </c>
       <c r="E22" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3611,7 +3617,7 @@
         <v>119</v>
       </c>
       <c r="E23" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="1:4">
@@ -3653,7 +3659,7 @@
         <v>119</v>
       </c>
       <c r="E26" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3695,7 +3701,7 @@
         <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3737,7 +3743,7 @@
         <v>119</v>
       </c>
       <c r="E32" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3854,7 +3860,7 @@
         <v>205</v>
       </c>
       <c r="B41" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C41" t="s">
         <v>27</v>
@@ -3910,7 +3916,7 @@
         <v>206</v>
       </c>
       <c r="B45" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C45" t="s">
         <v>27</v>
@@ -3998,7 +4004,7 @@
         <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -4057,7 +4063,7 @@
         <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4102,7 +4108,7 @@
         <v>119</v>
       </c>
       <c r="E10" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -4119,7 +4125,7 @@
         <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4150,7 +4156,7 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -4181,7 +4187,7 @@
         <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -4198,7 +4204,7 @@
         <v>119</v>
       </c>
       <c r="E16" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -4229,7 +4235,7 @@
         <v>35</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -4263,7 +4269,7 @@
         <v>168</v>
       </c>
       <c r="E20" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -4280,7 +4286,7 @@
         <v>119</v>
       </c>
       <c r="E21" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -4297,7 +4303,7 @@
         <v>35</v>
       </c>
       <c r="E22" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -4356,7 +4362,7 @@
         <v>168</v>
       </c>
       <c r="E26" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -4373,7 +4379,7 @@
         <v>119</v>
       </c>
       <c r="E27" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -4407,7 +4413,7 @@
         <v>35</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" ht="12" customHeight="1" spans="1:5">
@@ -4424,7 +4430,7 @@
         <v>119</v>
       </c>
       <c r="E30" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" ht="12" customHeight="1" spans="1:5">
@@ -4441,7 +4447,7 @@
         <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -4522,7 +4528,7 @@
         <v>200</v>
       </c>
       <c r="B37" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C37" t="s">
         <v>55</v>
@@ -4536,7 +4542,7 @@
         <v>200</v>
       </c>
       <c r="B38" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C38" t="s">
         <v>162</v>
@@ -4550,7 +4556,7 @@
         <v>200</v>
       </c>
       <c r="B39" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C39" t="s">
         <v>81</v>
@@ -4564,7 +4570,7 @@
         <v>200</v>
       </c>
       <c r="B40" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C40" t="s">
         <v>167</v>
@@ -4578,7 +4584,7 @@
         <v>200</v>
       </c>
       <c r="B41" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C41" t="s">
         <v>147</v>
@@ -4592,7 +4598,7 @@
         <v>200</v>
       </c>
       <c r="B42" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -4630,7 +4636,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -4663,7 +4669,7 @@
         <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -4672,7 +4678,7 @@
         <v>185</v>
       </c>
       <c r="E2" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4680,7 +4686,7 @@
         <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C3" t="s">
         <v>43</v>
@@ -4697,7 +4703,7 @@
         <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D4" t="s">
         <v>171</v>
@@ -4709,7 +4715,7 @@
         <v>205</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>57</v>
@@ -4724,7 +4730,7 @@
         <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C6" t="s">
         <v>43</v>
@@ -4733,7 +4739,7 @@
         <v>185</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4741,7 +4747,7 @@
         <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C7" t="s">
         <v>43</v>
@@ -4758,7 +4764,7 @@
         <v>206</v>
       </c>
       <c r="B8" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D8" t="s">
         <v>171</v>
@@ -4769,7 +4775,7 @@
         <v>206</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>57</v>
@@ -4965,16 +4971,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4988,7 +4994,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5002,7 +5008,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5016,12 +5022,12 @@
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B5" t="s">
         <v>47</v>
@@ -5030,7 +5036,7 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -5083,16 +5089,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5106,7 +5112,7 @@
         <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -5123,7 +5129,7 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
@@ -5140,7 +5146,7 @@
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5154,7 +5160,7 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -5168,7 +5174,7 @@
         <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5182,7 +5188,7 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E7" t="b">
         <v>1</v>
@@ -5238,16 +5244,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5261,7 +5267,7 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -5275,7 +5281,7 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -5289,7 +5295,7 @@
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -5303,7 +5309,7 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -5317,7 +5323,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" spans="1:4">
@@ -5331,7 +5337,7 @@
         <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" spans="1:4">
@@ -5345,7 +5351,7 @@
         <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" spans="1:4">
@@ -5359,7 +5365,7 @@
         <v>32</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" spans="1:4">
@@ -5373,7 +5379,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" spans="1:4">
@@ -5387,7 +5393,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:4">
@@ -5401,7 +5407,7 @@
         <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" spans="1:4">
@@ -5415,12 +5421,12 @@
         <v>32</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>139</v>
@@ -5429,7 +5435,7 @@
         <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" spans="1:7">
@@ -5443,7 +5449,7 @@
         <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>1</v>
@@ -5460,7 +5466,7 @@
         <v>32</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>1</v>
@@ -5477,7 +5483,7 @@
         <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>1</v>
@@ -5494,7 +5500,7 @@
         <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>1</v>
@@ -5511,7 +5517,7 @@
         <v>59</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" s="2" customFormat="1" ht="12" customHeight="1" spans="1:4">
@@ -5525,7 +5531,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" s="2" customFormat="1" spans="1:4">
@@ -5539,7 +5545,7 @@
         <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:4">
@@ -5553,7 +5559,7 @@
         <v>32</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" s="3" customFormat="1" spans="1:4">
@@ -5567,7 +5573,7 @@
         <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:4">
@@ -5581,7 +5587,7 @@
         <v>32</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:4">
@@ -5595,7 +5601,7 @@
         <v>32</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" s="4" customFormat="1" spans="1:6">
@@ -5609,7 +5615,7 @@
         <v>68</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F26" s="4" t="b">
         <v>1</v>
@@ -5626,7 +5632,7 @@
         <v>68</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="G27" s="4" t="b">
         <v>1</v>
@@ -5634,7 +5640,7 @@
     </row>
     <row r="28" s="4" customFormat="1" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>145</v>
@@ -5643,7 +5649,7 @@
         <v>59</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" customFormat="1" spans="1:4">
@@ -5657,7 +5663,7 @@
         <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5713,16 +5719,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5736,7 +5742,7 @@
         <v>68</v>
       </c>
       <c r="D2" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -5753,7 +5759,7 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
     </row>
     <row r="4" s="2" customFormat="1" spans="1:4">
@@ -5767,7 +5773,7 @@
         <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" spans="1:4">
@@ -5781,7 +5787,7 @@
         <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" spans="1:4">
@@ -5795,7 +5801,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -5809,7 +5815,7 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -5823,12 +5829,12 @@
         <v>59</v>
       </c>
       <c r="D8" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B9" t="s">
         <v>148</v>
@@ -5837,7 +5843,7 @@
         <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -5851,7 +5857,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5904,16 +5910,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5927,7 +5933,7 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:4">
@@ -5941,7 +5947,7 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5972,10 +5978,10 @@
   <sheetPr/>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomLeft" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="7"/>
@@ -6021,7 +6027,7 @@
         <v>195</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>196</v>
@@ -6127,7 +6133,7 @@
         <v>202</v>
       </c>
       <c r="C7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>199</v>
@@ -6150,7 +6156,7 @@
         <v>202</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>199</v>
@@ -6217,21 +6223,21 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B2" t="s">
         <v>142</v>
@@ -6240,7 +6246,7 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6254,7 +6260,7 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6268,7 +6274,7 @@
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1" spans="1:4">
@@ -6282,7 +6288,7 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:4">
@@ -6296,7 +6302,7 @@
         <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -6352,16 +6358,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6375,7 +6381,7 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6389,7 +6395,7 @@
         <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -6403,7 +6409,7 @@
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -6420,7 +6426,7 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -6476,16 +6482,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -6499,7 +6505,7 @@
         <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -6516,7 +6522,7 @@
         <v>59</v>
       </c>
       <c r="D3" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6530,12 +6536,12 @@
         <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B5" t="s">
         <v>142</v>
@@ -6544,12 +6550,12 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B6" t="s">
         <v>145</v>
@@ -6558,12 +6564,12 @@
         <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B7" t="s">
         <v>142</v>
@@ -6572,7 +6578,7 @@
         <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -6625,16 +6631,16 @@
         <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6648,7 +6654,7 @@
         <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6662,7 +6668,7 @@
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1" spans="1:4">
@@ -6676,7 +6682,7 @@
         <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -6707,7 +6713,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -6754,7 +6760,7 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -7217,7 +7223,7 @@
   <sheetPr/>
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
@@ -7644,9 +7650,6 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <ignoredErrors>
-    <ignoredError sqref="E11" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>